<commit_message>
adds further code to Login Controller, adds todo
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="172" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49A05528-F07C-4C25-8136-DD6D10E4961D}"/>
+  <xr:revisionPtr revIDLastSave="176" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01964676-0B98-46A6-B02E-EEA802F4EFC6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Stand</t>
   </si>
@@ -348,6 +348,9 @@
   </si>
   <si>
     <t>Unedingt ein Ehepaar mit derselben Adresse einbauen</t>
+  </si>
+  <si>
+    <t>Login Controller - credentials db check?</t>
   </si>
 </sst>
 </file>
@@ -478,13 +481,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>72</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -805,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -840,7 +843,7 @@
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2"/>
     </row>
@@ -849,245 +852,245 @@
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="2"/>
-    </row>
+    <row r="9" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
+      <c r="A11" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="2"/>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="A17" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
+      <c r="A21" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+      <c r="A22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A24" s="3"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
+      <c r="A26" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="A27" s="3"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
+      <c r="A28" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="3"/>
+      <c r="A31" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="A32" s="3"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>10</v>
+      <c r="A33" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>12</v>
+      <c r="A35" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
-        <v>13</v>
+      <c r="A37" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
-        <v>14</v>
+      <c r="A38" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="3"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
+      <c r="A39" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A46" s="8" t="s">
+    <row r="42" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A42" s="8" t="s">
         <v>22</v>
       </c>
     </row>
+    <row r="44" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" s="2"/>
+    </row>
+    <row r="46" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" s="2"/>
+    </row>
     <row r="48" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>20</v>
+      <c r="A48" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="B48" s="2"/>
     </row>
     <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>21</v>
+      <c r="A50" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="B50" s="2"/>
     </row>
     <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B52" s="2"/>
     </row>
-    <row r="54" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B54" s="2"/>
-    </row>
-    <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B56" s="2"/>
-    </row>
-    <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="1"/>
-      <c r="B57" s="2"/>
+    <row r="53" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
+      <c r="B53" s="2"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B54" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="9"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="9"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B58" s="9" t="s">
-        <v>27</v>
+      <c r="A58" s="9"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="9" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="9"/>
+      <c r="A60" s="9" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="9"/>
+      <c r="A61" s="9" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="9"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="9"/>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="9" t="s">
         <v>31</v>
       </c>
+    </row>
+    <row r="64" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="1"/>
+      <c r="B64" s="2"/>
+    </row>
+    <row r="65" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="1"/>
+      <c r="B65" s="2"/>
+    </row>
+    <row r="66" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="1"/>
+      <c r="B66" s="2"/>
+    </row>
+    <row r="67" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="1"/>
+      <c r="B67" s="2"/>
     </row>
     <row r="68" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
@@ -1097,33 +1100,23 @@
       <c r="A69" s="1"/>
       <c r="B69" s="2"/>
     </row>
-    <row r="70" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="1"/>
-      <c r="B70" s="2"/>
-    </row>
     <row r="71" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A71" s="1"/>
+      <c r="A71" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="B71" s="2"/>
     </row>
-    <row r="72" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="1"/>
-      <c r="B72" s="2"/>
-    </row>
     <row r="73" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="1"/>
+      <c r="A73" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="B73" s="2"/>
     </row>
     <row r="75" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B75" s="2"/>
-    </row>
-    <row r="77" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B77" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adds returning to main view
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="339" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73DA380A-8FD3-4F61-86F4-F2013C7A3AB2}"/>
+  <xr:revisionPtr revIDLastSave="353" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D85851A-8886-4EE3-A312-205AE382F046}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>Stand</t>
   </si>
@@ -396,6 +396,15 @@
   </si>
   <si>
     <t>gleiche Pfade in env Variable</t>
+  </si>
+  <si>
+    <t>Für den aktiven User eine Klasse mit Singelton pattern und properties machen mit Rollen. Dann habe ich es überall</t>
+  </si>
+  <si>
+    <t>In das Requirement Paper unbedingt einen go back button eintragen</t>
+  </si>
+  <si>
+    <t>abstrakte Klasse für alle Screens mit dem Go Back to Main Button</t>
   </si>
 </sst>
 </file>
@@ -527,13 +536,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>119</xdr:row>
+      <xdr:row>126</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>133</xdr:row>
+      <xdr:row>140</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -588,14 +597,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>91</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2680447</xdr:colOff>
-      <xdr:row>104</xdr:row>
-      <xdr:rowOff>14930</xdr:rowOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>14929</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -632,14 +641,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1206910</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>197222</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -687,13 +696,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2599763</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>158071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4464852</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>81114</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1008,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G142"/>
+  <dimension ref="A1:G149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1019,7 +1028,7 @@
     <col min="2" max="2" width="81" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1027,147 +1036,153 @@
         <v>45836</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>48</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
+    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>36</v>
-      </c>
+    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
       <c r="B16" s="2"/>
-      <c r="G16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
+    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>53</v>
+      </c>
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
+    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
+      <c r="G23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
     </row>
@@ -1175,14 +1190,16 @@
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
     </row>
+    <row r="34" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="2"/>
+    </row>
     <row r="35" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
     </row>
     <row r="36" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="s">
-        <v>39</v>
-      </c>
+      <c r="A36" s="1"/>
       <c r="B36" s="2"/>
     </row>
     <row r="37" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1190,9 +1207,7 @@
       <c r="B37" s="2"/>
     </row>
     <row r="38" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
-        <v>45</v>
-      </c>
+      <c r="A38" s="1"/>
       <c r="B38" s="2"/>
     </row>
     <row r="39" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1200,327 +1215,355 @@
       <c r="B39" s="2"/>
     </row>
     <row r="40" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="7" t="s">
-        <v>44</v>
-      </c>
+      <c r="A40" s="1"/>
       <c r="B40" s="2"/>
-    </row>
-    <row r="41" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="1"/>
-      <c r="B41" s="2"/>
     </row>
     <row r="42" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
     </row>
     <row r="43" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="1"/>
+      <c r="A43" s="7" t="s">
+        <v>39</v>
+      </c>
       <c r="B43" s="2"/>
     </row>
     <row r="44" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="7" t="s">
-        <v>31</v>
-      </c>
+      <c r="A44" s="1"/>
       <c r="B44" s="2"/>
     </row>
     <row r="45" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="7"/>
+      <c r="A45" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="B45" s="2"/>
     </row>
     <row r="46" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="7"/>
+      <c r="A46" s="1"/>
       <c r="B46" s="2"/>
     </row>
     <row r="47" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
+      <c r="B48" s="2"/>
+    </row>
+    <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="1"/>
+      <c r="B49" s="2"/>
+    </row>
+    <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+      <c r="B50" s="2"/>
+    </row>
+    <row r="51" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B51" s="2"/>
+    </row>
+    <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="7"/>
+      <c r="B52" s="2"/>
+    </row>
+    <row r="53" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="7"/>
+      <c r="B53" s="2"/>
+    </row>
+    <row r="54" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B47" s="2"/>
-    </row>
-    <row r="48" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="7"/>
-      <c r="B48" s="2"/>
-    </row>
-    <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="B54" s="2"/>
+    </row>
+    <row r="55" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="7"/>
+      <c r="B55" s="2"/>
+    </row>
+    <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="7"/>
-      <c r="B50" s="2"/>
-    </row>
-    <row r="51" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="7"/>
-      <c r="B51" s="2"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
+      <c r="B56" s="2"/>
+    </row>
+    <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="7"/>
+      <c r="B57" s="2"/>
+    </row>
+    <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="7"/>
+      <c r="B58" s="2"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="4" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="4"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="4"/>
-    </row>
-    <row r="58" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="6" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="4"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="4"/>
+    </row>
+    <row r="65" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="3"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="4" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="3"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="3"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="4" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="3"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="4" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="3"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="4" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="3"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="4" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="4" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="4" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" s="3"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" s="5" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="3"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="4" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="5" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" s="3"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" s="3" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" s="3"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77" s="5" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" s="4" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A81" s="8" t="s">
+    <row r="88" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A88" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
+    <row r="114" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
         <v>20</v>
       </c>
-      <c r="B107" s="2"/>
-    </row>
-    <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
+      <c r="B114" s="2"/>
+    </row>
+    <row r="116" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
         <v>21</v>
       </c>
-      <c r="B109" s="2"/>
-    </row>
-    <row r="111" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A111" s="7" t="s">
+      <c r="B116" s="2"/>
+    </row>
+    <row r="118" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A118" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B111" s="2"/>
-    </row>
-    <row r="112" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A112" s="7"/>
-      <c r="B112" s="2"/>
-    </row>
-    <row r="113" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A113" s="7" t="s">
+      <c r="B118" s="2"/>
+    </row>
+    <row r="119" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A119" s="7"/>
+      <c r="B119" s="2"/>
+    </row>
+    <row r="120" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A120" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B113" s="2"/>
-    </row>
-    <row r="114" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A114" s="7"/>
-      <c r="B114" s="2"/>
-    </row>
-    <row r="115" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A115" s="7" t="s">
+      <c r="B120" s="2"/>
+    </row>
+    <row r="121" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A121" s="7"/>
+      <c r="B121" s="2"/>
+    </row>
+    <row r="122" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A122" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B115" s="2"/>
-    </row>
-    <row r="117" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A117" s="7" t="s">
+      <c r="B122" s="2"/>
+    </row>
+    <row r="124" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A124" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B117" s="2"/>
-    </row>
-    <row r="118" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A118" s="1"/>
-      <c r="B118" s="2"/>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B119" s="9" t="s">
+      <c r="B124" s="2"/>
+    </row>
+    <row r="125" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A125" s="1"/>
+      <c r="B125" s="2"/>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B126" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" s="9"/>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A122" s="9"/>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A123" s="9"/>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" s="9" t="s">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" s="9"/>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" s="9"/>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" s="9"/>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A125" s="9" t="s">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A126" s="9" t="s">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A127" s="9"/>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A128" s="9" t="s">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" s="9"/>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A129" s="1"/>
-      <c r="B129" s="2"/>
-    </row>
-    <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A130" s="1"/>
-      <c r="B130" s="2"/>
-    </row>
-    <row r="131" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A131" s="1"/>
-      <c r="B131" s="2"/>
-    </row>
-    <row r="132" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A132" s="1"/>
-      <c r="B132" s="2"/>
-    </row>
-    <row r="133" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A133" s="1"/>
-      <c r="B133" s="2"/>
-    </row>
-    <row r="134" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A134" s="1"/>
-      <c r="B134" s="2"/>
-    </row>
     <row r="136" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A136" s="7" t="s">
+      <c r="A136" s="1"/>
+      <c r="B136" s="2"/>
+    </row>
+    <row r="137" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A137" s="1"/>
+      <c r="B137" s="2"/>
+    </row>
+    <row r="138" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A138" s="1"/>
+      <c r="B138" s="2"/>
+    </row>
+    <row r="139" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A139" s="1"/>
+      <c r="B139" s="2"/>
+    </row>
+    <row r="140" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A140" s="1"/>
+      <c r="B140" s="2"/>
+    </row>
+    <row r="141" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A141" s="1"/>
+      <c r="B141" s="2"/>
+    </row>
+    <row r="143" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A143" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B136" s="2"/>
-    </row>
-    <row r="138" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A138" s="7" t="s">
+      <c r="B143" s="2"/>
+    </row>
+    <row r="145" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A145" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B138" s="2"/>
-    </row>
-    <row r="140" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A140" s="7" t="s">
+      <c r="B145" s="2"/>
+    </row>
+    <row r="147" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A147" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B140" s="2"/>
-    </row>
-    <row r="142" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A142" s="7" t="s">
+      <c r="B147" s="2"/>
+    </row>
+    <row r="149" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A149" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B142" s="2"/>
+      <c r="B149" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
annotates the address and updates the docu
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="353" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D85851A-8886-4EE3-A312-205AE382F046}"/>
+  <xr:revisionPtr revIDLastSave="360" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A79C669-7F7C-436A-975E-2B78C0360F5D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>Stand</t>
   </si>
@@ -383,9 +383,6 @@
     <t xml:space="preserve">Rausnehmen </t>
   </si>
   <si>
-    <t>08.07.2025 -  Protokoll über Meeting mit Herrn Tatzreiter</t>
-  </si>
-  <si>
     <t>Umbauen auf Scene Switcher</t>
   </si>
   <si>
@@ -405,6 +402,12 @@
   </si>
   <si>
     <t>abstrakte Klasse für alle Screens mit dem Go Back to Main Button</t>
+  </si>
+  <si>
+    <t>next time -  Protokoll über Meeting mit Herrn Tatzreiter</t>
+  </si>
+  <si>
+    <t>Sicherheitsmechanismus wenn er Manager löscht. Der darf keine Employees mehr haben umgekehrt muss ein Controller einen Manager haben.</t>
   </si>
 </sst>
 </file>
@@ -536,13 +539,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>126</xdr:row>
+      <xdr:row>128</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>140</xdr:row>
+      <xdr:row>142</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -597,13 +600,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
-      <xdr:row>91</xdr:row>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2680447</xdr:colOff>
-      <xdr:row>111</xdr:row>
+      <xdr:row>113</xdr:row>
       <xdr:rowOff>14929</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -641,13 +644,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1206910</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>197222</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -696,13 +699,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2599763</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>158071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4464852</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>81114</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1017,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G149"/>
+  <dimension ref="A1:G151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1042,7 +1045,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2"/>
     </row>
@@ -1072,7 +1075,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="2"/>
     </row>
@@ -1082,7 +1085,7 @@
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B11" s="2"/>
     </row>
@@ -1092,7 +1095,7 @@
     </row>
     <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B13" s="2"/>
     </row>
@@ -1102,7 +1105,7 @@
     </row>
     <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B15" s="2"/>
     </row>
@@ -1112,7 +1115,7 @@
     </row>
     <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B17" s="2"/>
     </row>
@@ -1121,13 +1124,13 @@
       <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
+      <c r="A19" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
-        <v>53</v>
-      </c>
+      <c r="A20" s="1"/>
       <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1135,36 +1138,38 @@
       <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
+      <c r="A22" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="1"/>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="G23" t="s">
+      <c r="B25" s="2"/>
+      <c r="G25" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
+    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
@@ -1218,23 +1223,21 @@
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
     </row>
+    <row r="41" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="1"/>
+      <c r="B41" s="2"/>
+    </row>
     <row r="42" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B43" s="2"/>
-    </row>
     <row r="44" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
     </row>
     <row r="45" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B45" s="2"/>
     </row>
@@ -1244,7 +1247,7 @@
     </row>
     <row r="47" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B47" s="2"/>
     </row>
@@ -1253,7 +1256,9 @@
       <c r="B48" s="2"/>
     </row>
     <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="1"/>
+      <c r="A49" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="B49" s="2"/>
     </row>
     <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1261,23 +1266,21 @@
       <c r="B50" s="2"/>
     </row>
     <row r="51" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="1"/>
+      <c r="B51" s="2"/>
+    </row>
+    <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="1"/>
+      <c r="B52" s="2"/>
+    </row>
+    <row r="53" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B51" s="2"/>
-    </row>
-    <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="7"/>
-      <c r="B52" s="2"/>
-    </row>
-    <row r="53" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="7"/>
       <c r="B53" s="2"/>
     </row>
     <row r="54" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="A54" s="7"/>
       <c r="B54" s="2"/>
     </row>
     <row r="55" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1285,8 +1288,8 @@
       <c r="B55" s="2"/>
     </row>
     <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>43</v>
+      <c r="A56" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="B56" s="2"/>
     </row>
@@ -1295,59 +1298,61 @@
       <c r="B57" s="2"/>
     </row>
     <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="7"/>
+      <c r="A58" t="s">
+        <v>43</v>
+      </c>
       <c r="B58" s="2"/>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="s">
-        <v>2</v>
-      </c>
+    <row r="59" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="7"/>
+      <c r="B59" s="2"/>
+    </row>
+    <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="7"/>
+      <c r="B60" s="2"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="4"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="4"/>
-    </row>
-    <row r="65" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="6" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="4"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="4"/>
+    </row>
+    <row r="67" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="4" t="s">
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="3"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1355,108 +1360,106 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="3"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="3"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="A75" s="3"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="3"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="A80" s="3"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="3"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" s="3" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" s="3"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" s="5" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" s="4" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A88" s="8" t="s">
+    <row r="90" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A90" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
-        <v>20</v>
-      </c>
-      <c r="B114" s="2"/>
     </row>
     <row r="116" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
+        <v>20</v>
+      </c>
+      <c r="B116" s="2"/>
+    </row>
+    <row r="118" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
         <v>21</v>
       </c>
-      <c r="B116" s="2"/>
-    </row>
-    <row r="118" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A118" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="B118" s="2"/>
-    </row>
-    <row r="119" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A119" s="7"/>
-      <c r="B119" s="2"/>
     </row>
     <row r="120" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A120" s="7" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B120" s="2"/>
     </row>
@@ -1466,64 +1469,66 @@
     </row>
     <row r="122" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A122" s="7" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B122" s="2"/>
+    </row>
+    <row r="123" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A123" s="7"/>
+      <c r="B123" s="2"/>
     </row>
     <row r="124" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B124" s="2"/>
+    </row>
+    <row r="126" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A126" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B124" s="2"/>
-    </row>
-    <row r="125" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A125" s="1"/>
-      <c r="B125" s="2"/>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B126" s="9" t="s">
+      <c r="B126" s="2"/>
+    </row>
+    <row r="127" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A127" s="1"/>
+      <c r="B127" s="2"/>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B128" s="9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A128" s="9"/>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A129" s="9"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="9"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A131" s="9" t="s">
-        <v>27</v>
-      </c>
+      <c r="A131" s="9"/>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" s="9" t="s">
-        <v>28</v>
-      </c>
+      <c r="A132" s="9"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A134" s="9"/>
+      <c r="A134" s="9" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" s="9"/>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" s="9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A136" s="1"/>
-      <c r="B136" s="2"/>
-    </row>
-    <row r="137" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A137" s="1"/>
-      <c r="B137" s="2"/>
     </row>
     <row r="138" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A138" s="1"/>
@@ -1541,29 +1546,37 @@
       <c r="A141" s="1"/>
       <c r="B141" s="2"/>
     </row>
+    <row r="142" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A142" s="1"/>
+      <c r="B142" s="2"/>
+    </row>
     <row r="143" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A143" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="A143" s="1"/>
       <c r="B143" s="2"/>
     </row>
     <row r="145" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A145" s="7" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B145" s="2"/>
     </row>
     <row r="147" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A147" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B147" s="2"/>
     </row>
     <row r="149" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A149" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B149" s="2"/>
+    </row>
+    <row r="151" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A151" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B149" s="2"/>
+      <c r="B151" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adds self-reference in Person entity
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="360" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A79C669-7F7C-436A-975E-2B78C0360F5D}"/>
+  <xr:revisionPtr revIDLastSave="364" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72EFAD9D-9942-48CD-9DFE-45A11809D211}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>Stand</t>
   </si>
@@ -408,6 +408,9 @@
   </si>
   <si>
     <t>Sicherheitsmechanismus wenn er Manager löscht. Der darf keine Employees mehr haben umgekehrt muss ein Controller einen Manager haben.</t>
+  </si>
+  <si>
+    <t>roles Table nachziehen in der ERD</t>
   </si>
 </sst>
 </file>
@@ -539,13 +542,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>128</xdr:row>
+      <xdr:row>130</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>142</xdr:row>
+      <xdr:row>144</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -600,13 +603,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
-      <xdr:row>93</xdr:row>
+      <xdr:row>95</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2680447</xdr:colOff>
-      <xdr:row>113</xdr:row>
+      <xdr:row>115</xdr:row>
       <xdr:rowOff>14929</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -644,13 +647,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1206910</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>197222</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -699,13 +702,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2599763</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>158071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4464852</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>81114</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1020,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G151"/>
+  <dimension ref="A1:G153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1134,13 +1137,13 @@
       <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
+      <c r="A21" s="7" t="s">
+        <v>57</v>
+      </c>
       <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
-        <v>52</v>
-      </c>
+      <c r="A22" s="1"/>
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1148,36 +1151,38 @@
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
+      <c r="A24" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="G25" t="s">
+      <c r="B27" s="2"/>
+      <c r="G27" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
+    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="11" t="s">
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
     </row>
     <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
@@ -1231,23 +1236,21 @@
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
     </row>
+    <row r="43" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="2"/>
+    </row>
     <row r="44" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B45" s="2"/>
-    </row>
     <row r="46" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
     </row>
     <row r="47" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B47" s="2"/>
     </row>
@@ -1257,7 +1260,7 @@
     </row>
     <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B49" s="2"/>
     </row>
@@ -1266,7 +1269,9 @@
       <c r="B50" s="2"/>
     </row>
     <row r="51" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="1"/>
+      <c r="A51" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="B51" s="2"/>
     </row>
     <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1274,23 +1279,21 @@
       <c r="B52" s="2"/>
     </row>
     <row r="53" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="1"/>
+      <c r="B53" s="2"/>
+    </row>
+    <row r="54" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="1"/>
+      <c r="B54" s="2"/>
+    </row>
+    <row r="55" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B53" s="2"/>
-    </row>
-    <row r="54" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="7"/>
-      <c r="B54" s="2"/>
-    </row>
-    <row r="55" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="7"/>
       <c r="B55" s="2"/>
     </row>
     <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="A56" s="7"/>
       <c r="B56" s="2"/>
     </row>
     <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1298,8 +1301,8 @@
       <c r="B57" s="2"/>
     </row>
     <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>43</v>
+      <c r="A58" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="B58" s="2"/>
     </row>
@@ -1308,59 +1311,61 @@
       <c r="B59" s="2"/>
     </row>
     <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="7"/>
+      <c r="A60" t="s">
+        <v>43</v>
+      </c>
       <c r="B60" s="2"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="4" t="s">
-        <v>2</v>
-      </c>
+    <row r="61" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="7"/>
+      <c r="B61" s="2"/>
+    </row>
+    <row r="62" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="7"/>
+      <c r="B62" s="2"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="4"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="4"/>
-    </row>
-    <row r="67" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="6" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="4"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="4"/>
+    </row>
+    <row r="69" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="4" t="s">
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="3"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -1368,108 +1373,106 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="3"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="3"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="A77" s="3"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="3"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="A82" s="3"/>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" s="3"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" s="3" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" s="3"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" s="5" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" s="4" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A90" s="8" t="s">
+    <row r="92" spans="1:1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A92" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>20</v>
-      </c>
-      <c r="B116" s="2"/>
     </row>
     <row r="118" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
+        <v>20</v>
+      </c>
+      <c r="B118" s="2"/>
+    </row>
+    <row r="120" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
         <v>21</v>
       </c>
-      <c r="B118" s="2"/>
-    </row>
-    <row r="120" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A120" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="B120" s="2"/>
-    </row>
-    <row r="121" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A121" s="7"/>
-      <c r="B121" s="2"/>
     </row>
     <row r="122" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A122" s="7" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B122" s="2"/>
     </row>
@@ -1479,64 +1482,66 @@
     </row>
     <row r="124" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" s="7" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B124" s="2"/>
+    </row>
+    <row r="125" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A125" s="7"/>
+      <c r="B125" s="2"/>
     </row>
     <row r="126" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A126" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B126" s="2"/>
+    </row>
+    <row r="128" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A128" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B126" s="2"/>
-    </row>
-    <row r="127" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A127" s="1"/>
-      <c r="B127" s="2"/>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B128" s="9" t="s">
+      <c r="B128" s="2"/>
+    </row>
+    <row r="129" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A129" s="1"/>
+      <c r="B129" s="2"/>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B130" s="9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A130" s="9"/>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A131" s="9"/>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="9"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A133" s="9" t="s">
-        <v>27</v>
-      </c>
+      <c r="A133" s="9"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A134" s="9" t="s">
-        <v>28</v>
-      </c>
+      <c r="A134" s="9"/>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A136" s="9"/>
+      <c r="A136" s="9" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" s="9"/>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" s="9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A138" s="1"/>
-      <c r="B138" s="2"/>
-    </row>
-    <row r="139" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A139" s="1"/>
-      <c r="B139" s="2"/>
     </row>
     <row r="140" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A140" s="1"/>
@@ -1554,29 +1559,37 @@
       <c r="A143" s="1"/>
       <c r="B143" s="2"/>
     </row>
+    <row r="144" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A144" s="1"/>
+      <c r="B144" s="2"/>
+    </row>
     <row r="145" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A145" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="A145" s="1"/>
       <c r="B145" s="2"/>
     </row>
     <row r="147" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A147" s="7" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B147" s="2"/>
     </row>
     <row r="149" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A149" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B149" s="2"/>
     </row>
     <row r="151" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A151" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B151" s="2"/>
+    </row>
+    <row r="153" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A153" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B151" s="2"/>
+      <c r="B153" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adds entity manager provider and closes the factory in the shutdown process
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="364" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72EFAD9D-9942-48CD-9DFE-45A11809D211}"/>
+  <xr:revisionPtr revIDLastSave="385" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB21E6A8-64F6-4E21-9260-06F3B9167F78}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9510" yWindow="-70" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Stand</t>
   </si>
@@ -66,239 +66,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>private HBox hbox</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>private ObservableList&lt;Zahlungsart&gt; zahlungsartList</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>;</t>
-    </r>
-  </si>
-  <si>
-    <t>// Eigener ExecutorService für dieses Fenster</t>
-  </si>
-  <si>
-    <r>
-      <t>private ExecutorService executorService</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>;</t>
-    </r>
-  </si>
-  <si>
-    <t>@Override</t>
-  </si>
-  <si>
-    <r>
-      <t>public void initialize(URL url</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>ResourceBundle rb) {</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">    // ExecutorService erstellen</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    executorService = Executors.</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>newFixedThreadPool</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>// GUI initialisieren</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    zahlungsartList = FXCollections.</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>observableArrayList</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>()</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>listViewZahlungsart.setItems(zahlungsartList)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>;</t>
-    </r>
-  </si>
-  <si>
-    <t>……</t>
-  </si>
-  <si>
-    <t>MAPPING MIT DER ID VON HBOX IN FXML</t>
-  </si>
-  <si>
-    <t>Hier kann ich Prüfen und Ansprechen je nach Rolle</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>hbox.setVisible(false)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>;</t>
-    </r>
-  </si>
-  <si>
     <t>Scope, Nicht-Scope, funktionale Anforderungen( habe ich schon), nicht funktionale Anforderungen, Overview Ziel reinschreiben, Benutzerschnittstellen sind einzelne Windows,</t>
   </si>
   <si>
@@ -386,9 +153,6 @@
     <t>Umbauen auf Scene Switcher</t>
   </si>
   <si>
-    <t>First  data to login</t>
-  </si>
-  <si>
     <t xml:space="preserve">Rollen Argumente bei Login an Views übergeben </t>
   </si>
   <si>
@@ -411,13 +175,16 @@
   </si>
   <si>
     <t>roles Table nachziehen in der ERD</t>
+  </si>
+  <si>
+    <t>Entity Manager closed from every screen and from login button</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -441,13 +208,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos"/>
@@ -509,11 +269,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -542,13 +302,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>130</xdr:row>
+      <xdr:row>134</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>144</xdr:row>
+      <xdr:row>148</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -603,14 +363,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:row>99</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2680447</xdr:colOff>
-      <xdr:row>115</xdr:row>
-      <xdr:rowOff>14929</xdr:rowOff>
+      <xdr:colOff>2685527</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>18740</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -647,14 +407,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1206910</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>197222</xdr:rowOff>
+      <xdr:colOff>1200560</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>193412</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -702,14 +462,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2599763</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>158071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4464852</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>81114</xdr:rowOff>
+      <xdr:colOff>4461042</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>79844</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1023,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G153"/>
+  <dimension ref="A1:G157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1048,7 +808,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="B3" s="2"/>
     </row>
@@ -1058,17 +818,16 @@
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2"/>
     </row>
@@ -1078,7 +837,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B9" s="2"/>
     </row>
@@ -1088,7 +847,7 @@
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B11" s="2"/>
     </row>
@@ -1098,7 +857,7 @@
     </row>
     <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2"/>
     </row>
@@ -1108,7 +867,7 @@
     </row>
     <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B15" s="2"/>
     </row>
@@ -1118,7 +877,7 @@
     </row>
     <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B17" s="2"/>
     </row>
@@ -1128,7 +887,7 @@
     </row>
     <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B19" s="2"/>
     </row>
@@ -1138,7 +897,7 @@
     </row>
     <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="B21" s="2"/>
     </row>
@@ -1152,37 +911,35 @@
     </row>
     <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="B24" s="2"/>
+      <c r="G24" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
+      <c r="A25" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
+    <row r="26" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
-        <v>36</v>
-      </c>
+      <c r="A27" s="1"/>
       <c r="B27" s="2"/>
-      <c r="G27" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="A28" s="1"/>
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="11" t="s">
-        <v>37</v>
-      </c>
+    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="2"/>
     </row>
     <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
@@ -1232,36 +989,38 @@
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="1"/>
-      <c r="B42" s="2"/>
-    </row>
     <row r="43" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
     </row>
     <row r="44" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="1"/>
+      <c r="A44" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="B44" s="2"/>
     </row>
+    <row r="45" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="2"/>
+    </row>
     <row r="46" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="1"/>
+      <c r="A46" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="B46" s="2"/>
     </row>
     <row r="47" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="7" t="s">
-        <v>39</v>
-      </c>
+      <c r="A47" s="1"/>
       <c r="B47" s="2"/>
     </row>
     <row r="48" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="1"/>
+      <c r="A48" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="B48" s="2"/>
     </row>
     <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="7" t="s">
-        <v>45</v>
-      </c>
+      <c r="A49" s="1"/>
       <c r="B49" s="2"/>
     </row>
     <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1269,80 +1028,62 @@
       <c r="B50" s="2"/>
     </row>
     <row r="51" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="7" t="s">
-        <v>44</v>
-      </c>
+      <c r="A51" s="1"/>
       <c r="B51" s="2"/>
     </row>
     <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="1"/>
+      <c r="A52" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="B52" s="2"/>
     </row>
     <row r="53" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="1"/>
+      <c r="A53" s="7"/>
       <c r="B53" s="2"/>
     </row>
     <row r="54" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="1"/>
+      <c r="A54" s="7"/>
       <c r="B54" s="2"/>
     </row>
-    <row r="55" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B55" s="2"/>
-    </row>
-    <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="7"/>
-      <c r="B56" s="2"/>
-    </row>
-    <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="7"/>
-      <c r="B57" s="2"/>
-    </row>
     <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="A58" s="7"/>
       <c r="B58" s="2"/>
     </row>
     <row r="59" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="7"/>
       <c r="B59" s="2"/>
     </row>
-    <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>43</v>
-      </c>
-      <c r="B60" s="2"/>
-    </row>
-    <row r="61" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="7"/>
-      <c r="B61" s="2"/>
-    </row>
-    <row r="62" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="7"/>
-      <c r="B62" s="2"/>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="A64" s="4"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A65" s="4"/>
+    </row>
+    <row r="66" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="6"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="4"/>
@@ -1350,214 +1091,182 @@
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="4"/>
     </row>
-    <row r="69" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="3"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A70" s="4"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="A71" s="3"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="3"/>
+      <c r="A72" s="4"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="A73" s="4"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="3"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="4" t="s">
+      <c r="A75" s="4"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="4"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="4"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="4"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="3"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="5"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" s="4"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" s="5"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" s="3"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" s="3"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" s="5"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" s="4"/>
+    </row>
+    <row r="89" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A89" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="3"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="3"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" s="3"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A92" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A90" s="8"/>
+    </row>
+    <row r="91" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A91" s="8"/>
+    </row>
+    <row r="92" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A92" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B92" s="2"/>
+    </row>
+    <row r="93" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A93" s="7"/>
+      <c r="B93" s="2"/>
+    </row>
+    <row r="94" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
-        <v>20</v>
-      </c>
-      <c r="B118" s="2"/>
-    </row>
-    <row r="120" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
-        <v>21</v>
-      </c>
-      <c r="B120" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="B94" s="2"/>
+    </row>
+    <row r="96" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A96" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B96" s="2"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="122" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A122" s="7" t="s">
-        <v>23</v>
+      <c r="A122" t="s">
+        <v>5</v>
       </c>
       <c r="B122" s="2"/>
     </row>
-    <row r="123" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A123" s="7"/>
-      <c r="B123" s="2"/>
-    </row>
     <row r="124" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A124" s="7" t="s">
-        <v>42</v>
+      <c r="A124" t="s">
+        <v>6</v>
       </c>
       <c r="B124" s="2"/>
-    </row>
-    <row r="125" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A125" s="7"/>
-      <c r="B125" s="2"/>
     </row>
     <row r="126" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A126" s="7" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="B126" s="2"/>
+    </row>
+    <row r="127" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A127" s="7"/>
+      <c r="B127" s="2"/>
     </row>
     <row r="128" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A128" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B128" s="2"/>
     </row>
     <row r="129" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A129" s="1"/>
+      <c r="A129" s="7"/>
       <c r="B129" s="2"/>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B130" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" s="9"/>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A133" s="9"/>
+    <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A130" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B130" s="2"/>
+    </row>
+    <row r="132" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A132" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B132" s="2"/>
+    </row>
+    <row r="133" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A133" s="1"/>
+      <c r="B133" s="2"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A134" s="9"/>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A135" s="9" t="s">
-        <v>27</v>
+      <c r="B134" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A136" s="9" t="s">
-        <v>28</v>
-      </c>
+      <c r="A136" s="9"/>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A137" s="9" t="s">
-        <v>29</v>
-      </c>
+      <c r="A137" s="9"/>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="9"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A140" s="1"/>
-      <c r="B140" s="2"/>
-    </row>
-    <row r="141" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A141" s="1"/>
-      <c r="B141" s="2"/>
-    </row>
-    <row r="142" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A142" s="1"/>
-      <c r="B142" s="2"/>
-    </row>
-    <row r="143" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A143" s="1"/>
-      <c r="B143" s="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" s="9"/>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="144" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A144" s="1"/>
@@ -1567,29 +1276,45 @@
       <c r="A145" s="1"/>
       <c r="B145" s="2"/>
     </row>
+    <row r="146" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A146" s="1"/>
+      <c r="B146" s="2"/>
+    </row>
     <row r="147" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A147" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="A147" s="1"/>
       <c r="B147" s="2"/>
     </row>
+    <row r="148" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A148" s="1"/>
+      <c r="B148" s="2"/>
+    </row>
     <row r="149" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A149" s="7" t="s">
-        <v>32</v>
-      </c>
+      <c r="A149" s="1"/>
       <c r="B149" s="2"/>
     </row>
     <row r="151" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A151" s="7" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="B151" s="2"/>
     </row>
     <row r="153" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A153" s="7" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B153" s="2"/>
+    </row>
+    <row r="155" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A155" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B155" s="2"/>
+    </row>
+    <row r="157" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A157" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B157" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adds the possibility to query for persons
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="385" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB21E6A8-64F6-4E21-9260-06F3B9167F78}"/>
+  <xr:revisionPtr revIDLastSave="392" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{907086AE-9767-4FF5-9AE6-65A4AF5A45D7}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="-70" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Stand</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Entity Manager closed from every screen and from login button</t>
+  </si>
+  <si>
+    <t>1. Zuerst Login fertig mit DAO und controller dann restliche CRUD Personen Operationen</t>
   </si>
 </sst>
 </file>
@@ -302,13 +305,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>134</xdr:row>
+      <xdr:row>136</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>148</xdr:row>
+      <xdr:row>150</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -363,14 +366,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
-      <xdr:row>99</xdr:row>
+      <xdr:row>101</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2685527</xdr:colOff>
-      <xdr:row>119</xdr:row>
-      <xdr:rowOff>18740</xdr:rowOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>18739</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -407,13 +410,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1200560</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>193412</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -462,13 +465,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2599763</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>158071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4461042</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>79844</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -783,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G157"/>
+  <dimension ref="A1:G159"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -827,17 +830,15 @@
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="2"/>
+        <v>43</v>
+      </c>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B9" s="2"/>
     </row>
@@ -847,7 +848,7 @@
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B11" s="2"/>
     </row>
@@ -857,7 +858,7 @@
     </row>
     <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B13" s="2"/>
     </row>
@@ -867,7 +868,7 @@
     </row>
     <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="2"/>
     </row>
@@ -877,7 +878,7 @@
     </row>
     <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B17" s="2"/>
     </row>
@@ -887,7 +888,7 @@
     </row>
     <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B19" s="2"/>
     </row>
@@ -897,7 +898,7 @@
     </row>
     <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B21" s="2"/>
     </row>
@@ -906,36 +907,38 @@
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
+      <c r="A23" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="G24" t="s">
+      <c r="B26" s="2"/>
+      <c r="G26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
@@ -989,23 +992,21 @@
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
     </row>
+    <row r="42" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="2"/>
+    </row>
     <row r="43" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B44" s="2"/>
-    </row>
     <row r="45" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
     </row>
     <row r="46" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B46" s="2"/>
     </row>
@@ -1015,7 +1016,7 @@
     </row>
     <row r="48" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B48" s="2"/>
     </row>
@@ -1024,7 +1025,9 @@
       <c r="B49" s="2"/>
     </row>
     <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="1"/>
+      <c r="A50" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="B50" s="2"/>
     </row>
     <row r="51" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1032,67 +1035,69 @@
       <c r="B51" s="2"/>
     </row>
     <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="1"/>
+      <c r="B52" s="2"/>
+    </row>
+    <row r="53" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
+      <c r="B53" s="2"/>
+    </row>
+    <row r="54" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B52" s="2"/>
-    </row>
-    <row r="53" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="7"/>
-      <c r="B53" s="2"/>
-    </row>
-    <row r="54" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="7"/>
       <c r="B54" s="2"/>
     </row>
-    <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="7"/>
-      <c r="B58" s="2"/>
-    </row>
-    <row r="59" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="7"/>
-      <c r="B59" s="2"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="4" t="s">
-        <v>2</v>
-      </c>
+    <row r="55" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="7"/>
+      <c r="B55" s="2"/>
+    </row>
+    <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="7"/>
+      <c r="B56" s="2"/>
+    </row>
+    <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="7"/>
+      <c r="B60" s="2"/>
+    </row>
+    <row r="61" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="7"/>
+      <c r="B61" s="2"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="4"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="4"/>
-    </row>
-    <row r="66" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="6"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="4"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="4"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="4"/>
+    <row r="68" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="6"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="3"/>
+      <c r="A69" s="4"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="4"/>
@@ -1104,16 +1109,16 @@
       <c r="A72" s="4"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="4"/>
+      <c r="A73" s="3"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="3"/>
+      <c r="A74" s="4"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="4"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="4"/>
+      <c r="A76" s="3"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="4"/>
@@ -1122,92 +1127,88 @@
       <c r="A78" s="4"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="3"/>
+      <c r="A79" s="4"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="5"/>
+      <c r="A80" s="4"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" s="4"/>
+      <c r="A81" s="3"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="5"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="3"/>
+      <c r="A83" s="4"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" s="3"/>
+      <c r="A84" s="5"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" s="5"/>
+      <c r="A85" s="3"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" s="4"/>
-    </row>
-    <row r="89" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A89" s="8" t="s">
+      <c r="A86" s="3"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" s="5"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" s="4"/>
+    </row>
+    <row r="91" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A91" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A90" s="8"/>
-    </row>
-    <row r="91" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A91" s="8"/>
-    </row>
-    <row r="92" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A92" s="7" t="s">
+    <row r="92" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A92" s="8"/>
+    </row>
+    <row r="93" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A93" s="8"/>
+    </row>
+    <row r="94" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A94" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B92" s="2"/>
-    </row>
-    <row r="93" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A93" s="7"/>
-      <c r="B93" s="2"/>
-    </row>
-    <row r="94" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
+      <c r="B94" s="2"/>
+    </row>
+    <row r="95" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A95" s="7"/>
+      <c r="B95" s="2"/>
+    </row>
+    <row r="96" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>28</v>
       </c>
-      <c r="B94" s="2"/>
-    </row>
-    <row r="96" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A96" s="7" t="s">
+      <c r="B96" s="2"/>
+    </row>
+    <row r="98" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A98" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B96" s="2"/>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+      <c r="B98" s="2"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
-        <v>5</v>
-      </c>
-      <c r="B122" s="2"/>
     </row>
     <row r="124" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
+        <v>5</v>
+      </c>
+      <c r="B124" s="2"/>
+    </row>
+    <row r="126" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
         <v>6</v>
       </c>
-      <c r="B124" s="2"/>
-    </row>
-    <row r="126" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A126" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="B126" s="2"/>
-    </row>
-    <row r="127" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A127" s="7"/>
-      <c r="B127" s="2"/>
     </row>
     <row r="128" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A128" s="7" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B128" s="2"/>
     </row>
@@ -1217,64 +1218,66 @@
     </row>
     <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A130" s="7" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B130" s="2"/>
+    </row>
+    <row r="131" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A131" s="7"/>
+      <c r="B131" s="2"/>
     </row>
     <row r="132" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A132" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B132" s="2"/>
+    </row>
+    <row r="134" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A134" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B132" s="2"/>
-    </row>
-    <row r="133" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A133" s="1"/>
-      <c r="B133" s="2"/>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B134" s="9" t="s">
+      <c r="B134" s="2"/>
+    </row>
+    <row r="135" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A135" s="1"/>
+      <c r="B135" s="2"/>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B136" s="9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A136" s="9"/>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A137" s="9"/>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="9"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A139" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="A139" s="9"/>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A140" s="9" t="s">
-        <v>13</v>
-      </c>
+      <c r="A140" s="9"/>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" s="9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A142" s="9"/>
+      <c r="A142" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" s="9"/>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A144" s="1"/>
-      <c r="B144" s="2"/>
-    </row>
-    <row r="145" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A145" s="1"/>
-      <c r="B145" s="2"/>
     </row>
     <row r="146" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A146" s="1"/>
@@ -1292,29 +1295,37 @@
       <c r="A149" s="1"/>
       <c r="B149" s="2"/>
     </row>
+    <row r="150" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A150" s="1"/>
+      <c r="B150" s="2"/>
+    </row>
     <row r="151" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A151" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="A151" s="1"/>
       <c r="B151" s="2"/>
     </row>
     <row r="153" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A153" s="7" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B153" s="2"/>
     </row>
     <row r="155" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A155" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B155" s="2"/>
     </row>
     <row r="157" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A157" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B157" s="2"/>
+    </row>
+    <row r="159" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A159" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B157" s="2"/>
+      <c r="B159" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adds basics for time booking
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="414" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4EC75FC-B01B-45EA-BA4E-469CA8C9293F}"/>
+  <xr:revisionPtr revIDLastSave="429" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5E00B9F-3EB2-4D05-9754-BE196BA58B31}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="-70" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Stand</t>
   </si>
@@ -180,9 +180,6 @@
     <t>Entity Manager closed from every screen and from login button</t>
   </si>
   <si>
-    <t>1. Zuerst Login fertig mit DAO und controller dann restliche CRUD Personen Operationen</t>
-  </si>
-  <si>
     <t>Subordinates in DAO</t>
   </si>
   <si>
@@ -190,9 +187,6 @@
   </si>
   <si>
     <t>Wenn ich auf Logout button gehe context clearen</t>
-  </si>
-  <si>
-    <t>Konditional einblenden das main menu</t>
   </si>
 </sst>
 </file>
@@ -302,13 +296,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>125</xdr:row>
+      <xdr:row>113</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>139</xdr:row>
+      <xdr:row>127</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -363,14 +357,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
-      <xdr:row>90</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2685527</xdr:colOff>
-      <xdr:row>110</xdr:row>
-      <xdr:rowOff>18739</xdr:rowOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>18740</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -407,14 +401,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1200560</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>193412</xdr:rowOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>193413</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -462,14 +456,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2599763</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>158071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4461042</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>79845</xdr:rowOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>79844</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -783,10 +777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G150"/>
+  <dimension ref="A1:G144"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -817,41 +811,41 @@
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+      <c r="A5" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="2" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
+      <c r="A9" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-    </row>
     <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
+      <c r="A13" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -859,163 +853,138 @@
       <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
+      <c r="A15" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="A16" s="1"/>
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>20</v>
-      </c>
+    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
+      <c r="G22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>34</v>
-      </c>
+    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
-        <v>35</v>
-      </c>
+    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>38</v>
-      </c>
+    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>41</v>
-      </c>
+    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
       <c r="B32" s="2"/>
     </row>
-    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>36</v>
-      </c>
+    <row r="34" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
       <c r="B34" s="2"/>
     </row>
-    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
-        <v>21</v>
-      </c>
+    <row r="37" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
       <c r="B37" s="2"/>
-      <c r="G37" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
-        <v>25</v>
-      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
-      <c r="B40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="2"/>
+    </row>
+    <row r="41" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="1"/>
+    <row r="42" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="1"/>
+    <row r="44" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="1"/>
+    <row r="46" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
     </row>
@@ -1024,292 +993,267 @@
       <c r="B49" s="2"/>
     </row>
     <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="1"/>
+      <c r="A50" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="B50" s="2"/>
     </row>
     <row r="51" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="1"/>
+      <c r="A51" s="4"/>
       <c r="B51" s="2"/>
     </row>
     <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="1"/>
+      <c r="A52" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="B52" s="2"/>
     </row>
-    <row r="53" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="1"/>
-      <c r="B53" s="2"/>
-    </row>
-    <row r="54" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="1"/>
-      <c r="B54" s="2"/>
-    </row>
     <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="1"/>
+      <c r="A56" s="4"/>
       <c r="B56" s="2"/>
     </row>
     <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="A57" s="4"/>
       <c r="B57" s="2"/>
     </row>
-    <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="1"/>
-      <c r="B58" s="2"/>
-    </row>
-    <row r="59" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B59" s="2"/>
-    </row>
-    <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="1"/>
-      <c r="B60" s="2"/>
-    </row>
-    <row r="61" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B61" s="2"/>
-    </row>
-    <row r="62" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="1"/>
-      <c r="B62" s="2"/>
-    </row>
-    <row r="63" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="1"/>
-      <c r="B63" s="2"/>
-    </row>
-    <row r="64" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="1"/>
-      <c r="B64" s="2"/>
-    </row>
-    <row r="65" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B65" s="2"/>
-    </row>
-    <row r="66" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="4"/>
-      <c r="B66" s="2"/>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="3"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="3"/>
+    </row>
+    <row r="65" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A65" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A66" s="5"/>
     </row>
     <row r="67" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="9" t="s">
-        <v>44</v>
+      <c r="A67" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="B67" s="2"/>
     </row>
+    <row r="68" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A68" s="5"/>
+    </row>
+    <row r="69" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B69" s="2"/>
+    </row>
+    <row r="70" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A70" s="5"/>
+    </row>
     <row r="71" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A71" s="4"/>
+      <c r="A71" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="B71" s="2"/>
     </row>
     <row r="72" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="4"/>
       <c r="B72" s="2"/>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="3" t="s">
-        <v>4</v>
-      </c>
+    <row r="73" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>28</v>
+      </c>
+      <c r="B73" s="2"/>
+    </row>
+    <row r="75" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B75" s="2"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="3"/>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="3"/>
-    </row>
-    <row r="80" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A80" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A81" s="5"/>
-    </row>
-    <row r="82" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A82" s="5"/>
-    </row>
-    <row r="83" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B83" s="2"/>
-    </row>
-    <row r="84" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A84" s="4"/>
-      <c r="B84" s="2"/>
-    </row>
-    <row r="85" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>28</v>
-      </c>
-      <c r="B85" s="2"/>
-    </row>
-    <row r="87" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A87" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B87" s="2"/>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+      <c r="A77" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
+    <row r="101" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>5</v>
       </c>
-      <c r="B113" s="2"/>
-    </row>
-    <row r="115" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
+      <c r="B101" s="2"/>
+    </row>
+    <row r="103" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
         <v>6</v>
       </c>
-      <c r="B115" s="2"/>
-    </row>
-    <row r="117" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A117" s="4" t="s">
+      <c r="B103" s="2"/>
+    </row>
+    <row r="105" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A105" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B117" s="2"/>
-    </row>
-    <row r="118" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A118" s="4"/>
-      <c r="B118" s="2"/>
-    </row>
-    <row r="119" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A119" s="4" t="s">
+      <c r="B105" s="2"/>
+    </row>
+    <row r="106" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A106" s="4"/>
+      <c r="B106" s="2"/>
+    </row>
+    <row r="107" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A107" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B119" s="2"/>
-    </row>
-    <row r="120" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A120" s="4"/>
-      <c r="B120" s="2"/>
-    </row>
-    <row r="121" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A121" s="4" t="s">
+      <c r="B107" s="2"/>
+    </row>
+    <row r="108" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A108" s="4"/>
+      <c r="B108" s="2"/>
+    </row>
+    <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A109" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B121" s="2"/>
+      <c r="B109" s="2"/>
+    </row>
+    <row r="111" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A111" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B111" s="2"/>
+    </row>
+    <row r="112" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A112" s="1"/>
+      <c r="B112" s="2"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B113" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" s="6"/>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" s="6"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" s="6"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" s="6"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="123" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A123" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="A123" s="1"/>
       <c r="B123" s="2"/>
     </row>
     <row r="124" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" s="1"/>
       <c r="B124" s="2"/>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B125" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A127" s="6"/>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A128" s="6"/>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A129" s="6"/>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A130" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A131" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A133" s="6"/>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A134" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A135" s="1"/>
-      <c r="B135" s="2"/>
+    <row r="125" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A125" s="1"/>
+      <c r="B125" s="2"/>
+    </row>
+    <row r="126" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A126" s="1"/>
+      <c r="B126" s="2"/>
+    </row>
+    <row r="127" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A127" s="1"/>
+      <c r="B127" s="2"/>
+    </row>
+    <row r="128" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A128" s="1"/>
+      <c r="B128" s="2"/>
+    </row>
+    <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A130" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B130" s="2"/>
+    </row>
+    <row r="132" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A132" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B132" s="2"/>
+    </row>
+    <row r="134" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A134" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B134" s="2"/>
     </row>
     <row r="136" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A136" s="1"/>
+      <c r="A136" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="B136" s="2"/>
     </row>
-    <row r="137" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A137" s="1"/>
-      <c r="B137" s="2"/>
-    </row>
     <row r="138" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A138" s="1"/>
-      <c r="B138" s="2"/>
-    </row>
-    <row r="139" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A139" s="1"/>
-      <c r="B139" s="2"/>
+      <c r="A138" s="9" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="140" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A140" s="1"/>
+      <c r="A140" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="B140" s="2"/>
+    </row>
+    <row r="141" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A141" s="1"/>
+      <c r="B141" s="2"/>
     </row>
     <row r="142" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A142" s="4" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="B142" s="2"/>
     </row>
     <row r="144" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A144" s="4" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="B144" s="2"/>
-    </row>
-    <row r="146" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A146" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B146" s="2"/>
-    </row>
-    <row r="148" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A148" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B148" s="2"/>
-    </row>
-    <row r="150" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A150" s="9" t="s">
-        <v>46</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Builds request and maps it to person
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="429" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5E00B9F-3EB2-4D05-9754-BE196BA58B31}"/>
+  <xr:revisionPtr revIDLastSave="441" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0D8EEC6-825E-457E-8D5E-4402B4BD115E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Stand</t>
   </si>
@@ -180,13 +180,19 @@
     <t>Entity Manager closed from every screen and from login button</t>
   </si>
   <si>
-    <t>Subordinates in DAO</t>
-  </si>
-  <si>
     <t>Länge von Username und Passwort in der DB gleichziehen</t>
   </si>
   <si>
     <t>Wenn ich auf Logout button gehe context clearen</t>
+  </si>
+  <si>
+    <t>Rework the vacations screen for Admins and managers - different texts  - auto booking - Requirements anpassen</t>
+  </si>
+  <si>
+    <t>Requirements mit Projekt abstimmen</t>
+  </si>
+  <si>
+    <t>Class diagramm</t>
   </si>
 </sst>
 </file>
@@ -296,13 +302,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>113</xdr:row>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>127</xdr:row>
+      <xdr:row>133</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -357,13 +363,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2685527</xdr:colOff>
-      <xdr:row>98</xdr:row>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3295127</xdr:colOff>
+      <xdr:row>104</xdr:row>
       <xdr:rowOff>18740</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -401,13 +407,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1200560</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1810160</xdr:colOff>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>193413</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -456,13 +462,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2599763</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>158071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4461042</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>79844</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -777,14 +783,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G144"/>
+  <dimension ref="A1:G150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="168.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="81" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -812,7 +819,7 @@
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -838,61 +845,52 @@
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
     </row>
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+    </row>
     <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
+      <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
+      <c r="A21" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="A22" s="1"/>
       <c r="B22" s="2"/>
-      <c r="G22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
@@ -903,16 +901,24 @@
       <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
+      <c r="A28" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="B28" s="2"/>
+      <c r="G28" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
+      <c r="A29" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
+    <row r="30" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
@@ -950,14 +956,16 @@
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
     </row>
+    <row r="40" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="2"/>
+    </row>
     <row r="41" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
     </row>
     <row r="42" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="A42" s="1"/>
       <c r="B42" s="2"/>
     </row>
     <row r="43" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -965,27 +973,21 @@
       <c r="B43" s="2"/>
     </row>
     <row r="44" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
-        <v>30</v>
-      </c>
+      <c r="A44" s="1"/>
       <c r="B44" s="2"/>
     </row>
     <row r="45" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B46" s="2"/>
-    </row>
     <row r="47" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
     </row>
     <row r="48" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="1"/>
+      <c r="A48" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="B48" s="2"/>
     </row>
     <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -994,266 +996,292 @@
     </row>
     <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B50" s="2"/>
+    </row>
+    <row r="51" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="1"/>
+      <c r="B51" s="2"/>
+    </row>
+    <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B52" s="2"/>
+    </row>
+    <row r="53" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
+      <c r="B53" s="2"/>
+    </row>
+    <row r="54" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="1"/>
+      <c r="B54" s="2"/>
+    </row>
+    <row r="55" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="1"/>
+      <c r="B55" s="2"/>
+    </row>
+    <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B50" s="2"/>
-    </row>
-    <row r="51" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="4"/>
-      <c r="B51" s="2"/>
-    </row>
-    <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B52" s="2"/>
-    </row>
-    <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="4"/>
       <c r="B56" s="2"/>
     </row>
     <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="4"/>
       <c r="B57" s="2"/>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="3" t="s">
+    <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="9"/>
+      <c r="B58" s="2"/>
+    </row>
+    <row r="62" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="4"/>
+      <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="4"/>
+      <c r="B63" s="2"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="3" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="3" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="3" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="3"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="3"/>
-    </row>
-    <row r="65" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A65" s="5" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="3"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="3"/>
+    </row>
+    <row r="71" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A71" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A66" s="5"/>
-    </row>
-    <row r="67" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="4" t="s">
+    <row r="72" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A72" s="5"/>
+    </row>
+    <row r="73" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B67" s="2"/>
-    </row>
-    <row r="68" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A68" s="5"/>
-    </row>
-    <row r="69" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B69" s="2"/>
-    </row>
-    <row r="70" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A70" s="5"/>
-    </row>
-    <row r="71" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A71" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B71" s="2"/>
-    </row>
-    <row r="72" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="4"/>
-      <c r="B72" s="2"/>
-    </row>
-    <row r="73" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>28</v>
-      </c>
       <c r="B73" s="2"/>
+    </row>
+    <row r="74" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A74" s="5"/>
     </row>
     <row r="75" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B75" s="2"/>
+    </row>
+    <row r="76" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A76" s="5"/>
+    </row>
+    <row r="77" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B77" s="2"/>
+    </row>
+    <row r="78" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="4"/>
+      <c r="B78" s="2"/>
+    </row>
+    <row r="79" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>28</v>
+      </c>
+      <c r="B79" s="2"/>
+    </row>
+    <row r="81" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B75" s="2"/>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+      <c r="B81" s="2"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
+    <row r="107" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
         <v>5</v>
       </c>
-      <c r="B101" s="2"/>
-    </row>
-    <row r="103" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
+      <c r="B107" s="2"/>
+    </row>
+    <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
         <v>6</v>
-      </c>
-      <c r="B103" s="2"/>
-    </row>
-    <row r="105" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A105" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B105" s="2"/>
-    </row>
-    <row r="106" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A106" s="4"/>
-      <c r="B106" s="2"/>
-    </row>
-    <row r="107" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A107" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B107" s="2"/>
-    </row>
-    <row r="108" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A108" s="4"/>
-      <c r="B108" s="2"/>
-    </row>
-    <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A109" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="B109" s="2"/>
     </row>
     <row r="111" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A111" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B111" s="2"/>
+    </row>
+    <row r="112" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A112" s="4"/>
+      <c r="B112" s="2"/>
+    </row>
+    <row r="113" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A113" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B113" s="2"/>
+    </row>
+    <row r="114" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A114" s="4"/>
+      <c r="B114" s="2"/>
+    </row>
+    <row r="115" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A115" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B115" s="2"/>
+    </row>
+    <row r="117" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A117" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B111" s="2"/>
-    </row>
-    <row r="112" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A112" s="1"/>
-      <c r="B112" s="2"/>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B113" s="6" t="s">
+      <c r="B117" s="2"/>
+    </row>
+    <row r="118" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A118" s="1"/>
+      <c r="B118" s="2"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B119" s="6" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A115" s="6"/>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116" s="6"/>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" s="6"/>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120" s="6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="6"/>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A122" s="6" t="s">
+      <c r="A122" s="6"/>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" s="6"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" s="6"/>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A123" s="1"/>
-      <c r="B123" s="2"/>
-    </row>
-    <row r="124" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A124" s="1"/>
-      <c r="B124" s="2"/>
-    </row>
-    <row r="125" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A125" s="1"/>
-      <c r="B125" s="2"/>
-    </row>
-    <row r="126" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A126" s="1"/>
-      <c r="B126" s="2"/>
-    </row>
-    <row r="127" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A127" s="1"/>
-      <c r="B127" s="2"/>
-    </row>
-    <row r="128" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A128" s="1"/>
-      <c r="B128" s="2"/>
+    <row r="129" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A129" s="1"/>
+      <c r="B129" s="2"/>
     </row>
     <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A130" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="A130" s="1"/>
       <c r="B130" s="2"/>
     </row>
+    <row r="131" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A131" s="1"/>
+      <c r="B131" s="2"/>
+    </row>
     <row r="132" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A132" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="A132" s="1"/>
       <c r="B132" s="2"/>
     </row>
+    <row r="133" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A133" s="1"/>
+      <c r="B133" s="2"/>
+    </row>
     <row r="134" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A134" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="A134" s="1"/>
       <c r="B134" s="2"/>
     </row>
     <row r="136" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A136" s="4" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B136" s="2"/>
     </row>
     <row r="138" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A138" s="9" t="s">
-        <v>45</v>
-      </c>
+      <c r="A138" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B138" s="2"/>
     </row>
     <row r="140" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A140" s="4" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="B140" s="2"/>
-    </row>
-    <row r="141" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A141" s="1"/>
-      <c r="B141" s="2"/>
     </row>
     <row r="142" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A142" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B142" s="2"/>
+    </row>
+    <row r="144" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A144" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A146" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B146" s="2"/>
+    </row>
+    <row r="147" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A147" s="1"/>
+      <c r="B147" s="2"/>
+    </row>
+    <row r="148" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A148" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B142" s="2"/>
-    </row>
-    <row r="144" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A144" s="4" t="s">
+      <c r="B148" s="2"/>
+    </row>
+    <row r="150" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A150" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B144" s="2"/>
+      <c r="B150" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adds validation,adds dao, adds table view
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="441" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0D8EEC6-825E-457E-8D5E-4402B4BD115E}"/>
+  <xr:revisionPtr revIDLastSave="442" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{771647AE-A922-41A0-BFEC-039A503D59E7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Stand</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>Class diagramm</t>
+  </si>
+  <si>
+    <t>Überlegen wenn Manager request bestätigt, dann gleich TimeStamp erstellen?!?!?</t>
   </si>
 </sst>
 </file>
@@ -786,7 +789,7 @@
   <dimension ref="A1:G150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -846,7 +849,9 @@
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updates docs, shows the requests,....
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="442" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{771647AE-A922-41A0-BFEC-039A503D59E7}"/>
+  <xr:revisionPtr revIDLastSave="448" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{291BAAFE-67BB-4A7B-842F-D59BD34AFC81}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Stand</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>Überlegen wenn Manager request bestätigt, dann gleich TimeStamp erstellen?!?!?</t>
+  </si>
+  <si>
+    <t>Für das Bestätigen der Urlaubsanträge von Seiten des Managers unbedingt wieder Table View hernehmen mit Buttons darin. Vlt. 1 Button pro column.</t>
   </si>
 </sst>
 </file>
@@ -305,13 +308,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>119</xdr:row>
+      <xdr:row>121</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>133</xdr:row>
+      <xdr:row>135</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -366,13 +369,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3295127</xdr:colOff>
-      <xdr:row>104</xdr:row>
+      <xdr:row>106</xdr:row>
       <xdr:rowOff>18740</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -410,13 +413,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1810160</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>193413</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -465,13 +468,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2599763</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>158071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4461042</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>79844</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -786,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G150"/>
+  <dimension ref="A1:G152"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -840,7 +843,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B9" s="2"/>
     </row>
@@ -849,8 +852,8 @@
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>48</v>
+      <c r="A11" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B11" s="2"/>
     </row>
@@ -858,30 +861,30 @@
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>45</v>
-      </c>
+    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
@@ -889,7 +892,7 @@
     </row>
     <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B21" s="2"/>
     </row>
@@ -897,41 +900,43 @@
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
     </row>
-    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
+    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="G28" t="s">
+      <c r="B30" s="2"/>
+      <c r="G30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-      <c r="B32" s="2"/>
     </row>
     <row r="33" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
@@ -985,23 +990,21 @@
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
     </row>
+    <row r="46" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="1"/>
+      <c r="B46" s="2"/>
+    </row>
     <row r="47" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B48" s="2"/>
-    </row>
     <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
     </row>
     <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B50" s="2"/>
     </row>
@@ -1011,7 +1014,7 @@
     </row>
     <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B52" s="2"/>
     </row>
@@ -1020,7 +1023,9 @@
       <c r="B53" s="2"/>
     </row>
     <row r="54" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="1"/>
+      <c r="A54" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="B54" s="2"/>
     </row>
     <row r="55" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1028,73 +1033,72 @@
       <c r="B55" s="2"/>
     </row>
     <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="1"/>
+      <c r="B56" s="2"/>
+    </row>
+    <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="1"/>
+      <c r="B57" s="2"/>
+    </row>
+    <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B56" s="2"/>
-    </row>
-    <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="4"/>
-      <c r="B57" s="2"/>
-    </row>
-    <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="9"/>
       <c r="B58" s="2"/>
     </row>
-    <row r="62" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="4"/>
-      <c r="B62" s="2"/>
-    </row>
-    <row r="63" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="4"/>
-      <c r="B63" s="2"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="3" t="s">
-        <v>2</v>
-      </c>
+    <row r="59" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="4"/>
+      <c r="B59" s="2"/>
+    </row>
+    <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="9"/>
+      <c r="B60" s="2"/>
+    </row>
+    <row r="64" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="4"/>
+      <c r="B64" s="2"/>
+    </row>
+    <row r="65" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="4"/>
+      <c r="B65" s="2"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="3"/>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="3"/>
-    </row>
-    <row r="71" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A71" s="5" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="3"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="3"/>
+    </row>
+    <row r="73" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A73" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A72" s="5"/>
-    </row>
-    <row r="73" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B73" s="2"/>
     </row>
     <row r="74" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A74" s="5"/>
     </row>
     <row r="75" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B75" s="2"/>
     </row>
@@ -1103,56 +1107,55 @@
     </row>
     <row r="77" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B77" s="2"/>
+    </row>
+    <row r="78" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A78" s="5"/>
+    </row>
+    <row r="79" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B77" s="2"/>
-    </row>
-    <row r="78" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="4"/>
-      <c r="B78" s="2"/>
-    </row>
-    <row r="79" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+      <c r="B79" s="2"/>
+    </row>
+    <row r="80" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="4"/>
+      <c r="B80" s="2"/>
+    </row>
+    <row r="81" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>28</v>
       </c>
-      <c r="B79" s="2"/>
-    </row>
-    <row r="81" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A81" s="4" t="s">
+      <c r="B81" s="2"/>
+    </row>
+    <row r="83" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B81" s="2"/>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+      <c r="B83" s="2"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>5</v>
-      </c>
-      <c r="B107" s="2"/>
     </row>
     <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
+        <v>5</v>
+      </c>
+      <c r="B109" s="2"/>
+    </row>
+    <row r="111" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
         <v>6</v>
       </c>
-      <c r="B109" s="2"/>
-    </row>
-    <row r="111" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A111" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="B111" s="2"/>
-    </row>
-    <row r="112" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A112" s="4"/>
-      <c r="B112" s="2"/>
     </row>
     <row r="113" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B113" s="2"/>
     </row>
@@ -1162,64 +1165,66 @@
     </row>
     <row r="115" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B115" s="2"/>
+    </row>
+    <row r="116" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A116" s="4"/>
+      <c r="B116" s="2"/>
     </row>
     <row r="117" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B117" s="2"/>
+    </row>
+    <row r="119" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A119" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B117" s="2"/>
-    </row>
-    <row r="118" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A118" s="1"/>
-      <c r="B118" s="2"/>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B119" s="6" t="s">
+      <c r="B119" s="2"/>
+    </row>
+    <row r="120" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A120" s="1"/>
+      <c r="B120" s="2"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B121" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" s="6"/>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A122" s="6"/>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="6"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="A124" s="6"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A125" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A125" s="6"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A127" s="6"/>
+      <c r="A127" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" s="6"/>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A129" s="1"/>
-      <c r="B129" s="2"/>
-    </row>
-    <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A130" s="1"/>
-      <c r="B130" s="2"/>
     </row>
     <row r="131" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A131" s="1"/>
@@ -1237,56 +1242,64 @@
       <c r="A134" s="1"/>
       <c r="B134" s="2"/>
     </row>
+    <row r="135" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A135" s="1"/>
+      <c r="B135" s="2"/>
+    </row>
     <row r="136" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A136" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="A136" s="1"/>
       <c r="B136" s="2"/>
     </row>
     <row r="138" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A138" s="4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B138" s="2"/>
     </row>
     <row r="140" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A140" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B140" s="2"/>
     </row>
     <row r="142" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A142" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B142" s="2"/>
+    </row>
+    <row r="144" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A144" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B142" s="2"/>
-    </row>
-    <row r="144" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A144" s="9" t="s">
+      <c r="B144" s="2"/>
+    </row>
+    <row r="146" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A146" s="9" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A146" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B146" s="2"/>
-    </row>
-    <row r="147" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A147" s="1"/>
-      <c r="B147" s="2"/>
     </row>
     <row r="148" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A148" s="4" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B148" s="2"/>
+    </row>
+    <row r="149" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A149" s="1"/>
+      <c r="B149" s="2"/>
     </row>
     <row r="150" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A150" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B150" s="2"/>
+    </row>
+    <row r="152" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A152" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B150" s="2"/>
+      <c r="B152" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
starts setting up pending requests view for managers
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="448" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{291BAAFE-67BB-4A7B-842F-D59BD34AFC81}"/>
+  <xr:revisionPtr revIDLastSave="458" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6E2E75A-B277-4085-AAD5-853DFB04953C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Stand</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>Für das Bestätigen der Urlaubsanträge von Seiten des Managers unbedingt wieder Table View hernehmen mit Buttons darin. Vlt. 1 Button pro column.</t>
+  </si>
+  <si>
+    <t>Vacation request validieren dass es nicht 2 im gleichen Zeitraum gibt.</t>
+  </si>
+  <si>
+    <t>Manager AUTO Buchung Vacation erstellen.</t>
   </si>
 </sst>
 </file>
@@ -308,13 +314,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>121</xdr:row>
+      <xdr:row>125</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>135</xdr:row>
+      <xdr:row>139</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -369,13 +375,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3295127</xdr:colOff>
-      <xdr:row>106</xdr:row>
+      <xdr:row>110</xdr:row>
       <xdr:rowOff>18740</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -413,13 +419,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1810160</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>193413</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -468,13 +474,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2599763</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>158071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4461042</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>79844</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -789,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G152"/>
+  <dimension ref="A1:G156"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -862,169 +868,169 @@
       <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
+      <c r="A14" s="4"/>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
     </row>
-    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="G30" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
+    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
+      <c r="G34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
-      <c r="B36" s="2"/>
-    </row>
-    <row r="37" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
     </row>
-    <row r="38" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
+    </row>
+    <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
+      <c r="B48" s="2"/>
     </row>
     <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
     </row>
     <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="A50" s="1"/>
       <c r="B50" s="2"/>
     </row>
     <row r="51" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
     </row>
-    <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B52" s="2"/>
-    </row>
     <row r="53" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
     </row>
     <row r="54" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B54" s="2"/>
     </row>
@@ -1033,7 +1039,9 @@
       <c r="B55" s="2"/>
     </row>
     <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="1"/>
+      <c r="A56" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="B56" s="2"/>
     </row>
     <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1042,205 +1050,207 @@
     </row>
     <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B58" s="2"/>
+    </row>
+    <row r="59" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="1"/>
+      <c r="B59" s="2"/>
+    </row>
+    <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="1"/>
+      <c r="B60" s="2"/>
+    </row>
+    <row r="61" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="1"/>
+      <c r="B61" s="2"/>
+    </row>
+    <row r="62" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B58" s="2"/>
-    </row>
-    <row r="59" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="4"/>
-      <c r="B59" s="2"/>
-    </row>
-    <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="9"/>
-      <c r="B60" s="2"/>
+      <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="4"/>
+      <c r="B63" s="2"/>
     </row>
     <row r="64" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="4"/>
+      <c r="A64" s="9"/>
       <c r="B64" s="2"/>
     </row>
-    <row r="65" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="4"/>
-      <c r="B65" s="2"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
+    <row r="68" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="4"/>
+      <c r="B68" s="2"/>
+    </row>
+    <row r="69" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="4"/>
+      <c r="B69" s="2"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="3" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="3" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="3"/>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="3"/>
-    </row>
-    <row r="73" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A73" s="5" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="3"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="3"/>
+    </row>
+    <row r="77" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A77" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A74" s="5"/>
-    </row>
-    <row r="75" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B75" s="2"/>
-    </row>
-    <row r="76" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A76" s="5"/>
-    </row>
-    <row r="77" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B77" s="2"/>
     </row>
     <row r="78" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A78" s="5"/>
     </row>
     <row r="79" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B79" s="2"/>
     </row>
-    <row r="80" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A80" s="4"/>
-      <c r="B80" s="2"/>
+    <row r="80" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A80" s="5"/>
     </row>
     <row r="81" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>28</v>
+      <c r="A81" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="B81" s="2"/>
+    </row>
+    <row r="82" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A82" s="5"/>
     </row>
     <row r="83" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B83" s="2"/>
+    </row>
+    <row r="84" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="4"/>
+      <c r="B84" s="2"/>
+    </row>
+    <row r="85" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>28</v>
+      </c>
+      <c r="B85" s="2"/>
+    </row>
+    <row r="87" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A87" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B83" s="2"/>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+      <c r="B87" s="2"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
+    <row r="113" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
         <v>5</v>
       </c>
-      <c r="B109" s="2"/>
-    </row>
-    <row r="111" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
+      <c r="B113" s="2"/>
+    </row>
+    <row r="115" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
         <v>6</v>
       </c>
-      <c r="B111" s="2"/>
-    </row>
-    <row r="113" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A113" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B113" s="2"/>
-    </row>
-    <row r="114" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A114" s="4"/>
-      <c r="B114" s="2"/>
-    </row>
-    <row r="115" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A115" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="B115" s="2"/>
-    </row>
-    <row r="116" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A116" s="4"/>
-      <c r="B116" s="2"/>
     </row>
     <row r="117" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B117" s="2"/>
+    </row>
+    <row r="118" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A118" s="4"/>
+      <c r="B118" s="2"/>
     </row>
     <row r="119" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A119" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B119" s="2"/>
+    </row>
+    <row r="120" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A120" s="4"/>
+      <c r="B120" s="2"/>
+    </row>
+    <row r="121" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A121" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B121" s="2"/>
+    </row>
+    <row r="123" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A123" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B119" s="2"/>
-    </row>
-    <row r="120" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A120" s="1"/>
-      <c r="B120" s="2"/>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B121" s="6" t="s">
+      <c r="B123" s="2"/>
+    </row>
+    <row r="124" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A124" s="1"/>
+      <c r="B124" s="2"/>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B125" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A123" s="6"/>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" s="6"/>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A125" s="6"/>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A126" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A127" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A127" s="6"/>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A128" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="A128" s="6"/>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="6"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" s="6"/>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A131" s="1"/>
-      <c r="B131" s="2"/>
-    </row>
-    <row r="132" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A132" s="1"/>
-      <c r="B132" s="2"/>
-    </row>
-    <row r="133" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A133" s="1"/>
-      <c r="B133" s="2"/>
-    </row>
-    <row r="134" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A134" s="1"/>
-      <c r="B134" s="2"/>
     </row>
     <row r="135" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A135" s="1"/>
@@ -1250,56 +1260,72 @@
       <c r="A136" s="1"/>
       <c r="B136" s="2"/>
     </row>
+    <row r="137" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A137" s="1"/>
+      <c r="B137" s="2"/>
+    </row>
     <row r="138" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A138" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="A138" s="1"/>
       <c r="B138" s="2"/>
     </row>
+    <row r="139" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A139" s="1"/>
+      <c r="B139" s="2"/>
+    </row>
     <row r="140" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A140" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="A140" s="1"/>
       <c r="B140" s="2"/>
     </row>
     <row r="142" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A142" s="4" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B142" s="2"/>
     </row>
     <row r="144" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A144" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B144" s="2"/>
     </row>
     <row r="146" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A146" s="9" t="s">
-        <v>44</v>
-      </c>
+      <c r="A146" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B146" s="2"/>
     </row>
     <row r="148" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A148" s="4" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B148" s="2"/>
     </row>
-    <row r="149" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A149" s="1"/>
-      <c r="B149" s="2"/>
-    </row>
     <row r="150" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A150" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B150" s="2"/>
+      <c r="A150" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="152" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A152" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B152" s="2"/>
+    </row>
+    <row r="153" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A153" s="1"/>
+      <c r="B153" s="2"/>
+    </row>
+    <row r="154" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A154" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B154" s="2"/>
+    </row>
+    <row r="156" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A156" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B152" s="2"/>
+      <c r="B156" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adds updating of old requests, comments
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="462" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3119390C-6AC2-4591-9DC7-10159FCE0B41}"/>
+  <xr:revisionPtr revIDLastSave="486" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B805834-C50A-44BA-A320-DC4574492BAE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Stand</t>
   </si>
@@ -205,6 +205,15 @@
   </si>
   <si>
     <t>Manager AUTO Buchung Vacation erstellen.</t>
+  </si>
+  <si>
+    <t>In initialization von requests und vactions status von alten requests auf expired setzen</t>
+  </si>
+  <si>
+    <t>Vacation Controller fertig machen</t>
+  </si>
+  <si>
+    <t>Requirements Paper durchgehen was erledigt was nicht.</t>
   </si>
 </sst>
 </file>
@@ -276,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -291,6 +300,7 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -314,13 +324,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>127</xdr:row>
+      <xdr:row>131</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>141</xdr:row>
+      <xdr:row>145</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -375,14 +385,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
-      <xdr:row>92</xdr:row>
+      <xdr:row>96</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3295127</xdr:colOff>
-      <xdr:row>112</xdr:row>
-      <xdr:rowOff>18740</xdr:rowOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>18741</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -419,13 +429,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1810160</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>193412</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -474,13 +484,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2599763</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>158071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4461042</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>79844</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -795,10 +805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G158"/>
+  <dimension ref="A1:G162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A13" sqref="A12:A13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -821,7 +831,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="B3" s="2"/>
     </row>
@@ -830,26 +840,26 @@
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="A5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="2"/>
+      <c r="A7" s="9" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B9" s="2"/>
     </row>
@@ -857,47 +867,49 @@
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="2"/>
+        <v>54</v>
+      </c>
+      <c r="B11" s="9"/>
     </row>
     <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="B13" s="9"/>
     </row>
     <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
+      <c r="A14" s="1"/>
       <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
+      <c r="A15" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
+      <c r="A16" s="1"/>
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
+      <c r="A18" s="4"/>
       <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" s="2"/>
     </row>
@@ -905,30 +917,30 @@
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>45</v>
-      </c>
+    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
@@ -936,7 +948,7 @@
     </row>
     <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B29" s="2"/>
     </row>
@@ -944,41 +956,43 @@
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
     </row>
-    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
-      <c r="B35" s="2"/>
+    <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="2"/>
     </row>
     <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="1"/>
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="G36" t="s">
+      <c r="B38" s="2"/>
+      <c r="G38" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
+    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="8" t="s">
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="1"/>
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
-      <c r="B40" s="2"/>
     </row>
     <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
@@ -1032,23 +1046,21 @@
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
     </row>
+    <row r="54" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="1"/>
+      <c r="B54" s="2"/>
+    </row>
     <row r="55" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
     </row>
-    <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B56" s="2"/>
-    </row>
     <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
     </row>
     <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B58" s="2"/>
     </row>
@@ -1058,7 +1070,7 @@
     </row>
     <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B60" s="2"/>
     </row>
@@ -1067,7 +1079,9 @@
       <c r="B61" s="2"/>
     </row>
     <row r="62" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="1"/>
+      <c r="A62" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="B62" s="2"/>
     </row>
     <row r="63" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1075,206 +1089,206 @@
       <c r="B63" s="2"/>
     </row>
     <row r="64" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="1"/>
+      <c r="B64" s="2"/>
+    </row>
+    <row r="65" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="1"/>
+      <c r="B65" s="2"/>
+    </row>
+    <row r="66" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B64" s="2"/>
-    </row>
-    <row r="65" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="4"/>
-      <c r="B65" s="2"/>
-    </row>
-    <row r="66" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="9"/>
       <c r="B66" s="2"/>
     </row>
-    <row r="70" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="4"/>
-      <c r="B70" s="2"/>
-    </row>
-    <row r="71" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A71" s="4"/>
-      <c r="B71" s="2"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="3" t="s">
-        <v>2</v>
-      </c>
+    <row r="67" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="4"/>
+      <c r="B67" s="2"/>
+    </row>
+    <row r="68" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="9"/>
+      <c r="B68" s="2"/>
+    </row>
+    <row r="72" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="4"/>
+      <c r="B72" s="2"/>
+    </row>
+    <row r="73" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="4"/>
+      <c r="B73" s="2"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="3"/>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="3"/>
-    </row>
-    <row r="79" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A79" s="5" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="3"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="3"/>
+    </row>
+    <row r="81" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A81" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A80" s="5"/>
-    </row>
-    <row r="81" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A81" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B81" s="2"/>
     </row>
     <row r="82" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A82" s="5"/>
     </row>
     <row r="83" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B83" s="2"/>
-    </row>
-    <row r="84" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A84" s="5"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="4"/>
     </row>
     <row r="85" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B85" s="2"/>
     </row>
-    <row r="86" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="4"/>
-      <c r="B86" s="2"/>
+    <row r="86" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A86" s="5"/>
     </row>
     <row r="87" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>28</v>
+      <c r="A87" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="B87" s="2"/>
+    </row>
+    <row r="88" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A88" s="5"/>
     </row>
     <row r="89" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B89" s="2"/>
+    </row>
+    <row r="90" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A90" s="4"/>
+      <c r="B90" s="2"/>
+    </row>
+    <row r="91" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>28</v>
+      </c>
+      <c r="B91" s="2"/>
+    </row>
+    <row r="93" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A93" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B89" s="2"/>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
+      <c r="B93" s="2"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
+    <row r="119" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
         <v>5</v>
       </c>
-      <c r="B115" s="2"/>
-    </row>
-    <row r="117" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
+      <c r="B119" s="2"/>
+    </row>
+    <row r="121" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
         <v>6</v>
       </c>
-      <c r="B117" s="2"/>
-    </row>
-    <row r="119" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A119" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B119" s="2"/>
-    </row>
-    <row r="120" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A120" s="4"/>
-      <c r="B120" s="2"/>
-    </row>
-    <row r="121" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A121" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="B121" s="2"/>
-    </row>
-    <row r="122" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A122" s="4"/>
-      <c r="B122" s="2"/>
     </row>
     <row r="123" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A123" s="4" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B123" s="2"/>
+    </row>
+    <row r="124" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A124" s="4"/>
+      <c r="B124" s="2"/>
     </row>
     <row r="125" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A125" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B125" s="2"/>
+    </row>
+    <row r="126" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A126" s="4"/>
+      <c r="B126" s="2"/>
+    </row>
+    <row r="127" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A127" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B127" s="2"/>
+    </row>
+    <row r="129" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A129" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B125" s="2"/>
-    </row>
-    <row r="126" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A126" s="1"/>
-      <c r="B126" s="2"/>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B127" s="6" t="s">
+      <c r="B129" s="2"/>
+    </row>
+    <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A130" s="1"/>
+      <c r="B130" s="2"/>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B131" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A129" s="6"/>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A130" s="6"/>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A131" s="6"/>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A133" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A133" s="6"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A134" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="A134" s="6"/>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="6"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" s="6"/>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A137" s="1"/>
-      <c r="B137" s="2"/>
-    </row>
-    <row r="138" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A138" s="1"/>
-      <c r="B138" s="2"/>
-    </row>
-    <row r="139" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A139" s="1"/>
-      <c r="B139" s="2"/>
-    </row>
-    <row r="140" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A140" s="1"/>
-      <c r="B140" s="2"/>
     </row>
     <row r="141" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A141" s="1"/>
@@ -1284,56 +1298,72 @@
       <c r="A142" s="1"/>
       <c r="B142" s="2"/>
     </row>
+    <row r="143" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A143" s="1"/>
+      <c r="B143" s="2"/>
+    </row>
     <row r="144" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A144" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="A144" s="1"/>
       <c r="B144" s="2"/>
     </row>
+    <row r="145" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A145" s="1"/>
+      <c r="B145" s="2"/>
+    </row>
     <row r="146" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A146" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="A146" s="1"/>
       <c r="B146" s="2"/>
     </row>
     <row r="148" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A148" s="4" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B148" s="2"/>
     </row>
     <row r="150" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A150" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B150" s="2"/>
     </row>
     <row r="152" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A152" s="9" t="s">
-        <v>44</v>
-      </c>
+      <c r="A152" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B152" s="2"/>
     </row>
     <row r="154" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A154" s="4" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B154" s="2"/>
     </row>
-    <row r="155" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A155" s="1"/>
-      <c r="B155" s="2"/>
-    </row>
     <row r="156" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A156" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B156" s="2"/>
+      <c r="A156" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="158" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A158" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B158" s="2"/>
+    </row>
+    <row r="159" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A159" s="1"/>
+      <c r="B159" s="2"/>
+    </row>
+    <row r="160" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A160" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B160" s="2"/>
+    </row>
+    <row r="162" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A162" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B158" s="2"/>
+      <c r="B162" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adds comments,adds this, updates docu
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="486" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B805834-C50A-44BA-A320-DC4574492BAE}"/>
+  <xr:revisionPtr revIDLastSave="553" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD4E31B1-8E37-46CC-97FB-018F0060ABF5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
-  <si>
-    <t>Stand</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>…..</t>
   </si>
@@ -215,12 +212,41 @@
   <si>
     <t>Requirements Paper durchgehen was erledigt was nicht.</t>
   </si>
+  <si>
+    <t xml:space="preserve">Gegen Ende: </t>
+  </si>
+  <si>
+    <t>QA&lt;QA&lt;QA&lt;QA&lt;QA&lt;QA&lt;QA&lt;QA&lt;QA&lt;QA&lt;QA&lt;QA&lt;</t>
+  </si>
+  <si>
+    <t>ExecutorService mit einem Singelton Provider Pattern der ganzen App zur Verfügung stellen und in der zentralen Stopp Methode beim Shutdown schließen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statt dem FetchType Eager Loading - folgendes machen: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wenn ich diese Lazy Loading Exception habe wenn ich zum Beispiel die Entity verwende, dann muss ich diese Stelle in ein Try catch und dann folgendes machen: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ZUSÄTZLICH: 
+ANSTATT FETCH-TYPE EAGER WENN ICH DEN TYP VERWENDE PRPÜFEN OB HIBERNATE CONNECTION NOCH BESTEHT UND WENN NICHT, SIE MANUELL AUFBAUEN UND MACHE EIN GET ROLLEN:
+1.	Verbindung aufbauen
+2.	Get Rolllen
+3.	Und dann kann ich aus dem catch raus und weitermachen.</t>
+  </si>
+  <si>
+    <t>Wenn Zeit: ----------------------------------------------------------------</t>
+  </si>
+  <si>
+    <t>-------------------------------------------------------------------------------------------------------------------------</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +290,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -285,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -300,7 +334,11 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -324,13 +362,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>131</xdr:row>
+      <xdr:row>140</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>145</xdr:row>
+      <xdr:row>154</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -385,13 +423,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>105</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3295127</xdr:colOff>
-      <xdr:row>116</xdr:row>
+      <xdr:row>125</xdr:row>
       <xdr:rowOff>18741</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -429,13 +467,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1810160</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>193412</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -484,13 +522,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2599763</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>158071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4461042</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>79844</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -805,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G162"/>
+  <dimension ref="A1:G171"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,31 +856,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2">
-        <v>45836</v>
-      </c>
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
+      <c r="A2" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>52</v>
-      </c>
+      <c r="A3" s="1"/>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+      <c r="A4" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>39</v>
-      </c>
+      <c r="A5" s="4"/>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -850,16 +884,18 @@
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="A7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>37</v>
+      <c r="A9" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="B9" s="2"/>
     </row>
@@ -867,155 +903,160 @@
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="9"/>
-    </row>
-    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="9"/>
+    <row r="13" spans="1:2" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>40</v>
-      </c>
+      <c r="A15" s="1"/>
       <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
+      <c r="A16" s="11" t="s">
+        <v>61</v>
+      </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>48</v>
-      </c>
+      <c r="A17" s="1"/>
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="2"/>
+      <c r="A18" s="9" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="9"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="9"/>
+    </row>
+    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
-    </row>
-    <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-      <c r="B32" s="2"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
-      <c r="B36" s="2"/>
-    </row>
-    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
-      <c r="B37" s="2"/>
     </row>
     <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B38" s="2"/>
-      <c r="G38" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="A39" s="1"/>
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="8" t="s">
-        <v>22</v>
-      </c>
+    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="2"/>
     </row>
     <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="1"/>
-      <c r="B42" s="2"/>
-    </row>
-    <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="1"/>
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="1"/>
-      <c r="B44" s="2"/>
-    </row>
-    <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="1"/>
-      <c r="B45" s="2"/>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="10"/>
     </row>
     <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="1"/>
+      <c r="A46" t="s">
+        <v>46</v>
+      </c>
       <c r="B46" s="2"/>
     </row>
     <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1023,16 +1064,24 @@
       <c r="B47" s="2"/>
     </row>
     <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="1"/>
+      <c r="A48" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="B48" s="2"/>
+      <c r="G48" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="1"/>
+      <c r="A49" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="B49" s="2"/>
     </row>
-    <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="1"/>
-      <c r="B50" s="2"/>
+    <row r="50" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="8" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="51" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
@@ -1054,14 +1103,16 @@
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
     </row>
+    <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="1"/>
+      <c r="B56" s="2"/>
+    </row>
     <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
     </row>
     <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="A58" s="1"/>
       <c r="B58" s="2"/>
     </row>
     <row r="59" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1069,9 +1120,7 @@
       <c r="B59" s="2"/>
     </row>
     <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="s">
-        <v>30</v>
-      </c>
+      <c r="A60" s="1"/>
       <c r="B60" s="2"/>
     </row>
     <row r="61" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1079,9 +1128,7 @@
       <c r="B61" s="2"/>
     </row>
     <row r="62" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="A62" s="1"/>
       <c r="B62" s="2"/>
     </row>
     <row r="63" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1098,272 +1145,313 @@
     </row>
     <row r="66" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B66" s="2"/>
     </row>
     <row r="67" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="4"/>
+      <c r="A67" s="1"/>
       <c r="B67" s="2"/>
     </row>
     <row r="68" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A68" s="9"/>
+      <c r="A68" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="B68" s="2"/>
     </row>
+    <row r="69" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="1"/>
+      <c r="B69" s="2"/>
+    </row>
+    <row r="70" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B70" s="2"/>
+    </row>
+    <row r="71" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A71" s="4"/>
+      <c r="B71" s="2"/>
+    </row>
     <row r="72" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="4"/>
+      <c r="A72" s="9"/>
       <c r="B72" s="2"/>
     </row>
-    <row r="73" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="4"/>
-      <c r="B73" s="2"/>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="3" t="s">
+    <row r="76" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="4"/>
+      <c r="B76" s="2"/>
+    </row>
+    <row r="77" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="4"/>
+      <c r="B77" s="2"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="3" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="3" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="3"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="3"/>
-    </row>
-    <row r="81" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A81" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A82" s="5"/>
-    </row>
-    <row r="83" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A84" s="4"/>
-    </row>
-    <row r="85" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A85" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B85" s="2"/>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" s="3"/>
+    </row>
+    <row r="85" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A85" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="86" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A86" s="5"/>
     </row>
-    <row r="87" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A87" s="4" t="s">
+    <row r="87" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A87" s="5"/>
+    </row>
+    <row r="88" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A89" s="5"/>
+    </row>
+    <row r="90" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A90" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A91" s="5"/>
+    </row>
+    <row r="92" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A92" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A93" s="4"/>
+    </row>
+    <row r="94" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A94" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B94" s="2"/>
+    </row>
+    <row r="95" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A95" s="5"/>
+    </row>
+    <row r="96" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A96" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B96" s="2"/>
+    </row>
+    <row r="97" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A97" s="5"/>
+    </row>
+    <row r="98" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A98" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B98" s="2"/>
+    </row>
+    <row r="99" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A99" s="4"/>
+      <c r="B99" s="2"/>
+    </row>
+    <row r="100" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>27</v>
+      </c>
+      <c r="B100" s="2"/>
+    </row>
+    <row r="102" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A102" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B102" s="2"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
         <v>31</v>
       </c>
-      <c r="B87" s="2"/>
-    </row>
-    <row r="88" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A88" s="5"/>
-    </row>
-    <row r="89" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A89" s="4" t="s">
+    </row>
+    <row r="128" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>4</v>
+      </c>
+      <c r="B128" s="2"/>
+    </row>
+    <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>5</v>
+      </c>
+      <c r="B130" s="2"/>
+    </row>
+    <row r="132" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A132" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B132" s="2"/>
+    </row>
+    <row r="133" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A133" s="4"/>
+      <c r="B133" s="2"/>
+    </row>
+    <row r="134" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A134" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B134" s="2"/>
+    </row>
+    <row r="135" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A135" s="4"/>
+      <c r="B135" s="2"/>
+    </row>
+    <row r="136" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A136" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B136" s="2"/>
+    </row>
+    <row r="138" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A138" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B138" s="2"/>
+    </row>
+    <row r="139" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A139" s="1"/>
+      <c r="B139" s="2"/>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B140" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" s="6"/>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" s="6"/>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" s="6"/>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148" s="6"/>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A150" s="1"/>
+      <c r="B150" s="2"/>
+    </row>
+    <row r="151" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A151" s="1"/>
+      <c r="B151" s="2"/>
+    </row>
+    <row r="152" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A152" s="1"/>
+      <c r="B152" s="2"/>
+    </row>
+    <row r="153" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A153" s="1"/>
+      <c r="B153" s="2"/>
+    </row>
+    <row r="154" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A154" s="1"/>
+      <c r="B154" s="2"/>
+    </row>
+    <row r="155" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A155" s="1"/>
+      <c r="B155" s="2"/>
+    </row>
+    <row r="157" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A157" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B157" s="2"/>
+    </row>
+    <row r="159" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A159" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B159" s="2"/>
+    </row>
+    <row r="161" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A161" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B161" s="2"/>
+    </row>
+    <row r="163" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A163" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B163" s="2"/>
+    </row>
+    <row r="165" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A165" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A167" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B167" s="2"/>
+    </row>
+    <row r="168" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A168" s="1"/>
+      <c r="B168" s="2"/>
+    </row>
+    <row r="169" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A169" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B169" s="2"/>
+    </row>
+    <row r="171" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A171" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B89" s="2"/>
-    </row>
-    <row r="90" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A90" s="4"/>
-      <c r="B90" s="2"/>
-    </row>
-    <row r="91" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>28</v>
-      </c>
-      <c r="B91" s="2"/>
-    </row>
-    <row r="93" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A93" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B93" s="2"/>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
-        <v>5</v>
-      </c>
-      <c r="B119" s="2"/>
-    </row>
-    <row r="121" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
-        <v>6</v>
-      </c>
-      <c r="B121" s="2"/>
-    </row>
-    <row r="123" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A123" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B123" s="2"/>
-    </row>
-    <row r="124" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A124" s="4"/>
-      <c r="B124" s="2"/>
-    </row>
-    <row r="125" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A125" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B125" s="2"/>
-    </row>
-    <row r="126" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A126" s="4"/>
-      <c r="B126" s="2"/>
-    </row>
-    <row r="127" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A127" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B127" s="2"/>
-    </row>
-    <row r="129" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A129" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B129" s="2"/>
-    </row>
-    <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A130" s="1"/>
-      <c r="B130" s="2"/>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B131" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A133" s="6"/>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A134" s="6"/>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A135" s="6"/>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A136" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A137" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A138" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A139" s="6"/>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A140" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A141" s="1"/>
-      <c r="B141" s="2"/>
-    </row>
-    <row r="142" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A142" s="1"/>
-      <c r="B142" s="2"/>
-    </row>
-    <row r="143" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A143" s="1"/>
-      <c r="B143" s="2"/>
-    </row>
-    <row r="144" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A144" s="1"/>
-      <c r="B144" s="2"/>
-    </row>
-    <row r="145" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A145" s="1"/>
-      <c r="B145" s="2"/>
-    </row>
-    <row r="146" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A146" s="1"/>
-      <c r="B146" s="2"/>
-    </row>
-    <row r="148" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A148" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B148" s="2"/>
-    </row>
-    <row r="150" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A150" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B150" s="2"/>
-    </row>
-    <row r="152" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A152" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B152" s="2"/>
-    </row>
-    <row r="154" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A154" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B154" s="2"/>
-    </row>
-    <row r="156" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A156" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A158" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B158" s="2"/>
-    </row>
-    <row r="159" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A159" s="1"/>
-      <c r="B159" s="2"/>
-    </row>
-    <row r="160" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A160" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B160" s="2"/>
-    </row>
-    <row r="162" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A162" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B162" s="2"/>
+      <c r="B171" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adds validation for request with same start time
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="553" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD4E31B1-8E37-46CC-97FB-018F0060ABF5}"/>
+  <xr:revisionPtr revIDLastSave="611" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAC967CE-2DEE-470E-831B-68C067F19BC7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>…..</t>
   </si>
@@ -207,16 +207,10 @@
     <t>In initialization von requests und vactions status von alten requests auf expired setzen</t>
   </si>
   <si>
-    <t>Vacation Controller fertig machen</t>
-  </si>
-  <si>
     <t>Requirements Paper durchgehen was erledigt was nicht.</t>
   </si>
   <si>
     <t xml:space="preserve">Gegen Ende: </t>
-  </si>
-  <si>
-    <t>QA&lt;QA&lt;QA&lt;QA&lt;QA&lt;QA&lt;QA&lt;QA&lt;QA&lt;QA&lt;QA&lt;QA&lt;</t>
   </si>
   <si>
     <t>ExecutorService mit einem Singelton Provider Pattern der ganzen App zur Verfügung stellen und in der zentralen Stopp Methode beim Shutdown schließen</t>
@@ -240,6 +234,18 @@
   </si>
   <si>
     <t>-------------------------------------------------------------------------------------------------------------------------</t>
+  </si>
+  <si>
+    <t>Validieren, dass wenn er die Vacation requests aus der Vergangenheit bereits accepted sind er diese nicht auf experied setzt.</t>
+  </si>
+  <si>
+    <t>Manager vacation - deny</t>
+  </si>
+  <si>
+    <t>Vacation Controller fertig machen - Deny button</t>
+  </si>
+  <si>
+    <t>_____________________</t>
   </si>
 </sst>
 </file>
@@ -362,13 +368,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>140</xdr:row>
+      <xdr:row>174</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>154</xdr:row>
+      <xdr:row>188</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -423,13 +429,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
-      <xdr:row>105</xdr:row>
+      <xdr:row>139</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3295127</xdr:colOff>
-      <xdr:row>125</xdr:row>
+      <xdr:row>159</xdr:row>
       <xdr:rowOff>18741</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -467,13 +473,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1810160</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>193412</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -522,13 +528,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2599763</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>158071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4461042</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>79844</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -843,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G171"/>
+  <dimension ref="A1:G205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -871,7 +877,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" s="2"/>
     </row>
@@ -885,7 +891,7 @@
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B7" s="2"/>
     </row>
@@ -895,7 +901,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B9" s="2"/>
     </row>
@@ -905,7 +911,7 @@
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B11" s="2"/>
     </row>
@@ -915,7 +921,7 @@
     </row>
     <row r="13" spans="1:2" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B13" s="2"/>
     </row>
@@ -929,7 +935,7 @@
     </row>
     <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B16" s="2"/>
     </row>
@@ -957,7 +963,7 @@
     </row>
     <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B22" s="9"/>
     </row>
@@ -966,38 +972,31 @@
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="9"/>
+      <c r="A24" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
       <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
+      <c r="A29" s="1"/>
       <c r="B29" s="2"/>
     </row>
     <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>49</v>
+      <c r="A30" t="s">
+        <v>44</v>
       </c>
       <c r="B30" s="2"/>
     </row>
@@ -1007,116 +1006,107 @@
     </row>
     <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B32" s="2"/>
     </row>
-    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
-        <v>37</v>
+    <row r="40" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="10"/>
-    </row>
-    <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>46</v>
-      </c>
+    <row r="42" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="2"/>
+    </row>
+    <row r="43" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="2"/>
+    </row>
+    <row r="46" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="1"/>
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="1"/>
+    <row r="47" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
-        <v>20</v>
-      </c>
+    <row r="48" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
       <c r="B48" s="2"/>
-      <c r="G48" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="B49" s="2"/>
     </row>
-    <row r="50" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="1"/>
-      <c r="B51" s="2"/>
+    <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="4"/>
+      <c r="B50" s="2"/>
     </row>
     <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
     </row>
-    <row r="53" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="1"/>
-      <c r="B53" s="2"/>
-    </row>
     <row r="54" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
     </row>
-    <row r="55" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="1"/>
-      <c r="B55" s="2"/>
-    </row>
-    <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="1"/>
-      <c r="B56" s="2"/>
-    </row>
-    <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="1"/>
-      <c r="B57" s="2"/>
-    </row>
-    <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="1"/>
-      <c r="B58" s="2"/>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="59" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="1"/>
+      <c r="A59" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="B59" s="2"/>
     </row>
     <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1124,190 +1114,280 @@
       <c r="B60" s="2"/>
     </row>
     <row r="61" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="1"/>
+      <c r="A61" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="B61" s="2"/>
     </row>
     <row r="62" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
     </row>
-    <row r="63" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="1"/>
-      <c r="B63" s="2"/>
-    </row>
-    <row r="64" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="1"/>
-      <c r="B64" s="2"/>
-    </row>
-    <row r="65" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="1"/>
-      <c r="B65" s="2"/>
-    </row>
-    <row r="66" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="4" t="s">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" s="10"/>
+    </row>
+    <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>46</v>
+      </c>
+      <c r="B67" s="2"/>
+    </row>
+    <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="1"/>
+      <c r="B68" s="2"/>
+    </row>
+    <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B69" s="2"/>
+      <c r="G69" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B70" s="2"/>
+    </row>
+    <row r="71" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="1"/>
+      <c r="B72" s="2"/>
+    </row>
+    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="1"/>
+      <c r="B73" s="2"/>
+    </row>
+    <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="1"/>
+      <c r="B74" s="2"/>
+    </row>
+    <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="1"/>
+      <c r="B75" s="2"/>
+    </row>
+    <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="1"/>
+      <c r="B76" s="2"/>
+    </row>
+    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="1"/>
+      <c r="B77" s="2"/>
+    </row>
+    <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="1"/>
+      <c r="B78" s="2"/>
+    </row>
+    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="1"/>
+      <c r="B79" s="2"/>
+    </row>
+    <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="1"/>
+      <c r="B80" s="2"/>
+    </row>
+    <row r="81" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="1"/>
+      <c r="B81" s="2"/>
+    </row>
+    <row r="82" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="1"/>
+      <c r="B82" s="2"/>
+    </row>
+    <row r="83" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="1"/>
+      <c r="B83" s="2"/>
+    </row>
+    <row r="84" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="1"/>
+      <c r="B84" s="2"/>
+    </row>
+    <row r="85" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="1"/>
+      <c r="B85" s="2"/>
+    </row>
+    <row r="86" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A86" s="1"/>
+      <c r="B86" s="2"/>
+    </row>
+    <row r="87" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A87" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B66" s="2"/>
-    </row>
-    <row r="67" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="1"/>
-      <c r="B67" s="2"/>
-    </row>
-    <row r="68" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A68" s="4" t="s">
+      <c r="B87" s="2"/>
+    </row>
+    <row r="88" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="1"/>
+      <c r="B88" s="2"/>
+    </row>
+    <row r="89" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A89" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B68" s="2"/>
-    </row>
-    <row r="69" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="1"/>
-      <c r="B69" s="2"/>
-    </row>
-    <row r="70" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="4" t="s">
+      <c r="B89" s="2"/>
+    </row>
+    <row r="90" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A90" s="1"/>
+      <c r="B90" s="2"/>
+    </row>
+    <row r="91" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A91" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B70" s="2"/>
-    </row>
-    <row r="71" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A71" s="4"/>
-      <c r="B71" s="2"/>
-    </row>
-    <row r="72" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="9"/>
-      <c r="B72" s="2"/>
-    </row>
-    <row r="76" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="4"/>
-      <c r="B76" s="2"/>
-    </row>
-    <row r="77" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="4"/>
-      <c r="B77" s="2"/>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="3" t="s">
+      <c r="B91" s="2"/>
+    </row>
+    <row r="92" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A92" s="4"/>
+      <c r="B92" s="2"/>
+    </row>
+    <row r="93" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A93" s="9"/>
+      <c r="B93" s="2"/>
+    </row>
+    <row r="97" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A97" s="4"/>
+      <c r="B97" s="2"/>
+    </row>
+    <row r="98" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A98" s="4"/>
+      <c r="B98" s="2"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="3" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="3" t="s">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" s="3" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="3"/>
-    </row>
-    <row r="85" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A85" s="5" t="s">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" s="3"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" s="3"/>
+    </row>
+    <row r="106" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A106" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A86" s="5"/>
-    </row>
-    <row r="87" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A87" s="5"/>
-    </row>
-    <row r="88" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A88" s="4" t="s">
+    <row r="107" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A107" s="5"/>
+    </row>
+    <row r="108" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A108" s="5"/>
+    </row>
+    <row r="109" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A109" s="5"/>
+    </row>
+    <row r="110" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A110" s="5"/>
+    </row>
+    <row r="111" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A111" s="5"/>
+    </row>
+    <row r="112" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A112" s="5"/>
+    </row>
+    <row r="113" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A113" s="5"/>
+    </row>
+    <row r="114" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A114" s="5"/>
+    </row>
+    <row r="115" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A115" s="5"/>
+    </row>
+    <row r="116" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A116" s="5"/>
+    </row>
+    <row r="117" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A117" s="5"/>
+    </row>
+    <row r="118" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A118" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A119" s="4"/>
+    </row>
+    <row r="120" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A120" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A121" s="5"/>
+    </row>
+    <row r="122" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A122" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A89" s="5"/>
-    </row>
-    <row r="90" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A90" s="4" t="s">
+    <row r="123" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A123" s="5"/>
+    </row>
+    <row r="124" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A124" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A91" s="5"/>
-    </row>
-    <row r="92" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A92" s="4" t="s">
+    <row r="125" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A125" s="5"/>
+    </row>
+    <row r="126" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A126" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A93" s="4"/>
-    </row>
-    <row r="94" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A94" s="4" t="s">
+    <row r="127" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A127" s="4"/>
+    </row>
+    <row r="128" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A128" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B94" s="2"/>
-    </row>
-    <row r="95" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A95" s="5"/>
-    </row>
-    <row r="96" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A96" s="4" t="s">
+      <c r="B128" s="2"/>
+    </row>
+    <row r="129" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A129" s="5"/>
+    </row>
+    <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A130" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B96" s="2"/>
-    </row>
-    <row r="97" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A97" s="5"/>
-    </row>
-    <row r="98" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A98" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B98" s="2"/>
-    </row>
-    <row r="99" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A99" s="4"/>
-      <c r="B99" s="2"/>
-    </row>
-    <row r="100" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>27</v>
-      </c>
-      <c r="B100" s="2"/>
-    </row>
-    <row r="102" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A102" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B102" s="2"/>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
-        <v>4</v>
-      </c>
-      <c r="B128" s="2"/>
-    </row>
-    <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
-        <v>5</v>
-      </c>
       <c r="B130" s="2"/>
+    </row>
+    <row r="131" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A131" s="5"/>
     </row>
     <row r="132" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A132" s="4" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B132" s="2"/>
     </row>
@@ -1316,142 +1396,181 @@
       <c r="B133" s="2"/>
     </row>
     <row r="134" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A134" s="4" t="s">
-        <v>26</v>
+      <c r="A134" t="s">
+        <v>27</v>
       </c>
       <c r="B134" s="2"/>
-    </row>
-    <row r="135" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A135" s="4"/>
-      <c r="B135" s="2"/>
     </row>
     <row r="136" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A136" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B136" s="2"/>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>4</v>
+      </c>
+      <c r="B162" s="2"/>
+    </row>
+    <row r="164" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>5</v>
+      </c>
+      <c r="B164" s="2"/>
+    </row>
+    <row r="166" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A166" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B166" s="2"/>
+    </row>
+    <row r="167" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A167" s="4"/>
+      <c r="B167" s="2"/>
+    </row>
+    <row r="168" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A168" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B168" s="2"/>
+    </row>
+    <row r="169" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A169" s="4"/>
+      <c r="B169" s="2"/>
+    </row>
+    <row r="170" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A170" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B136" s="2"/>
-    </row>
-    <row r="138" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A138" s="4" t="s">
+      <c r="B170" s="2"/>
+    </row>
+    <row r="172" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A172" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B138" s="2"/>
-    </row>
-    <row r="139" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A139" s="1"/>
-      <c r="B139" s="2"/>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B140" s="6" t="s">
+      <c r="B172" s="2"/>
+    </row>
+    <row r="173" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A173" s="1"/>
+      <c r="B173" s="2"/>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B174" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A142" s="6"/>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A143" s="6"/>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A144" s="6"/>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A145" s="6" t="s">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A176" s="6"/>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A177" s="6"/>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A178" s="6"/>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A179" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A146" s="6" t="s">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A180" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A147" s="6" t="s">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A181" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A148" s="6"/>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A149" s="6" t="s">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A182" s="6"/>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A183" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A150" s="1"/>
-      <c r="B150" s="2"/>
-    </row>
-    <row r="151" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A151" s="1"/>
-      <c r="B151" s="2"/>
-    </row>
-    <row r="152" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A152" s="1"/>
-      <c r="B152" s="2"/>
-    </row>
-    <row r="153" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A153" s="1"/>
-      <c r="B153" s="2"/>
-    </row>
-    <row r="154" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A154" s="1"/>
-      <c r="B154" s="2"/>
-    </row>
-    <row r="155" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A155" s="1"/>
-      <c r="B155" s="2"/>
-    </row>
-    <row r="157" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A157" s="4" t="s">
+    <row r="184" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A184" s="1"/>
+      <c r="B184" s="2"/>
+    </row>
+    <row r="185" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A185" s="1"/>
+      <c r="B185" s="2"/>
+    </row>
+    <row r="186" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A186" s="1"/>
+      <c r="B186" s="2"/>
+    </row>
+    <row r="187" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A187" s="1"/>
+      <c r="B187" s="2"/>
+    </row>
+    <row r="188" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A188" s="1"/>
+      <c r="B188" s="2"/>
+    </row>
+    <row r="189" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A189" s="1"/>
+      <c r="B189" s="2"/>
+    </row>
+    <row r="191" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A191" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B157" s="2"/>
-    </row>
-    <row r="159" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A159" s="4" t="s">
+      <c r="B191" s="2"/>
+    </row>
+    <row r="193" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A193" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B159" s="2"/>
-    </row>
-    <row r="161" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A161" s="4" t="s">
+      <c r="B193" s="2"/>
+    </row>
+    <row r="195" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A195" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B161" s="2"/>
-    </row>
-    <row r="163" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A163" s="4" t="s">
+      <c r="B195" s="2"/>
+    </row>
+    <row r="197" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A197" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B163" s="2"/>
-    </row>
-    <row r="165" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A165" s="9" t="s">
+      <c r="B197" s="2"/>
+    </row>
+    <row r="199" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A199" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A167" s="4" t="s">
+    <row r="201" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A201" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B167" s="2"/>
-    </row>
-    <row r="168" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A168" s="1"/>
-      <c r="B168" s="2"/>
-    </row>
-    <row r="169" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A169" s="4" t="s">
+      <c r="B201" s="2"/>
+    </row>
+    <row r="202" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A202" s="1"/>
+      <c r="B202" s="2"/>
+    </row>
+    <row r="203" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A203" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B169" s="2"/>
-    </row>
-    <row r="171" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A171" s="4" t="s">
+      <c r="B203" s="2"/>
+    </row>
+    <row r="205" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A205" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B171" s="2"/>
+      <c r="B205" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updates docu, adds Create Employee View
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="656" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0604D58D-13F5-4BE4-9741-88511EE13EB7}"/>
+  <xr:revisionPtr revIDLastSave="685" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72C25583-C4E5-4D2A-A67C-40E22149E06E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
   <si>
     <t>…..</t>
   </si>
@@ -249,6 +249,30 @@
   </si>
   <si>
     <t>Überlegen wenn Manager sich Urlaub selber einträgt, dann gleich Zeitbuchung machen!</t>
+  </si>
+  <si>
+    <t>eigene Adress Form machen</t>
+  </si>
+  <si>
+    <t>Im Employee Overview Button machen "Erstelle einen Mitarbeiter"</t>
+  </si>
+  <si>
+    <t>So fort bei Auswählen der Rolle anfangen die anderen auszublenden - Superior oder Subordinates</t>
+  </si>
+  <si>
+    <t>Eigener Screen Employees reporting to me and all employees</t>
+  </si>
+  <si>
+    <t>UseCreate an Employee to update</t>
+  </si>
+  <si>
+    <t>Doku updaten</t>
+  </si>
+  <si>
+    <t>All Employees not slectable</t>
+  </si>
+  <si>
+    <t>Context to save employee to update</t>
   </si>
 </sst>
 </file>
@@ -380,13 +404,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>152</xdr:row>
+      <xdr:row>168</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>166</xdr:row>
+      <xdr:row>182</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -441,14 +465,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
-      <xdr:row>117</xdr:row>
+      <xdr:row>133</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3295127</xdr:colOff>
-      <xdr:row>137</xdr:row>
-      <xdr:rowOff>18740</xdr:rowOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>18741</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -485,14 +509,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1810160</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>193412</xdr:rowOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>193411</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -540,13 +564,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2599763</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>158071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4461042</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>79844</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -861,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G183"/>
+  <dimension ref="A1:G199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -898,47 +922,49 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="A7" s="1"/>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="A9" s="1"/>
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="A11" s="1"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
+    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
-        <v>57</v>
-      </c>
+    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
       <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -946,8 +972,8 @@
       <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
-        <v>59</v>
+      <c r="A16" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="B16" s="2"/>
     </row>
@@ -955,8 +981,10 @@
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
+    <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -964,7 +992,9 @@
       <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -972,58 +1002,56 @@
       <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
-        <v>42</v>
-      </c>
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
+      <c r="A23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>36</v>
-      </c>
+      <c r="A24" s="1"/>
       <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
+      <c r="A25" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="9"/>
+      <c r="A26" s="1"/>
+      <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
+      <c r="A27" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="11" t="s">
-        <v>63</v>
-      </c>
+    <row r="28" spans="1:2" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
+    <row r="29" spans="1:2" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="B29" s="2"/>
     </row>
     <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>47</v>
-      </c>
+      <c r="A30" s="1"/>
       <c r="B30" s="2"/>
     </row>
     <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>64</v>
-      </c>
+      <c r="A31" s="1"/>
       <c r="B31" s="2"/>
     </row>
     <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B32" s="2"/>
     </row>
@@ -1032,273 +1060,285 @@
       <c r="B33" s="2"/>
     </row>
     <row r="34" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>39</v>
-      </c>
+      <c r="A34" s="1"/>
       <c r="B34" s="2"/>
     </row>
     <row r="35" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="36" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+    </row>
+    <row r="40" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="1"/>
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" s="9"/>
+    </row>
+    <row r="43" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="2"/>
+    </row>
+    <row r="46" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="2"/>
+    </row>
+    <row r="47" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" s="2"/>
+    </row>
+    <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="1"/>
+      <c r="B49" s="2"/>
+    </row>
+    <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" s="2"/>
+    </row>
+    <row r="51" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="1"/>
+      <c r="B51" s="2"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
+    <row r="55" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
-      <c r="B40" s="2"/>
-    </row>
-    <row r="41" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B41" s="2"/>
-    </row>
-    <row r="42" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="1"/>
-      <c r="B42" s="2"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="10"/>
-    </row>
-    <row r="47" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>46</v>
-      </c>
-      <c r="B47" s="2"/>
-    </row>
-    <row r="48" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="1"/>
-      <c r="B48" s="2"/>
-    </row>
-    <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B49" s="2"/>
-      <c r="G49" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B50" s="2"/>
-    </row>
-    <row r="51" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="1"/>
-      <c r="B52" s="2"/>
-    </row>
-    <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="1"/>
-      <c r="B53" s="2"/>
-    </row>
-    <row r="54" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="1"/>
-      <c r="B54" s="2"/>
-    </row>
-    <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="1"/>
       <c r="B55" s="2"/>
     </row>
-    <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
     </row>
-    <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="1"/>
+    <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="B57" s="2"/>
     </row>
-    <row r="58" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
     </row>
-    <row r="59" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="1"/>
-      <c r="B59" s="2"/>
-    </row>
-    <row r="60" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="1"/>
-      <c r="B60" s="2"/>
-    </row>
-    <row r="61" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="1"/>
-      <c r="B61" s="2"/>
-    </row>
-    <row r="62" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="1"/>
-      <c r="B62" s="2"/>
-    </row>
-    <row r="63" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="1"/>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="10"/>
+    </row>
+    <row r="63" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>46</v>
+      </c>
       <c r="B63" s="2"/>
     </row>
-    <row r="64" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
     </row>
-    <row r="65" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="1"/>
+    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="B65" s="2"/>
-    </row>
-    <row r="66" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="1"/>
+      <c r="G65" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="B66" s="2"/>
     </row>
-    <row r="67" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B67" s="2"/>
-    </row>
-    <row r="68" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="2"/>
     </row>
-    <row r="69" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="4" t="s">
-        <v>23</v>
-      </c>
+    <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="1"/>
       <c r="B69" s="2"/>
     </row>
-    <row r="70" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
     </row>
-    <row r="71" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A71" s="4" t="s">
+    <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A71" s="1"/>
+      <c r="B71" s="2"/>
+    </row>
+    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="1"/>
+      <c r="B72" s="2"/>
+    </row>
+    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="1"/>
+      <c r="B73" s="2"/>
+    </row>
+    <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="1"/>
+      <c r="B74" s="2"/>
+    </row>
+    <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="1"/>
+      <c r="B75" s="2"/>
+    </row>
+    <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="1"/>
+      <c r="B76" s="2"/>
+    </row>
+    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="1"/>
+      <c r="B77" s="2"/>
+    </row>
+    <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="1"/>
+      <c r="B78" s="2"/>
+    </row>
+    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="1"/>
+      <c r="B79" s="2"/>
+    </row>
+    <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="1"/>
+      <c r="B80" s="2"/>
+    </row>
+    <row r="81" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="1"/>
+      <c r="B81" s="2"/>
+    </row>
+    <row r="82" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="1"/>
+      <c r="B82" s="2"/>
+    </row>
+    <row r="83" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B83" s="2"/>
+    </row>
+    <row r="84" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="1"/>
+      <c r="B84" s="2"/>
+    </row>
+    <row r="85" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B85" s="2"/>
+    </row>
+    <row r="86" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A86" s="1"/>
+      <c r="B86" s="2"/>
+    </row>
+    <row r="87" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A87" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B71" s="2"/>
-    </row>
-    <row r="72" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="4"/>
-      <c r="B72" s="2"/>
-    </row>
-    <row r="73" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="9"/>
-      <c r="B73" s="2"/>
-    </row>
-    <row r="77" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="4"/>
-      <c r="B77" s="2"/>
-    </row>
-    <row r="78" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="4"/>
-      <c r="B78" s="2"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="3"/>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" s="3"/>
-    </row>
-    <row r="86" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A86" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A87" s="5"/>
+      <c r="B87" s="2"/>
     </row>
     <row r="88" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A88" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A90" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A91" s="5"/>
-    </row>
-    <row r="92" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A92" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B92" s="2"/>
+      <c r="A88" s="4"/>
+      <c r="B88" s="2"/>
+    </row>
+    <row r="89" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A89" s="9"/>
+      <c r="B89" s="2"/>
     </row>
     <row r="93" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="4"/>
       <c r="B93" s="2"/>
     </row>
     <row r="94" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>44</v>
-      </c>
+      <c r="A94" s="4"/>
       <c r="B94" s="2"/>
     </row>
-    <row r="95" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A95" s="5"/>
-    </row>
-    <row r="96" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A96" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A97" s="4"/>
-    </row>
-    <row r="98" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A98" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A99" s="5"/>
-    </row>
-    <row r="100" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A100" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A101" s="5"/>
-    </row>
-    <row r="102" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A102" s="4" t="s">
-        <v>29</v>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" s="3"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" s="3"/>
+    </row>
+    <row r="102" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A102" s="13" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="21" x14ac:dyDescent="0.4">
@@ -1306,199 +1346,212 @@
     </row>
     <row r="104" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A105" s="4"/>
+        <v>61</v>
+      </c>
     </row>
     <row r="106" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B106" s="2"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="107" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A107" s="5"/>
     </row>
     <row r="108" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B108" s="2"/>
     </row>
-    <row r="109" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A109" s="5"/>
+    <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A109" s="4"/>
+      <c r="B109" s="2"/>
     </row>
     <row r="110" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A110" s="4" t="s">
-        <v>32</v>
+      <c r="A110" t="s">
+        <v>44</v>
       </c>
       <c r="B110" s="2"/>
     </row>
-    <row r="111" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A111" s="4"/>
-      <c r="B111" s="2"/>
+    <row r="111" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A111" s="5"/>
     </row>
     <row r="112" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>27</v>
-      </c>
-      <c r="B112" s="2"/>
+      <c r="A112" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A113" s="4"/>
     </row>
     <row r="114" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A115" s="5"/>
+    </row>
+    <row r="116" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A116" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A117" s="5"/>
+    </row>
+    <row r="118" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A118" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A119" s="5"/>
+    </row>
+    <row r="120" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A120" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A121" s="4"/>
+    </row>
+    <row r="122" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A122" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B122" s="2"/>
+    </row>
+    <row r="123" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A123" s="5"/>
+    </row>
+    <row r="124" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A124" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B124" s="2"/>
+    </row>
+    <row r="125" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A125" s="5"/>
+    </row>
+    <row r="126" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A126" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B126" s="2"/>
+    </row>
+    <row r="127" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A127" s="4"/>
+      <c r="B127" s="2"/>
+    </row>
+    <row r="128" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>27</v>
+      </c>
+      <c r="B128" s="2"/>
+    </row>
+    <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A130" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B114" s="2"/>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
+      <c r="B130" s="2"/>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
+    <row r="156" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
         <v>4</v>
       </c>
-      <c r="B140" s="2"/>
-    </row>
-    <row r="142" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A142" t="s">
+      <c r="B156" s="2"/>
+    </row>
+    <row r="158" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
         <v>5</v>
       </c>
-      <c r="B142" s="2"/>
-    </row>
-    <row r="144" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A144" s="4" t="s">
+      <c r="B158" s="2"/>
+    </row>
+    <row r="160" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A160" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B144" s="2"/>
-    </row>
-    <row r="145" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A145" s="4"/>
-      <c r="B145" s="2"/>
-    </row>
-    <row r="146" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A146" s="4" t="s">
+      <c r="B160" s="2"/>
+    </row>
+    <row r="161" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A161" s="4"/>
+      <c r="B161" s="2"/>
+    </row>
+    <row r="162" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A162" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B146" s="2"/>
-    </row>
-    <row r="147" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A147" s="4"/>
-      <c r="B147" s="2"/>
-    </row>
-    <row r="148" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A148" s="4" t="s">
+      <c r="B162" s="2"/>
+    </row>
+    <row r="163" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A163" s="4"/>
+      <c r="B163" s="2"/>
+    </row>
+    <row r="164" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A164" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B148" s="2"/>
-    </row>
-    <row r="150" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A150" s="4" t="s">
+      <c r="B164" s="2"/>
+    </row>
+    <row r="166" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A166" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B150" s="2"/>
-    </row>
-    <row r="151" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A151" s="1"/>
-      <c r="B151" s="2"/>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B152" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A154" s="6"/>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A155" s="6"/>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A156" s="6"/>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A157" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A158" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A159" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A160" s="6"/>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A161" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A162" s="1"/>
-      <c r="B162" s="2"/>
-    </row>
-    <row r="163" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A163" s="1"/>
-      <c r="B163" s="2"/>
-    </row>
-    <row r="164" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A164" s="1"/>
-      <c r="B164" s="2"/>
-    </row>
-    <row r="165" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A165" s="1"/>
-      <c r="B165" s="2"/>
-    </row>
-    <row r="166" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A166" s="1"/>
       <c r="B166" s="2"/>
     </row>
     <row r="167" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A167" s="1"/>
       <c r="B167" s="2"/>
     </row>
-    <row r="169" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A169" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B169" s="2"/>
-    </row>
-    <row r="171" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A171" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B171" s="2"/>
-    </row>
-    <row r="173" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A173" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B173" s="2"/>
-    </row>
-    <row r="175" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A175" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B175" s="2"/>
-    </row>
-    <row r="177" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A177" s="9" t="s">
-        <v>43</v>
-      </c>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B168" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A170" s="6"/>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A171" s="6"/>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A172" s="6"/>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A173" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A174" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A175" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A176" s="6"/>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A177" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A178" s="1"/>
+      <c r="B178" s="2"/>
     </row>
     <row r="179" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A179" s="4" t="s">
-        <v>40</v>
-      </c>
+      <c r="A179" s="1"/>
       <c r="B179" s="2"/>
     </row>
     <row r="180" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1506,16 +1559,67 @@
       <c r="B180" s="2"/>
     </row>
     <row r="181" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A181" s="4" t="s">
+      <c r="A181" s="1"/>
+      <c r="B181" s="2"/>
+    </row>
+    <row r="182" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A182" s="1"/>
+      <c r="B182" s="2"/>
+    </row>
+    <row r="183" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A183" s="1"/>
+      <c r="B183" s="2"/>
+    </row>
+    <row r="185" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A185" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B185" s="2"/>
+    </row>
+    <row r="187" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A187" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B187" s="2"/>
+    </row>
+    <row r="189" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A189" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B189" s="2"/>
+    </row>
+    <row r="191" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A191" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B191" s="2"/>
+    </row>
+    <row r="193" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A193" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A195" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B195" s="2"/>
+    </row>
+    <row r="196" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A196" s="1"/>
+      <c r="B196" s="2"/>
+    </row>
+    <row r="197" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A197" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B181" s="2"/>
-    </row>
-    <row r="183" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A183" s="4" t="s">
+      <c r="B197" s="2"/>
+    </row>
+    <row r="199" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A199" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B183" s="2"/>
+      <c r="B199" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adds going forward and backward functionality
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="685" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72C25583-C4E5-4D2A-A67C-40E22149E06E}"/>
+  <xr:revisionPtr revIDLastSave="688" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10958D38-EA16-449B-B3FF-6F50BD239BF5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
   <si>
     <t>…..</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>Context to save employee to update</t>
+  </si>
+  <si>
+    <t>Constants Employee overview</t>
   </si>
 </sst>
 </file>
@@ -404,13 +407,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>170</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>182</xdr:row>
+      <xdr:row>184</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -465,13 +468,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
-      <xdr:row>133</xdr:row>
+      <xdr:row>135</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3295127</xdr:colOff>
-      <xdr:row>153</xdr:row>
+      <xdr:row>155</xdr:row>
       <xdr:rowOff>18741</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -509,13 +512,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1810160</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>193411</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -564,13 +567,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2599763</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>158071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4461042</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>79844</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -885,10 +888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G199"/>
+  <dimension ref="A1:G201"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -993,7 +996,7 @@
     </row>
     <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B20" s="2"/>
     </row>
@@ -1002,13 +1005,13 @@
       <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="A23" s="1"/>
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1017,7 +1020,7 @@
     </row>
     <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B25" s="2"/>
     </row>
@@ -1026,33 +1029,33 @@
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>56</v>
+      <c r="A27" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="1:2" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="1:2" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="12" t="s">
-        <v>57</v>
+    <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
+    <row r="31" spans="1:2" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="B31" s="2"/>
     </row>
     <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="A32" s="1"/>
       <c r="B32" s="2"/>
     </row>
     <row r="33" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1060,7 +1063,9 @@
       <c r="B33" s="2"/>
     </row>
     <row r="34" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
+      <c r="A34" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="B34" s="2"/>
     </row>
     <row r="35" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1076,68 +1081,66 @@
       <c r="B37" s="2"/>
     </row>
     <row r="38" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="9" t="s">
-        <v>42</v>
-      </c>
+      <c r="A38" s="1"/>
+      <c r="B38" s="2"/>
     </row>
     <row r="39" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
+      <c r="B39" s="2"/>
     </row>
     <row r="40" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B40" s="2"/>
+      <c r="A40" s="9" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="41" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
-      <c r="B41" s="2"/>
     </row>
     <row r="42" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B42" s="9"/>
+        <v>36</v>
+      </c>
+      <c r="B42" s="2"/>
     </row>
     <row r="43" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
     </row>
     <row r="44" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B44" s="2"/>
+      <c r="A44" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" s="9"/>
     </row>
     <row r="45" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
     </row>
     <row r="46" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" s="2"/>
+    </row>
+    <row r="47" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B46" s="2"/>
-    </row>
-    <row r="47" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
+      <c r="B48" s="2"/>
+    </row>
+    <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B47" s="2"/>
-    </row>
-    <row r="48" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="11" t="s">
+      <c r="B49" s="2"/>
+    </row>
+    <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="11" t="s">
         <v>63</v>
-      </c>
-      <c r="B48" s="2"/>
-    </row>
-    <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="1"/>
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="B50" s="2"/>
     </row>
@@ -1145,24 +1148,24 @@
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B52" s="2"/>
+    </row>
+    <row r="53" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
+      <c r="B53" s="2"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B55" s="2"/>
-    </row>
-    <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="1"/>
-      <c r="B56" s="2"/>
     </row>
     <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B57" s="2"/>
     </row>
@@ -1170,51 +1173,53 @@
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="10" t="s">
+    <row r="59" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B59" s="2"/>
+    </row>
+    <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="1"/>
+      <c r="B60" s="2"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="10"/>
-    </row>
-    <row r="63" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="10"/>
+    </row>
+    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>46</v>
       </c>
-      <c r="B63" s="2"/>
-    </row>
-    <row r="64" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="1"/>
-      <c r="B64" s="2"/>
-    </row>
-    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="4" t="s">
+      <c r="B65" s="2"/>
+    </row>
+    <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="1"/>
+      <c r="B66" s="2"/>
+    </row>
+    <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B65" s="2"/>
-      <c r="G65" t="s">
+      <c r="B67" s="2"/>
+      <c r="G67" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="4" t="s">
+    <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B66" s="2"/>
-    </row>
-    <row r="67" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="8" t="s">
+      <c r="B68" s="2"/>
+    </row>
+    <row r="69" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A68" s="1"/>
-      <c r="B68" s="2"/>
-    </row>
-    <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="1"/>
-      <c r="B69" s="2"/>
     </row>
     <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
@@ -1269,9 +1274,7 @@
       <c r="B82" s="2"/>
     </row>
     <row r="83" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="4" t="s">
-        <v>28</v>
-      </c>
+      <c r="A83" s="1"/>
       <c r="B83" s="2"/>
     </row>
     <row r="84" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1280,7 +1283,7 @@
     </row>
     <row r="85" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B85" s="2"/>
     </row>
@@ -1290,111 +1293,113 @@
     </row>
     <row r="87" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B87" s="2"/>
+    </row>
+    <row r="88" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="1"/>
+      <c r="B88" s="2"/>
+    </row>
+    <row r="89" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A89" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B87" s="2"/>
-    </row>
-    <row r="88" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A88" s="4"/>
-      <c r="B88" s="2"/>
-    </row>
-    <row r="89" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A89" s="9"/>
       <c r="B89" s="2"/>
     </row>
-    <row r="93" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A93" s="4"/>
-      <c r="B93" s="2"/>
-    </row>
-    <row r="94" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A94" s="4"/>
-      <c r="B94" s="2"/>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" s="3" t="s">
-        <v>1</v>
-      </c>
+    <row r="90" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A90" s="4"/>
+      <c r="B90" s="2"/>
+    </row>
+    <row r="91" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A91" s="9"/>
+      <c r="B91" s="2"/>
+    </row>
+    <row r="95" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A95" s="4"/>
+      <c r="B95" s="2"/>
+    </row>
+    <row r="96" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A96" s="4"/>
+      <c r="B96" s="2"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="3"/>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" s="3"/>
-    </row>
-    <row r="102" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A102" s="13" t="s">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" s="3"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" s="3"/>
+    </row>
+    <row r="104" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A104" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A103" s="5"/>
-    </row>
-    <row r="104" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A104" s="4" t="s">
-        <v>61</v>
-      </c>
+    <row r="105" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A105" s="5"/>
     </row>
     <row r="106" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A107" s="5"/>
+        <v>61</v>
+      </c>
     </row>
     <row r="108" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A109" s="5"/>
+    </row>
+    <row r="110" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A110" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B108" s="2"/>
-    </row>
-    <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A109" s="4"/>
-      <c r="B109" s="2"/>
-    </row>
-    <row r="110" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
+      <c r="B110" s="2"/>
+    </row>
+    <row r="111" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A111" s="4"/>
+      <c r="B111" s="2"/>
+    </row>
+    <row r="112" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
         <v>44</v>
       </c>
-      <c r="B110" s="2"/>
-    </row>
-    <row r="111" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A111" s="5"/>
-    </row>
-    <row r="112" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A112" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A113" s="4"/>
+      <c r="B112" s="2"/>
+    </row>
+    <row r="113" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A113" s="5"/>
     </row>
     <row r="114" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A115" s="5"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A115" s="4"/>
     </row>
     <row r="116" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="21" x14ac:dyDescent="0.4">
@@ -1402,7 +1407,7 @@
     </row>
     <row r="118" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="21" x14ac:dyDescent="0.4">
@@ -1410,24 +1415,23 @@
     </row>
     <row r="120" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A120" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A121" s="4"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A121" s="5"/>
     </row>
     <row r="122" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A122" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B122" s="2"/>
-    </row>
-    <row r="123" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A123" s="5"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A123" s="4"/>
     </row>
     <row r="124" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B124" s="2"/>
     </row>
@@ -1436,56 +1440,55 @@
     </row>
     <row r="126" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A126" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B126" s="2"/>
+    </row>
+    <row r="127" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A127" s="5"/>
+    </row>
+    <row r="128" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A128" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B126" s="2"/>
-    </row>
-    <row r="127" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A127" s="4"/>
-      <c r="B127" s="2"/>
-    </row>
-    <row r="128" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
+      <c r="B128" s="2"/>
+    </row>
+    <row r="129" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A129" s="4"/>
+      <c r="B129" s="2"/>
+    </row>
+    <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
         <v>27</v>
       </c>
-      <c r="B128" s="2"/>
-    </row>
-    <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A130" s="4" t="s">
+      <c r="B130" s="2"/>
+    </row>
+    <row r="132" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A132" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B130" s="2"/>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
+      <c r="B132" s="2"/>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="156" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A156" t="s">
-        <v>4</v>
-      </c>
-      <c r="B156" s="2"/>
     </row>
     <row r="158" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
+        <v>4</v>
+      </c>
+      <c r="B158" s="2"/>
+    </row>
+    <row r="160" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
         <v>5</v>
       </c>
-      <c r="B158" s="2"/>
-    </row>
-    <row r="160" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A160" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="B160" s="2"/>
-    </row>
-    <row r="161" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A161" s="4"/>
-      <c r="B161" s="2"/>
     </row>
     <row r="162" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A162" s="4" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B162" s="2"/>
     </row>
@@ -1495,64 +1498,66 @@
     </row>
     <row r="164" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A164" s="4" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B164" s="2"/>
+    </row>
+    <row r="165" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A165" s="4"/>
+      <c r="B165" s="2"/>
     </row>
     <row r="166" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A166" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B166" s="2"/>
+    </row>
+    <row r="168" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A168" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B166" s="2"/>
-    </row>
-    <row r="167" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A167" s="1"/>
-      <c r="B167" s="2"/>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B168" s="6" t="s">
+      <c r="B168" s="2"/>
+    </row>
+    <row r="169" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A169" s="1"/>
+      <c r="B169" s="2"/>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B170" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A170" s="6"/>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A171" s="6"/>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" s="6"/>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A173" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="A173" s="6"/>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A174" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="A174" s="6"/>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A176" s="6"/>
+      <c r="A176" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A178" s="6"/>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A179" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="178" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A178" s="1"/>
-      <c r="B178" s="2"/>
-    </row>
-    <row r="179" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A179" s="1"/>
-      <c r="B179" s="2"/>
     </row>
     <row r="180" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A180" s="1"/>
@@ -1570,56 +1575,64 @@
       <c r="A183" s="1"/>
       <c r="B183" s="2"/>
     </row>
+    <row r="184" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A184" s="1"/>
+      <c r="B184" s="2"/>
+    </row>
     <row r="185" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A185" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="A185" s="1"/>
       <c r="B185" s="2"/>
     </row>
     <row r="187" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A187" s="4" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B187" s="2"/>
     </row>
     <row r="189" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A189" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B189" s="2"/>
     </row>
     <row r="191" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A191" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B191" s="2"/>
+    </row>
+    <row r="193" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A193" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B191" s="2"/>
-    </row>
-    <row r="193" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A193" s="9" t="s">
+      <c r="B193" s="2"/>
+    </row>
+    <row r="195" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A195" s="9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="195" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A195" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B195" s="2"/>
-    </row>
-    <row r="196" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A196" s="1"/>
-      <c r="B196" s="2"/>
     </row>
     <row r="197" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A197" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B197" s="2"/>
+    </row>
+    <row r="198" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A198" s="1"/>
+      <c r="B198" s="2"/>
     </row>
     <row r="199" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A199" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B199" s="2"/>
+    </row>
+    <row r="201" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A201" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B199" s="2"/>
+      <c r="B201" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adds creating a new employee
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="688" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10958D38-EA16-449B-B3FF-6F50BD239BF5}"/>
+  <xr:revisionPtr revIDLastSave="715" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E06F7E78-B51B-429C-8A95-A80A371BCA87}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
   <si>
     <t>…..</t>
   </si>
@@ -258,9 +258,6 @@
   </si>
   <si>
     <t>So fort bei Auswählen der Rolle anfangen die anderen auszublenden - Superior oder Subordinates</t>
-  </si>
-  <si>
-    <t>Eigener Screen Employees reporting to me and all employees</t>
   </si>
   <si>
     <t>UseCreate an Employee to update</t>
@@ -407,13 +404,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>170</xdr:row>
+      <xdr:row>167</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>184</xdr:row>
+      <xdr:row>181</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -468,13 +465,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
-      <xdr:row>135</xdr:row>
+      <xdr:row>132</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3295127</xdr:colOff>
-      <xdr:row>155</xdr:row>
+      <xdr:row>152</xdr:row>
       <xdr:rowOff>18741</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -512,13 +509,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1810160</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>193411</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -567,13 +564,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2599763</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>158071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4461042</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>79844</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -888,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G201"/>
+  <dimension ref="A1:G198"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -925,89 +922,87 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="4" t="s">
         <v>65</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7" s="4"/>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>66</v>
+      <c r="A8" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
+      <c r="A9" s="4"/>
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>67</v>
+      <c r="A10" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
+      <c r="A11" s="4"/>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>68</v>
+      <c r="A12" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
+      <c r="A13" s="4"/>
       <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="A14" s="1"/>
       <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="A16" s="1"/>
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>71</v>
-      </c>
+    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
       <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
+      <c r="A19" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>73</v>
-      </c>
+    <row r="20" spans="1:2" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
+    <row r="21" spans="1:2" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="A22" s="1"/>
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1015,13 +1010,13 @@
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
+      <c r="A24" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="A25" s="1"/>
       <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1029,9 +1024,7 @@
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="A27" s="1"/>
       <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1039,23 +1032,21 @@
       <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="A29" s="1"/>
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:2" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
-    </row>
-    <row r="31" spans="1:2" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" s="2"/>
+    <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
     </row>
     <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
+      <c r="A32" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="B32" s="2"/>
     </row>
     <row r="33" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1063,17 +1054,19 @@
       <c r="B33" s="2"/>
     </row>
     <row r="34" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B34" s="2"/>
+      <c r="A34" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="9"/>
     </row>
     <row r="35" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
     </row>
     <row r="36" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
+      <c r="A36" s="11" t="s">
+        <v>63</v>
+      </c>
       <c r="B36" s="2"/>
     </row>
     <row r="37" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1081,24 +1074,30 @@
       <c r="B37" s="2"/>
     </row>
     <row r="38" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
+      <c r="A38" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="B38" s="2"/>
     </row>
     <row r="39" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="1"/>
+      <c r="A39" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="B39" s="2"/>
     </row>
     <row r="40" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="9" t="s">
-        <v>42</v>
-      </c>
+      <c r="A40" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="2"/>
     </row>
     <row r="41" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
+      <c r="B41" s="2"/>
     </row>
     <row r="42" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B42" s="2"/>
     </row>
@@ -1106,458 +1105,450 @@
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B44" s="9"/>
-    </row>
-    <row r="45" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="1"/>
-      <c r="B45" s="2"/>
-    </row>
-    <row r="46" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B46" s="2"/>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="47" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="1"/>
+      <c r="A47" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="B47" s="2"/>
     </row>
     <row r="48" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
-        <v>47</v>
-      </c>
+      <c r="A48" s="1"/>
       <c r="B48" s="2"/>
     </row>
-    <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="B49" s="2"/>
     </row>
-    <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="11" t="s">
-        <v>63</v>
-      </c>
+    <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
       <c r="B50" s="2"/>
     </row>
-    <row r="51" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="1"/>
-      <c r="B51" s="2"/>
-    </row>
-    <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B52" s="2"/>
-    </row>
-    <row r="53" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="1"/>
-      <c r="B53" s="2"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="10"/>
+    </row>
+    <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>46</v>
+      </c>
+      <c r="B55" s="2"/>
+    </row>
+    <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="1"/>
+      <c r="B56" s="2"/>
+    </row>
+    <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B57" s="2"/>
-    </row>
-    <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="1"/>
+      <c r="G57" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="B58" s="2"/>
     </row>
-    <row r="59" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B59" s="2"/>
-    </row>
-    <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="10"/>
-    </row>
-    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>46</v>
-      </c>
+    <row r="61" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="1"/>
+      <c r="B61" s="2"/>
+    </row>
+    <row r="62" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="1"/>
+      <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="1"/>
+      <c r="B63" s="2"/>
+    </row>
+    <row r="64" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="1"/>
+      <c r="B64" s="2"/>
+    </row>
+    <row r="65" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="1"/>
       <c r="B65" s="2"/>
     </row>
-    <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="2"/>
     </row>
-    <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="4" t="s">
-        <v>20</v>
-      </c>
+    <row r="67" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="1"/>
       <c r="B67" s="2"/>
-      <c r="G67" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A68" s="4" t="s">
-        <v>24</v>
-      </c>
+    </row>
+    <row r="68" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="1"/>
       <c r="B68" s="2"/>
     </row>
-    <row r="69" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="1"/>
+      <c r="B69" s="2"/>
+    </row>
+    <row r="70" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
     </row>
-    <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="2"/>
     </row>
-    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
     </row>
-    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="2"/>
     </row>
-    <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="2"/>
     </row>
-    <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="1"/>
+    <row r="75" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B75" s="2"/>
     </row>
-    <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
     </row>
-    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="1"/>
+    <row r="77" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="B77" s="2"/>
     </row>
-    <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="2"/>
     </row>
-    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A79" s="1"/>
+    <row r="79" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="B79" s="2"/>
     </row>
-    <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A80" s="1"/>
+    <row r="80" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="4"/>
       <c r="B80" s="2"/>
     </row>
     <row r="81" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A81" s="1"/>
+      <c r="A81" s="9"/>
       <c r="B81" s="2"/>
     </row>
-    <row r="82" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="1"/>
-      <c r="B82" s="2"/>
-    </row>
-    <row r="83" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="1"/>
-      <c r="B83" s="2"/>
-    </row>
-    <row r="84" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A84" s="1"/>
-      <c r="B84" s="2"/>
-    </row>
     <row r="85" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A85" s="4" t="s">
-        <v>28</v>
-      </c>
+      <c r="A85" s="4"/>
       <c r="B85" s="2"/>
     </row>
     <row r="86" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="1"/>
+      <c r="A86" s="4"/>
       <c r="B86" s="2"/>
     </row>
-    <row r="87" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A87" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B87" s="2"/>
-    </row>
-    <row r="88" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A88" s="1"/>
-      <c r="B88" s="2"/>
-    </row>
-    <row r="89" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A89" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B89" s="2"/>
-    </row>
-    <row r="90" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A90" s="4"/>
-      <c r="B90" s="2"/>
-    </row>
-    <row r="91" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A91" s="9"/>
-      <c r="B91" s="2"/>
-    </row>
-    <row r="95" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A95" s="4"/>
-      <c r="B95" s="2"/>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" s="3"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" s="3"/>
+    </row>
+    <row r="94" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A94" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="96" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="4"/>
-      <c r="B96" s="2"/>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" s="3"/>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" s="3"/>
-    </row>
-    <row r="104" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A104" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A105" s="5"/>
-    </row>
-    <row r="106" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A106" s="4" t="s">
+    </row>
+    <row r="97" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A97" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A98" s="13"/>
+    </row>
+    <row r="99" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A99" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B99" s="2"/>
+    </row>
+    <row r="100" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A100" s="4"/>
+      <c r="B100" s="2"/>
+    </row>
+    <row r="101" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A101" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B101" s="2"/>
+    </row>
+    <row r="102" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A102" s="5"/>
+    </row>
+    <row r="103" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A103" s="4" t="s">
         <v>61</v>
       </c>
     </row>
+    <row r="105" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A105" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A106" s="5"/>
+    </row>
+    <row r="107" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A107" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B107" s="2"/>
+    </row>
     <row r="108" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A108" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A109" s="5"/>
-    </row>
-    <row r="110" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A110" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B110" s="2"/>
+      <c r="A108" s="4"/>
+      <c r="B108" s="2"/>
+    </row>
+    <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>44</v>
+      </c>
+      <c r="B109" s="2"/>
+    </row>
+    <row r="110" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A110" s="5"/>
     </row>
     <row r="111" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A111" s="4"/>
-      <c r="B111" s="2"/>
+      <c r="A111" s="4" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="112" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>44</v>
-      </c>
-      <c r="B112" s="2"/>
-    </row>
-    <row r="113" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A113" s="5"/>
-    </row>
-    <row r="114" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A114" s="4" t="s">
-        <v>49</v>
-      </c>
+      <c r="A112" s="4"/>
+    </row>
+    <row r="113" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A113" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A114" s="5"/>
     </row>
     <row r="115" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A115" s="4"/>
-    </row>
-    <row r="116" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A116" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A117" s="5"/>
-    </row>
-    <row r="118" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A118" s="4" t="s">
+      <c r="A115" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A119" s="5"/>
+    <row r="116" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A116" s="5"/>
+    </row>
+    <row r="117" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A117" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A118" s="5"/>
+    </row>
+    <row r="119" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A119" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="120" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A120" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A121" s="5"/>
-    </row>
-    <row r="122" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A122" s="4" t="s">
-        <v>48</v>
-      </c>
+      <c r="A120" s="4"/>
+    </row>
+    <row r="121" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A121" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B121" s="2"/>
+    </row>
+    <row r="122" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A122" s="5"/>
     </row>
     <row r="123" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A123" s="4"/>
-    </row>
-    <row r="124" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A124" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B124" s="2"/>
-    </row>
-    <row r="125" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A125" s="5"/>
+      <c r="A123" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B123" s="2"/>
+    </row>
+    <row r="124" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A124" s="5"/>
+    </row>
+    <row r="125" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A125" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B125" s="2"/>
     </row>
     <row r="126" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A126" s="4" t="s">
-        <v>30</v>
-      </c>
+      <c r="A126" s="4"/>
       <c r="B126" s="2"/>
     </row>
-    <row r="127" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A127" s="5"/>
-    </row>
-    <row r="128" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A128" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B128" s="2"/>
+    <row r="127" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>27</v>
+      </c>
+      <c r="B127" s="2"/>
     </row>
     <row r="129" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A129" s="4"/>
+      <c r="A129" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="B129" s="2"/>
     </row>
-    <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
-        <v>27</v>
-      </c>
-      <c r="B130" s="2"/>
-    </row>
-    <row r="132" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A132" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B132" s="2"/>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A134" t="s">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A158" t="s">
+    <row r="155" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
         <v>4</v>
       </c>
-      <c r="B158" s="2"/>
+      <c r="B155" s="2"/>
+    </row>
+    <row r="157" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>5</v>
+      </c>
+      <c r="B157" s="2"/>
+    </row>
+    <row r="159" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A159" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B159" s="2"/>
     </row>
     <row r="160" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A160" t="s">
-        <v>5</v>
-      </c>
+      <c r="A160" s="4"/>
       <c r="B160" s="2"/>
     </row>
+    <row r="161" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A161" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B161" s="2"/>
+    </row>
     <row r="162" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A162" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A162" s="4"/>
       <c r="B162" s="2"/>
     </row>
     <row r="163" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A163" s="4"/>
+      <c r="A163" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="B163" s="2"/>
     </row>
-    <row r="164" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A164" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B164" s="2"/>
-    </row>
     <row r="165" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A165" s="4"/>
+      <c r="A165" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="B165" s="2"/>
     </row>
     <row r="166" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A166" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="A166" s="1"/>
       <c r="B166" s="2"/>
     </row>
-    <row r="168" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A168" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B168" s="2"/>
-    </row>
-    <row r="169" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A169" s="1"/>
-      <c r="B169" s="2"/>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B167" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A169" s="6"/>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B170" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="A170" s="6"/>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A171" s="6"/>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A172" s="6"/>
+      <c r="A172" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A173" s="6"/>
+      <c r="A173" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A174" s="6"/>
+      <c r="A174" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A175" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="A175" s="6"/>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A177" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A178" s="6"/>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A179" s="6" t="s">
         <v>14</v>
       </c>
+    </row>
+    <row r="177" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A177" s="1"/>
+      <c r="B177" s="2"/>
+    </row>
+    <row r="178" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A178" s="1"/>
+      <c r="B178" s="2"/>
+    </row>
+    <row r="179" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A179" s="1"/>
+      <c r="B179" s="2"/>
     </row>
     <row r="180" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A180" s="1"/>
@@ -1571,68 +1562,56 @@
       <c r="A182" s="1"/>
       <c r="B182" s="2"/>
     </row>
-    <row r="183" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A183" s="1"/>
-      <c r="B183" s="2"/>
-    </row>
     <row r="184" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A184" s="1"/>
+      <c r="A184" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="B184" s="2"/>
     </row>
-    <row r="185" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A185" s="1"/>
-      <c r="B185" s="2"/>
-    </row>
-    <row r="187" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A187" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B187" s="2"/>
-    </row>
-    <row r="189" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A189" s="4" t="s">
+    <row r="186" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A186" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B189" s="2"/>
-    </row>
-    <row r="191" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A191" s="4" t="s">
+      <c r="B186" s="2"/>
+    </row>
+    <row r="188" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A188" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B191" s="2"/>
-    </row>
-    <row r="193" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A193" s="4" t="s">
+      <c r="B188" s="2"/>
+    </row>
+    <row r="190" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A190" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B193" s="2"/>
+      <c r="B190" s="2"/>
+    </row>
+    <row r="192" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A192" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A194" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B194" s="2"/>
     </row>
     <row r="195" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A195" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A197" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B197" s="2"/>
+      <c r="A195" s="1"/>
+      <c r="B195" s="2"/>
+    </row>
+    <row r="196" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A196" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B196" s="2"/>
     </row>
     <row r="198" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A198" s="1"/>
+      <c r="A198" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="B198" s="2"/>
-    </row>
-    <row r="199" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A199" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B199" s="2"/>
-    </row>
-    <row r="201" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A201" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B201" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adds extra validation to vacation
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="787" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81F7A2FA-4174-4B01-99CE-2172DB8DD7F2}"/>
+  <xr:revisionPtr revIDLastSave="831" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{876C9665-2050-439D-BED0-6CA1BB97DC91}"/>
   <bookViews>
     <workbookView xWindow="9510" yWindow="-70" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
   <si>
     <t>…..</t>
   </si>
@@ -315,6 +315,12 @@
   </si>
   <si>
     <t>Arbeitszeiten aufs Monat bezogen</t>
+  </si>
+  <si>
+    <t>Vacation Enddatum validieren</t>
+  </si>
+  <si>
+    <t>Vacation Startdate filtern nach User</t>
   </si>
 </sst>
 </file>
@@ -402,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -426,6 +432,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -449,13 +457,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>201</xdr:row>
+      <xdr:row>205</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>215</xdr:row>
+      <xdr:row>219</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -510,13 +518,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
-      <xdr:row>166</xdr:row>
+      <xdr:row>170</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3295127</xdr:colOff>
-      <xdr:row>186</xdr:row>
+      <xdr:row>190</xdr:row>
       <xdr:rowOff>18741</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -554,13 +562,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>87</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1810160</xdr:colOff>
-      <xdr:row>97</xdr:row>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>193411</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -609,13 +617,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2599763</xdr:colOff>
-      <xdr:row>87</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>158071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4461042</xdr:colOff>
-      <xdr:row>100</xdr:row>
+      <xdr:row>101</xdr:row>
       <xdr:rowOff>79844</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -930,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G232"/>
+  <dimension ref="A1:G236"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -967,76 +975,75 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
+      <c r="A6" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="4"/>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
       <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="4"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>84</v>
-      </c>
+      <c r="A17" s="4"/>
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
       <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="4"/>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
       <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1048,41 +1055,41 @@
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="4"/>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>75</v>
-      </c>
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
       <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="4"/>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
       <c r="B29" s="2"/>
     </row>
     <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1090,72 +1097,72 @@
       <c r="B30" s="2"/>
     </row>
     <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="4"/>
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
       <c r="B32" s="2"/>
     </row>
     <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
+      <c r="A33" s="4"/>
       <c r="B33" s="2"/>
     </row>
     <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="1"/>
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
       <c r="B35" s="2"/>
     </row>
     <row r="36" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="1"/>
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="2"/>
-    </row>
-    <row r="37" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
       <c r="B37" s="2"/>
     </row>
     <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="1"/>
+      <c r="B38" s="2"/>
+    </row>
+    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="2"/>
-    </row>
-    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="1"/>
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="1:3" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="12" t="s">
+    <row r="40" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="1:3" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B40" s="2"/>
-    </row>
-    <row r="41" spans="1:3" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="1"/>
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="14" t="s">
+    <row r="42" spans="1:3" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="2"/>
+    </row>
+    <row r="43" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="B42" s="2"/>
-    </row>
-    <row r="43" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B43" s="1"/>
-      <c r="C43" s="2"/>
-    </row>
-    <row r="45" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B45" s="1"/>
-      <c r="C45" s="2"/>
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B44" s="1"/>
+      <c r="C44" s="2"/>
     </row>
     <row r="46" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B46" s="1"/>
@@ -1178,15 +1185,15 @@
       <c r="C50" s="2"/>
     </row>
     <row r="51" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="11" t="s">
-        <v>59</v>
-      </c>
       <c r="B51" s="1"/>
       <c r="C51" s="2"/>
     </row>
     <row r="52" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="1"/>
-      <c r="B52" s="2"/>
+      <c r="A52" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" s="1"/>
+      <c r="C52" s="2"/>
     </row>
     <row r="53" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
@@ -1205,147 +1212,147 @@
       <c r="B56" s="2"/>
     </row>
     <row r="57" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="9" t="s">
+      <c r="A57" s="1"/>
+      <c r="B57" s="2"/>
+    </row>
+    <row r="58" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B57" s="2"/>
-    </row>
-    <row r="58" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="1"/>
+      <c r="B58" s="2"/>
     </row>
     <row r="59" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="1"/>
+    </row>
+    <row r="60" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="1"/>
-      <c r="B60" s="2"/>
-    </row>
     <row r="61" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="1"/>
+      <c r="B61" s="2"/>
+    </row>
+    <row r="62" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B61" s="2"/>
-    </row>
-    <row r="62" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="1"/>
-      <c r="B62" s="9"/>
+      <c r="B62" s="2"/>
     </row>
     <row r="63" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="11" t="s">
+      <c r="A63" s="1"/>
+      <c r="B63" s="9"/>
+    </row>
+    <row r="64" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B63" s="2"/>
-    </row>
-    <row r="64" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="1"/>
       <c r="B64" s="2"/>
     </row>
     <row r="65" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="4" t="s">
-        <v>47</v>
-      </c>
+      <c r="A65" s="1"/>
       <c r="B65" s="2"/>
     </row>
     <row r="66" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B66" s="2"/>
+    </row>
+    <row r="67" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B66" s="2"/>
-    </row>
-    <row r="67" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="11" t="s">
+      <c r="B67" s="2"/>
+    </row>
+    <row r="68" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B67" s="2"/>
-    </row>
-    <row r="68" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A68" s="1"/>
       <c r="B68" s="2"/>
     </row>
     <row r="69" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="4" t="s">
+      <c r="A69" s="1"/>
+      <c r="B69" s="2"/>
+    </row>
+    <row r="70" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B69" s="2"/>
-    </row>
-    <row r="70" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="1"/>
       <c r="B70" s="2"/>
     </row>
     <row r="71" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+      <c r="A71" s="1"/>
+      <c r="B71" s="2"/>
+    </row>
+    <row r="72" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>45</v>
       </c>
-      <c r="B71" s="2"/>
-    </row>
-    <row r="74" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="4" t="s">
+      <c r="B72" s="2"/>
+    </row>
+    <row r="75" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="1"/>
-      <c r="B75" s="2"/>
-    </row>
     <row r="76" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="4" t="s">
+      <c r="A76" s="1"/>
+      <c r="B76" s="2"/>
+    </row>
+    <row r="77" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B76" s="2"/>
-    </row>
-    <row r="77" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="1"/>
       <c r="B77" s="2"/>
     </row>
     <row r="78" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="1"/>
       <c r="B78" s="2"/>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="10" t="s">
+    <row r="79" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B79" s="2"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A81" s="10"/>
-    </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
+      <c r="A82" s="10"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="1"/>
-      <c r="B83" s="2"/>
-    </row>
     <row r="84" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A84" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="A84" s="1"/>
       <c r="B84" s="2"/>
     </row>
     <row r="85" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B85" s="2"/>
+    </row>
+    <row r="86" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A86" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B85" s="2"/>
-      <c r="G85" t="s">
+      <c r="B86" s="2"/>
+      <c r="G86" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="8" t="s">
+    <row r="87" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A87" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B86" s="2"/>
-    </row>
-    <row r="87" spans="1:7" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A87" s="1"/>
-    </row>
-    <row r="88" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B87" s="2"/>
+    </row>
+    <row r="88" spans="1:7" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
-      <c r="B88" s="2"/>
     </row>
     <row r="89" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
@@ -1400,202 +1407,203 @@
       <c r="B101" s="2"/>
     </row>
     <row r="102" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A102" s="4" t="s">
+      <c r="A102" s="1"/>
+      <c r="B102" s="2"/>
+    </row>
+    <row r="103" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A103" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B102" s="2"/>
-    </row>
-    <row r="103" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A103" s="1"/>
       <c r="B103" s="2"/>
     </row>
     <row r="104" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A104" s="4" t="s">
+      <c r="A104" s="1"/>
+      <c r="B104" s="2"/>
+    </row>
+    <row r="105" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A105" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B104" s="2"/>
-    </row>
-    <row r="105" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A105" s="1"/>
       <c r="B105" s="2"/>
     </row>
     <row r="106" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A106" s="4" t="s">
+      <c r="A106" s="1"/>
+      <c r="B106" s="2"/>
+    </row>
+    <row r="107" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A107" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B106" s="2"/>
-    </row>
-    <row r="107" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A107" s="4"/>
       <c r="B107" s="2"/>
     </row>
     <row r="108" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A108" s="9"/>
+      <c r="A108" s="4"/>
       <c r="B108" s="2"/>
     </row>
     <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A109" s="9"/>
       <c r="B109" s="2"/>
     </row>
-    <row r="112" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A112" s="4"/>
+    <row r="110" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B110" s="2"/>
     </row>
     <row r="113" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" s="4"/>
-      <c r="B113" s="2"/>
     </row>
     <row r="114" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A114" s="3" t="s">
+      <c r="A114" s="4"/>
+      <c r="B114" s="2"/>
+    </row>
+    <row r="115" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A115" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B114" s="2"/>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A115" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="B115" s="2"/>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" s="3"/>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="3"/>
     </row>
-    <row r="121" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A121" s="13" t="s">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" s="3"/>
+    </row>
+    <row r="122" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A122" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="38.4" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A122" s="13"/>
-    </row>
-    <row r="123" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="123" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A123" s="13"/>
     </row>
-    <row r="124" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A125" s="13"/>
-    </row>
-    <row r="126" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A126" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.7">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="4"/>
+    </row>
+    <row r="126" spans="1:2" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A126" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A127" s="13"/>
     </row>
     <row r="128" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A128" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A129" s="13"/>
+    </row>
+    <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A130" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A131" s="13"/>
+    </row>
+    <row r="132" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A132" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="4" t="s">
+    <row r="133" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A130" s="4"/>
-    </row>
-    <row r="131" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A131" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A132" s="13"/>
-    </row>
-    <row r="133" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A133" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B133" s="2"/>
     </row>
     <row r="134" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A134" s="4"/>
-      <c r="B134" s="2"/>
     </row>
     <row r="135" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A135" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B135" s="2"/>
-    </row>
-    <row r="136" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A136" s="5"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A136" s="13"/>
     </row>
     <row r="137" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A137" s="4" t="s">
-        <v>61</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B137" s="2"/>
+    </row>
+    <row r="138" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A138" s="4"/>
+      <c r="B138" s="2"/>
     </row>
     <row r="139" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A139" s="4" t="s">
-        <v>60</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="B139" s="2"/>
     </row>
     <row r="140" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A140" s="5"/>
     </row>
     <row r="141" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A141" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B141" s="2"/>
-    </row>
-    <row r="142" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A142" s="4"/>
-      <c r="B142" s="2"/>
+        <v>61</v>
+      </c>
     </row>
     <row r="143" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A143" t="s">
-        <v>44</v>
-      </c>
-      <c r="B143" s="2"/>
+      <c r="A143" s="4" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="144" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A144" s="5"/>
     </row>
     <row r="145" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A145" s="4" t="s">
-        <v>49</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B145" s="2"/>
     </row>
     <row r="146" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A146" s="4"/>
+      <c r="B146" s="2"/>
     </row>
     <row r="147" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A147" s="4" t="s">
-        <v>62</v>
-      </c>
+      <c r="A147" t="s">
+        <v>44</v>
+      </c>
+      <c r="B147" s="2"/>
     </row>
     <row r="148" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A148" s="5"/>
     </row>
     <row r="149" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A149" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A150" s="5"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A150" s="4"/>
     </row>
     <row r="151" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A151" s="4" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="21" x14ac:dyDescent="0.4">
@@ -1603,157 +1611,157 @@
     </row>
     <row r="153" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A153" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A154" s="4"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A154" s="5"/>
     </row>
     <row r="155" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A155" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B155" s="2"/>
+        <v>29</v>
+      </c>
     </row>
     <row r="156" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A156" s="5"/>
     </row>
     <row r="157" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A157" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B157" s="2"/>
-    </row>
-    <row r="158" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A158" s="5"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A158" s="4"/>
     </row>
     <row r="159" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A159" s="4" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B159" s="2"/>
     </row>
-    <row r="160" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A160" s="4"/>
-      <c r="B160" s="2"/>
+    <row r="160" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A160" s="5"/>
     </row>
     <row r="161" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
-        <v>27</v>
+      <c r="A161" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="B161" s="2"/>
+    </row>
+    <row r="162" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A162" s="5"/>
     </row>
     <row r="163" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A163" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B163" s="2"/>
+    </row>
+    <row r="164" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A164" s="4"/>
+      <c r="B164" s="2"/>
+    </row>
+    <row r="165" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>27</v>
+      </c>
+      <c r="B165" s="2"/>
+    </row>
+    <row r="167" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A167" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B163" s="2"/>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A165" t="s">
+      <c r="B167" s="2"/>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A189" t="s">
+    <row r="193" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
         <v>4</v>
       </c>
-      <c r="B189" s="2"/>
-    </row>
-    <row r="191" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A191" t="s">
+      <c r="B193" s="2"/>
+    </row>
+    <row r="195" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
         <v>5</v>
       </c>
-      <c r="B191" s="2"/>
-    </row>
-    <row r="193" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A193" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B193" s="2"/>
-    </row>
-    <row r="194" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A194" s="4"/>
-      <c r="B194" s="2"/>
-    </row>
-    <row r="195" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A195" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="B195" s="2"/>
-    </row>
-    <row r="196" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A196" s="4"/>
-      <c r="B196" s="2"/>
     </row>
     <row r="197" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A197" s="4" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B197" s="2"/>
+    </row>
+    <row r="198" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A198" s="4"/>
+      <c r="B198" s="2"/>
     </row>
     <row r="199" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A199" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B199" s="2"/>
+    </row>
+    <row r="200" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A200" s="4"/>
+      <c r="B200" s="2"/>
+    </row>
+    <row r="201" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A201" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B201" s="2"/>
+    </row>
+    <row r="203" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A203" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B199" s="2"/>
-    </row>
-    <row r="200" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A200" s="1"/>
-      <c r="B200" s="2"/>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B201" s="6" t="s">
+      <c r="B203" s="2"/>
+    </row>
+    <row r="204" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A204" s="1"/>
+      <c r="B204" s="2"/>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B205" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A203" s="6"/>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A204" s="6"/>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A205" s="6"/>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A206" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A207" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="A207" s="6"/>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A208" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A208" s="6"/>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" s="6"/>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A211" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A212" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A213" s="6"/>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A214" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="211" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A211" s="1"/>
-      <c r="B211" s="2"/>
-    </row>
-    <row r="212" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A212" s="1"/>
-      <c r="B212" s="2"/>
-    </row>
-    <row r="213" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A213" s="1"/>
-      <c r="B213" s="2"/>
-    </row>
-    <row r="214" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A214" s="1"/>
-      <c r="B214" s="2"/>
     </row>
     <row r="215" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A215" s="1"/>
@@ -1763,56 +1771,72 @@
       <c r="A216" s="1"/>
       <c r="B216" s="2"/>
     </row>
+    <row r="217" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A217" s="1"/>
+      <c r="B217" s="2"/>
+    </row>
     <row r="218" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A218" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="A218" s="1"/>
       <c r="B218" s="2"/>
     </row>
+    <row r="219" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A219" s="1"/>
+      <c r="B219" s="2"/>
+    </row>
     <row r="220" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A220" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="A220" s="1"/>
       <c r="B220" s="2"/>
     </row>
     <row r="222" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A222" s="4" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B222" s="2"/>
     </row>
     <row r="224" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A224" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B224" s="2"/>
     </row>
     <row r="226" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A226" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="A226" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B226" s="2"/>
     </row>
     <row r="228" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A228" s="4" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B228" s="2"/>
     </row>
-    <row r="229" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A229" s="1"/>
-      <c r="B229" s="2"/>
-    </row>
     <row r="230" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A230" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B230" s="2"/>
+      <c r="A230" s="9" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="232" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A232" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B232" s="2"/>
+    </row>
+    <row r="233" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A233" s="1"/>
+      <c r="B233" s="2"/>
+    </row>
+    <row r="234" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A234" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B234" s="2"/>
+    </row>
+    <row r="236" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A236" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B232" s="2"/>
+      <c r="B236" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Shows remaining vacation time
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="831" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{876C9665-2050-439D-BED0-6CA1BB97DC91}"/>
+  <xr:revisionPtr revIDLastSave="883" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC9CAA12-4A2E-4A3C-B13F-DD27FA7089A2}"/>
   <bookViews>
     <workbookView xWindow="9510" yWindow="-70" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="93">
   <si>
     <t>…..</t>
   </si>
@@ -317,10 +317,25 @@
     <t>Arbeitszeiten aufs Monat bezogen</t>
   </si>
   <si>
-    <t>Vacation Enddatum validieren</t>
-  </si>
-  <si>
     <t>Vacation Startdate filtern nach User</t>
+  </si>
+  <si>
+    <t>Start und Enddatum in Zeitraum</t>
+  </si>
+  <si>
+    <t>Admin: create employee - Vorauswahl Felder Employee und Manager</t>
+  </si>
+  <si>
+    <t>Manager: Manager und Admin Felder deaktivieren.</t>
+  </si>
+  <si>
+    <t>Alles auf Exekutor Service Provider umstellen</t>
+  </si>
+  <si>
+    <t>Accepted Requeszs löschen dann man flow durchprobieren.</t>
+  </si>
+  <si>
+    <t>Rest Holiday accepted holidays - auch prüfen bei acceptor + DB  mit Restvacaion anzeigen + bei Vacation nehmen weiter + bei Manager und Admin</t>
   </si>
 </sst>
 </file>
@@ -408,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -432,8 +447,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -457,13 +470,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>205</xdr:row>
+      <xdr:row>219</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>219</xdr:row>
+      <xdr:row>233</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -518,14 +531,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
-      <xdr:row>170</xdr:row>
+      <xdr:row>186</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>3295127</xdr:colOff>
-      <xdr:row>190</xdr:row>
-      <xdr:rowOff>18741</xdr:rowOff>
+      <xdr:colOff>3295762</xdr:colOff>
+      <xdr:row>206</xdr:row>
+      <xdr:rowOff>19376</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -562,13 +575,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>88</xdr:row>
+      <xdr:row>96</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1810160</xdr:colOff>
-      <xdr:row>98</xdr:row>
+      <xdr:colOff>1809525</xdr:colOff>
+      <xdr:row>106</xdr:row>
       <xdr:rowOff>193411</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -617,13 +630,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2599763</xdr:colOff>
-      <xdr:row>88</xdr:row>
+      <xdr:row>94</xdr:row>
       <xdr:rowOff>158071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4461042</xdr:colOff>
-      <xdr:row>101</xdr:row>
+      <xdr:row>107</xdr:row>
       <xdr:rowOff>79844</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -938,10 +951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G236"/>
+  <dimension ref="A1:G252"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A131" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A132" sqref="A132:XFD134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -974,29 +987,13 @@
       <c r="A5" s="4"/>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8" s="2"/>
-    </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>80</v>
+      <c r="A10" t="s">
+        <v>79</v>
       </c>
       <c r="B10" s="2"/>
     </row>
@@ -1006,7 +1003,7 @@
     </row>
     <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B12" s="2"/>
     </row>
@@ -1016,16 +1013,17 @@
     </row>
     <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
       <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B16" s="2"/>
     </row>
@@ -1034,6 +1032,9 @@
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1042,7 +1043,7 @@
     </row>
     <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B20" s="2"/>
     </row>
@@ -1051,45 +1052,39 @@
       <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
+      <c r="A22" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>75</v>
-      </c>
+      <c r="A25" s="4"/>
       <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>78</v>
-      </c>
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>76</v>
-      </c>
+      <c r="A27" s="4"/>
       <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
+      <c r="A28" s="4" t="s">
+        <v>85</v>
+      </c>
       <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>77</v>
-      </c>
+      <c r="A29" s="4"/>
       <c r="B29" s="2"/>
     </row>
     <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1102,182 +1097,184 @@
     </row>
     <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="4"/>
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="4"/>
+      <c r="B38" s="2"/>
+    </row>
+    <row r="39" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="4"/>
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" s="2"/>
-    </row>
-    <row r="36" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
-      <c r="B36" s="2"/>
-    </row>
-    <row r="37" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
-      <c r="B38" s="2"/>
-    </row>
-    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="1:3" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="12" t="s">
-        <v>57</v>
-      </c>
+    <row r="41" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="4"/>
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="1:3" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="14" t="s">
-        <v>72</v>
+    <row r="43" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B44" s="1"/>
-      <c r="C44" s="2"/>
-    </row>
-    <row r="46" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B46" s="1"/>
-      <c r="C46" s="2"/>
-    </row>
-    <row r="47" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B47" s="1"/>
-      <c r="C47" s="2"/>
-    </row>
-    <row r="48" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B48" s="1"/>
-      <c r="C48" s="2"/>
-    </row>
-    <row r="49" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B49" s="1"/>
-      <c r="C49" s="2"/>
+    <row r="44" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45" s="2"/>
+    </row>
+    <row r="46" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="1"/>
+      <c r="B46" s="2"/>
+    </row>
+    <row r="47" spans="1:2" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48" spans="1:2" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
+      <c r="B48" s="2"/>
+    </row>
+    <row r="49" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49" s="2"/>
     </row>
     <row r="50" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B51" s="1"/>
-      <c r="C51" s="2"/>
+    <row r="51" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="14" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="52" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="11" t="s">
-        <v>59</v>
-      </c>
       <c r="B52" s="1"/>
       <c r="C52" s="2"/>
     </row>
     <row r="53" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="1"/>
-      <c r="B53" s="2"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="2"/>
     </row>
     <row r="54" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="1"/>
-      <c r="B54" s="2"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="2"/>
     </row>
     <row r="55" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="1"/>
-      <c r="B55" s="2"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="2"/>
     </row>
     <row r="56" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="1"/>
-      <c r="B56" s="2"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="2"/>
     </row>
     <row r="57" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="1"/>
-      <c r="B57" s="2"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="2"/>
     </row>
     <row r="58" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B58" s="2"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="2"/>
     </row>
     <row r="59" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="1"/>
+      <c r="B59" s="2"/>
     </row>
     <row r="60" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="s">
-        <v>36</v>
-      </c>
+      <c r="A60" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" s="2"/>
     </row>
     <row r="61" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
     </row>
     <row r="62" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="4" t="s">
-        <v>52</v>
-      </c>
+      <c r="A62" s="1"/>
       <c r="B62" s="2"/>
     </row>
     <row r="63" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
-      <c r="B63" s="9"/>
+      <c r="B63" s="2"/>
     </row>
     <row r="64" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="11" t="s">
-        <v>63</v>
-      </c>
+      <c r="A64" s="1"/>
       <c r="B64" s="2"/>
     </row>
     <row r="65" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
-      <c r="B65" s="2"/>
     </row>
     <row r="66" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B66" s="2"/>
+      <c r="A66" s="9" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="67" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="4" t="s">
-        <v>64</v>
-      </c>
+      <c r="A67" s="1"/>
       <c r="B67" s="2"/>
     </row>
     <row r="68" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A68" s="11" t="s">
-        <v>63</v>
+      <c r="A68" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="B68" s="2"/>
     </row>
     <row r="69" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
-      <c r="B69" s="2"/>
+      <c r="B69" s="9"/>
     </row>
     <row r="70" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="B70" s="2"/>
     </row>
@@ -1286,45 +1283,59 @@
       <c r="B71" s="2"/>
     </row>
     <row r="72" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>45</v>
+      <c r="A72" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="B72" s="2"/>
+    </row>
+    <row r="73" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="1"/>
+      <c r="B73" s="2"/>
+    </row>
+    <row r="74" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B74" s="2"/>
     </row>
     <row r="75" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B75" s="2"/>
+    </row>
+    <row r="76" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B76" s="2"/>
+    </row>
+    <row r="77" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="1"/>
+      <c r="B77" s="2"/>
+    </row>
+    <row r="78" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B78" s="2"/>
+    </row>
+    <row r="79" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="1"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B82" s="2"/>
+    </row>
+    <row r="83" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="1"/>
-      <c r="B76" s="2"/>
-    </row>
-    <row r="77" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B77" s="2"/>
-    </row>
-    <row r="78" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="1"/>
-      <c r="B78" s="2"/>
-    </row>
-    <row r="79" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B79" s="2"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A81" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A82" s="10"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>46</v>
-      </c>
+      <c r="B83" s="2"/>
     </row>
     <row r="84" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
@@ -1332,54 +1343,50 @@
     </row>
     <row r="85" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B85" s="2"/>
     </row>
     <row r="86" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B86" s="2"/>
-      <c r="G86" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A87" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B87" s="2"/>
-    </row>
-    <row r="88" spans="1:7" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A88" s="1"/>
-    </row>
-    <row r="89" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A89" s="1"/>
-      <c r="B89" s="2"/>
+      <c r="A86" s="1"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A89" s="10" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="90" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A90" s="1"/>
+      <c r="A90" s="10"/>
       <c r="B90" s="2"/>
     </row>
     <row r="91" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A91" s="1"/>
+      <c r="A91" t="s">
+        <v>46</v>
+      </c>
       <c r="B91" s="2"/>
     </row>
     <row r="92" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
+      <c r="G92" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="93" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A93" s="1"/>
+      <c r="A93" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="B93" s="2"/>
     </row>
-    <row r="94" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A94" s="1"/>
-      <c r="B94" s="2"/>
+    <row r="94" spans="1:7" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A94" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="95" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A95" s="1"/>
+      <c r="A95" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="B95" s="2"/>
     </row>
     <row r="96" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1411,9 +1418,7 @@
       <c r="B102" s="2"/>
     </row>
     <row r="103" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A103" s="4" t="s">
-        <v>28</v>
-      </c>
+      <c r="A103" s="1"/>
       <c r="B103" s="2"/>
     </row>
     <row r="104" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1421,9 +1426,7 @@
       <c r="B104" s="2"/>
     </row>
     <row r="105" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A105" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="A105" s="1"/>
       <c r="B105" s="2"/>
     </row>
     <row r="106" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1431,195 +1434,198 @@
       <c r="B106" s="2"/>
     </row>
     <row r="107" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A107" s="4" t="s">
+      <c r="A107" s="1"/>
+      <c r="B107" s="2"/>
+    </row>
+    <row r="108" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A108" s="1"/>
+      <c r="B108" s="2"/>
+    </row>
+    <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A109" s="1"/>
+      <c r="B109" s="2"/>
+    </row>
+    <row r="110" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A110" s="1"/>
+      <c r="B110" s="2"/>
+    </row>
+    <row r="111" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A111" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B111" s="2"/>
+    </row>
+    <row r="112" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A112" s="1"/>
+      <c r="B112" s="2"/>
+    </row>
+    <row r="113" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A113" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B113" s="2"/>
+    </row>
+    <row r="114" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A114" s="1"/>
+      <c r="B114" s="2"/>
+    </row>
+    <row r="115" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A115" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B107" s="2"/>
-    </row>
-    <row r="108" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A108" s="4"/>
-      <c r="B108" s="2"/>
-    </row>
-    <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A109" s="9"/>
-      <c r="B109" s="2"/>
-    </row>
-    <row r="110" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B110" s="2"/>
-    </row>
-    <row r="113" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A113" s="4"/>
-    </row>
-    <row r="114" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A114" s="4"/>
-      <c r="B114" s="2"/>
-    </row>
-    <row r="115" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A115" s="3" t="s">
+      <c r="B115" s="2"/>
+    </row>
+    <row r="116" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A116" s="4"/>
+      <c r="B116" s="2"/>
+    </row>
+    <row r="117" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A117" s="9"/>
+    </row>
+    <row r="120" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B120" s="2"/>
+    </row>
+    <row r="121" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A121" s="4"/>
+      <c r="B121" s="2"/>
+    </row>
+    <row r="122" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A122" s="4"/>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B115" s="2"/>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116" s="3" t="s">
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" s="3" t="s">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" s="3" t="s">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" s="3"/>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120" s="3"/>
-    </row>
-    <row r="122" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A122" s="13" t="s">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" s="3"/>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" s="3"/>
+    </row>
+    <row r="130" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A130" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A123" s="13"/>
-    </row>
-    <row r="124" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="4"/>
-    </row>
-    <row r="126" spans="1:2" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A126" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A127" s="13"/>
-    </row>
-    <row r="128" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A128" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A129" s="13"/>
-    </row>
-    <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A130" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="131" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A131" s="13"/>
     </row>
     <row r="132" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A132" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B132" s="2"/>
+    </row>
+    <row r="133" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A133" s="4"/>
+      <c r="B133" s="2"/>
+    </row>
+    <row r="134" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A134" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B134" s="2"/>
+    </row>
+    <row r="135" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A135" s="13"/>
+    </row>
+    <row r="136" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A136" s="13"/>
+    </row>
+    <row r="137" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A137" s="13"/>
+    </row>
+    <row r="138" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A139" s="13"/>
+    </row>
+    <row r="140" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A140" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A141" s="4"/>
+    </row>
+    <row r="142" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A142" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A143" s="13"/>
+    </row>
+    <row r="144" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A144" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A145" s="13"/>
+    </row>
+    <row r="146" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A146" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A147" s="13"/>
+    </row>
+    <row r="148" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A148" s="4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A134" s="4"/>
-    </row>
-    <row r="135" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A135" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A136" s="13"/>
-    </row>
-    <row r="137" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A137" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B137" s="2"/>
-    </row>
-    <row r="138" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A138" s="4"/>
-      <c r="B138" s="2"/>
-    </row>
-    <row r="139" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A139" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B139" s="2"/>
-    </row>
-    <row r="140" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A140" s="5"/>
-    </row>
-    <row r="141" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A141" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A143" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A144" s="5"/>
-    </row>
-    <row r="145" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A145" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B145" s="2"/>
-    </row>
-    <row r="146" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A146" s="4"/>
-      <c r="B146" s="2"/>
-    </row>
-    <row r="147" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
-        <v>44</v>
-      </c>
-      <c r="B147" s="2"/>
-    </row>
-    <row r="148" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A148" s="5"/>
     </row>
     <row r="149" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A149" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="4"/>
     </row>
     <row r="151" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A151" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A152" s="5"/>
+        <v>71</v>
+      </c>
+      <c r="B151" s="2"/>
+    </row>
+    <row r="152" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A152" s="13"/>
+      <c r="B152" s="2"/>
     </row>
     <row r="153" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A153" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A154" s="5"/>
+        <v>65</v>
+      </c>
+      <c r="B153" s="2"/>
+    </row>
+    <row r="154" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A154" s="4"/>
     </row>
     <row r="155" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A155" s="4" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="21" x14ac:dyDescent="0.4">
@@ -1627,199 +1633,218 @@
     </row>
     <row r="157" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A157" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A158" s="4"/>
+        <v>61</v>
+      </c>
     </row>
     <row r="159" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A159" s="4" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="B159" s="2"/>
     </row>
     <row r="160" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A160" s="5"/>
+      <c r="B160" s="2"/>
     </row>
     <row r="161" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A161" s="4" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B161" s="2"/>
     </row>
-    <row r="162" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A162" s="5"/>
-    </row>
-    <row r="163" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A163" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B163" s="2"/>
-    </row>
-    <row r="164" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A164" s="4"/>
-      <c r="B164" s="2"/>
+    <row r="162" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A162" s="4"/>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A164" s="5"/>
     </row>
     <row r="165" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A165" t="s">
-        <v>27</v>
-      </c>
-      <c r="B165" s="2"/>
+      <c r="A165" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A166" s="4"/>
     </row>
     <row r="167" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A167" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A168" s="5"/>
+    </row>
+    <row r="169" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A169" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A170" s="5"/>
+    </row>
+    <row r="171" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A171" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A172" s="5"/>
+    </row>
+    <row r="173" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A173" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B173" s="2"/>
+    </row>
+    <row r="174" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A174" s="4"/>
+    </row>
+    <row r="175" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A175" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B175" s="2"/>
+    </row>
+    <row r="176" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A176" s="5"/>
+    </row>
+    <row r="177" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A177" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B177" s="2"/>
+    </row>
+    <row r="178" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A178" s="5"/>
+      <c r="B178" s="2"/>
+    </row>
+    <row r="179" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A179" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B179" s="2"/>
+    </row>
+    <row r="180" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A180" s="4"/>
+    </row>
+    <row r="181" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>27</v>
+      </c>
+      <c r="B181" s="2"/>
+    </row>
+    <row r="183" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A183" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B167" s="2"/>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A169" t="s">
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A193" t="s">
+    <row r="207" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B207" s="2"/>
+    </row>
+    <row r="209" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
         <v>4</v>
       </c>
-      <c r="B193" s="2"/>
-    </row>
-    <row r="195" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A195" t="s">
+      <c r="B209" s="2"/>
+    </row>
+    <row r="211" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
         <v>5</v>
       </c>
-      <c r="B195" s="2"/>
-    </row>
-    <row r="197" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A197" s="4" t="s">
+      <c r="B211" s="2"/>
+    </row>
+    <row r="212" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B212" s="2"/>
+    </row>
+    <row r="213" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A213" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B197" s="2"/>
-    </row>
-    <row r="198" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A198" s="4"/>
-      <c r="B198" s="2"/>
-    </row>
-    <row r="199" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A199" s="4" t="s">
+      <c r="B213" s="2"/>
+    </row>
+    <row r="214" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A214" s="4"/>
+      <c r="B214" s="2"/>
+    </row>
+    <row r="215" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A215" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B199" s="2"/>
-    </row>
-    <row r="200" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A200" s="4"/>
-      <c r="B200" s="2"/>
-    </row>
-    <row r="201" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A201" s="4" t="s">
+      <c r="B215" s="2"/>
+    </row>
+    <row r="216" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A216" s="4"/>
+    </row>
+    <row r="217" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A217" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B201" s="2"/>
-    </row>
-    <row r="203" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A203" s="4" t="s">
+      <c r="B217" s="2"/>
+    </row>
+    <row r="218" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B218" s="2"/>
+    </row>
+    <row r="219" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A219" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B203" s="2"/>
-    </row>
-    <row r="204" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A204" s="1"/>
-      <c r="B204" s="2"/>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B205" s="6" t="s">
+      <c r="B219" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A207" s="6"/>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A208" s="6"/>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A209" s="6"/>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A210" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A211" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A212" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A213" s="6"/>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A214" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A215" s="1"/>
-      <c r="B215" s="2"/>
-    </row>
-    <row r="216" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A216" s="1"/>
-      <c r="B216" s="2"/>
-    </row>
-    <row r="217" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A217" s="1"/>
-      <c r="B217" s="2"/>
-    </row>
-    <row r="218" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A218" s="1"/>
-      <c r="B218" s="2"/>
-    </row>
-    <row r="219" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A219" s="1"/>
-      <c r="B219" s="2"/>
     </row>
     <row r="220" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A220" s="1"/>
-      <c r="B220" s="2"/>
-    </row>
-    <row r="222" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A222" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B222" s="2"/>
-    </row>
-    <row r="224" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A224" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B224" s="2"/>
-    </row>
-    <row r="226" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A226" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B226" s="2"/>
-    </row>
-    <row r="228" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A228" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B228" s="2"/>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A223" s="6"/>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A224" s="6"/>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A225" s="6"/>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A226" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A227" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A228" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A229" s="6"/>
+      <c r="B229" s="2"/>
     </row>
     <row r="230" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A230" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="A230" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B230" s="2"/>
+    </row>
+    <row r="231" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A231" s="1"/>
+      <c r="B231" s="2"/>
     </row>
     <row r="232" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A232" s="4" t="s">
-        <v>40</v>
-      </c>
+      <c r="A232" s="1"/>
       <c r="B232" s="2"/>
     </row>
     <row r="233" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1827,16 +1852,67 @@
       <c r="B233" s="2"/>
     </row>
     <row r="234" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A234" s="4" t="s">
+      <c r="A234" s="1"/>
+      <c r="B234" s="2"/>
+    </row>
+    <row r="235" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A235" s="1"/>
+    </row>
+    <row r="236" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A236" s="1"/>
+      <c r="B236" s="2"/>
+    </row>
+    <row r="238" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A238" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B238" s="2"/>
+    </row>
+    <row r="240" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A240" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B240" s="2"/>
+    </row>
+    <row r="242" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A242" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B242" s="2"/>
+    </row>
+    <row r="244" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A244" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A246" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B246" s="2"/>
+    </row>
+    <row r="247" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B247" s="2"/>
+    </row>
+    <row r="248" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A248" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B248" s="2"/>
+    </row>
+    <row r="249" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A249" s="1"/>
+    </row>
+    <row r="250" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A250" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B234" s="2"/>
-    </row>
-    <row r="236" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A236" s="4" t="s">
+      <c r="B250" s="2"/>
+    </row>
+    <row r="252" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A252" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B236" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
sets selection model all employees to null
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -968,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A14:XFD18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
blocks fields for creation and updating
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1005" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE0BFEB2-EEB9-4B9D-8C7B-58625365CDC5}"/>
+  <xr:revisionPtr revIDLastSave="1007" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53908103-7A8F-49F5-8219-036B0187B914}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -403,13 +403,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>211</xdr:row>
+      <xdr:row>212</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>225</xdr:row>
+      <xdr:row>226</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -464,13 +464,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
-      <xdr:row>179</xdr:row>
+      <xdr:row>180</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3295762</xdr:colOff>
-      <xdr:row>199</xdr:row>
+      <xdr:row>200</xdr:row>
       <xdr:rowOff>1595</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -829,10 +829,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G245"/>
+  <dimension ref="A1:G246"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -870,9 +870,6 @@
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1273,385 +1270,387 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="104" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A104" s="12"/>
     </row>
-    <row r="105" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A105" s="12"/>
-    </row>
-    <row r="106" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A106" s="3" t="s">
+    <row r="105" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A106" s="12"/>
+    </row>
+    <row r="107" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A107" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B106" s="2"/>
-    </row>
-    <row r="107" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A107" s="3"/>
       <c r="B107" s="2"/>
     </row>
     <row r="108" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A108" s="3" t="s">
+      <c r="A108" s="3"/>
+      <c r="B108" s="2"/>
+    </row>
+    <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A109" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B108" s="2"/>
-    </row>
-    <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
+      <c r="B109" s="2"/>
+    </row>
+    <row r="110" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
         <v>58</v>
-      </c>
-      <c r="B109" s="2"/>
-    </row>
-    <row r="110" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A110" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="B110" s="2"/>
     </row>
     <row r="111" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B111" s="2"/>
+    </row>
+    <row r="112" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A112" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B111" s="2"/>
-    </row>
-    <row r="112" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A112" s="3"/>
       <c r="B112" s="2"/>
     </row>
     <row r="113" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A113" s="3" t="s">
+      <c r="A113" s="3"/>
+      <c r="B113" s="2"/>
+    </row>
+    <row r="114" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A114" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A114" s="12"/>
-    </row>
-    <row r="115" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A115" s="3" t="s">
+    <row r="115" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A115" s="12"/>
+    </row>
+    <row r="116" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A116" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A116" s="12"/>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
+    <row r="117" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A117" s="12"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A118" s="12"/>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
+    <row r="119" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A119" s="12"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A120" s="12"/>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
+    <row r="121" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A121" s="12"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A122" s="12"/>
-    </row>
-    <row r="123" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A123" s="3" t="s">
+    <row r="123" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A123" s="12"/>
+    </row>
+    <row r="124" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A124" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A124" s="12"/>
-      <c r="B124" s="2"/>
-    </row>
-    <row r="125" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A125" s="3" t="s">
+    <row r="125" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A125" s="12"/>
+      <c r="B125" s="2"/>
+    </row>
+    <row r="126" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A126" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B125" s="2"/>
-    </row>
-    <row r="126" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A126" s="3"/>
       <c r="B126" s="2"/>
     </row>
     <row r="127" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A127" s="3" t="s">
+      <c r="A127" s="3"/>
+      <c r="B127" s="2"/>
+    </row>
+    <row r="128" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A128" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A128" s="12"/>
-    </row>
-    <row r="129" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="129" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A129" s="12"/>
     </row>
-    <row r="130" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="130" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A130" s="12"/>
     </row>
-    <row r="131" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="3" t="s">
+    <row r="131" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A131" s="12"/>
+    </row>
+    <row r="132" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A132" s="12"/>
-    </row>
-    <row r="133" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A133" s="3" t="s">
+    <row r="133" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A133" s="12"/>
+    </row>
+    <row r="134" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A134" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A134" s="3"/>
-    </row>
     <row r="135" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A135" s="3" t="s">
+      <c r="A135" s="3"/>
+    </row>
+    <row r="136" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A136" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A136" s="12"/>
-    </row>
-    <row r="137" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="3" t="s">
+    <row r="137" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A137" s="12"/>
+    </row>
+    <row r="138" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A138" s="12"/>
-    </row>
-    <row r="139" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="3" t="s">
+    <row r="139" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A139" s="12"/>
+    </row>
+    <row r="140" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A140" s="12"/>
-    </row>
-    <row r="141" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A141" s="3" t="s">
+    <row r="141" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A141" s="12"/>
+    </row>
+    <row r="142" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A142" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="3" t="s">
+    <row r="143" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A143" s="3"/>
-      <c r="B143" s="2"/>
-    </row>
     <row r="144" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A144" s="3" t="s">
+      <c r="A144" s="3"/>
+      <c r="B144" s="2"/>
+    </row>
+    <row r="145" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A145" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B144" s="2"/>
-    </row>
-    <row r="145" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A145" s="12"/>
       <c r="B145" s="2"/>
     </row>
-    <row r="146" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A146" s="3" t="s">
+    <row r="146" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A146" s="12"/>
+      <c r="B146" s="2"/>
+    </row>
+    <row r="147" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A147" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A147" s="3"/>
-    </row>
     <row r="148" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A148" s="3" t="s">
+      <c r="A148" s="3"/>
+    </row>
+    <row r="149" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A149" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A149" s="4"/>
-    </row>
-    <row r="150" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A150" s="3" t="s">
+    <row r="150" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A150" s="4"/>
+    </row>
+    <row r="151" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A151" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B151" s="2"/>
-    </row>
     <row r="152" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A152" s="3" t="s">
+      <c r="B152" s="2"/>
+    </row>
+    <row r="153" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A153" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B152" s="2"/>
-    </row>
-    <row r="153" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A153" s="4"/>
       <c r="B153" s="2"/>
     </row>
-    <row r="154" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A154" s="3" t="s">
+    <row r="154" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A154" s="4"/>
+      <c r="B154" s="2"/>
+    </row>
+    <row r="155" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A155" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A155" s="3"/>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A156" t="s">
+    <row r="156" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A156" s="3"/>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A157" s="4"/>
-    </row>
-    <row r="158" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A158" s="3" t="s">
+    <row r="158" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A158" s="4"/>
+    </row>
+    <row r="159" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A159" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A159" s="3"/>
-    </row>
     <row r="160" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A160" s="3" t="s">
+      <c r="A160" s="3"/>
+    </row>
+    <row r="161" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A161" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A161" s="4"/>
-    </row>
-    <row r="162" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A162" s="3" t="s">
+    <row r="162" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A162" s="4"/>
+    </row>
+    <row r="163" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A163" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A163" s="4"/>
-    </row>
-    <row r="164" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A164" s="3" t="s">
+    <row r="164" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A164" s="4"/>
+    </row>
+    <row r="165" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A165" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A165" s="4"/>
-      <c r="B165" s="2"/>
-    </row>
-    <row r="166" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A166" s="3" t="s">
+    <row r="166" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A166" s="4"/>
+      <c r="B166" s="2"/>
+    </row>
+    <row r="167" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A167" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A167" s="3"/>
-      <c r="B167" s="2"/>
-    </row>
     <row r="168" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A168" s="3" t="s">
+      <c r="A168" s="3"/>
+      <c r="B168" s="2"/>
+    </row>
+    <row r="169" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A169" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A169" s="4"/>
-      <c r="B169" s="2"/>
-    </row>
-    <row r="170" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A170" s="3" t="s">
+    <row r="170" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A170" s="4"/>
+      <c r="B170" s="2"/>
+    </row>
+    <row r="171" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A171" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B170" s="2"/>
-    </row>
-    <row r="171" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A171" s="4"/>
       <c r="B171" s="2"/>
     </row>
-    <row r="172" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A172" s="3" t="s">
+    <row r="172" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A172" s="4"/>
+      <c r="B172" s="2"/>
+    </row>
+    <row r="173" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A173" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A173" s="3"/>
-      <c r="B173" s="2"/>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A174" t="s">
+    <row r="174" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A174" s="3"/>
+      <c r="B174" s="2"/>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A176" s="3" t="s">
+    <row r="177" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A177" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A178" t="s">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B199" s="2"/>
-    </row>
-    <row r="201" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B201" s="2"/>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A202" t="s">
+    <row r="200" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B200" s="2"/>
+    </row>
+    <row r="202" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B202" s="2"/>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B203" s="2"/>
-    </row>
     <row r="204" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A204" t="s">
+      <c r="B204" s="2"/>
+    </row>
+    <row r="205" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
         <v>1</v>
       </c>
-      <c r="B204" s="2"/>
-    </row>
-    <row r="205" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B205" s="2"/>
     </row>
     <row r="206" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A206" s="3" t="s">
+      <c r="B206" s="2"/>
+    </row>
+    <row r="207" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A207" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B206" s="2"/>
-    </row>
-    <row r="207" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A207" s="3"/>
       <c r="B207" s="2"/>
     </row>
     <row r="208" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A208" s="3" t="s">
+      <c r="A208" s="3"/>
+      <c r="B208" s="2"/>
+    </row>
+    <row r="209" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A209" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="209" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A209" s="3"/>
-      <c r="B209" s="2"/>
-    </row>
     <row r="210" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A210" s="3" t="s">
+      <c r="A210" s="3"/>
+      <c r="B210" s="2"/>
+    </row>
+    <row r="211" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A211" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B210" s="2"/>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B211" s="5" t="s">
+      <c r="B211" s="2"/>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B212" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="212" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A212" s="3" t="s">
+    <row r="213" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A213" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="213" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A213" s="1"/>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A216" s="5"/>
+    <row r="214" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A214" s="1"/>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" s="5"/>
@@ -1660,33 +1659,32 @@
       <c r="A218" s="5"/>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A219" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="A219" s="5"/>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A221" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="221" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A221" s="5" t="s">
+    <row r="222" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A222" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B221" s="2"/>
-    </row>
-    <row r="222" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A222" s="5"/>
       <c r="B222" s="2"/>
     </row>
     <row r="223" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A223" s="5" t="s">
+      <c r="A223" s="5"/>
+      <c r="B223" s="2"/>
+    </row>
+    <row r="224" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A224" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B223" s="2"/>
-    </row>
-    <row r="224" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A224" s="1"/>
       <c r="B224" s="2"/>
     </row>
     <row r="225" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1699,71 +1697,75 @@
     </row>
     <row r="227" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A227" s="1"/>
+      <c r="B227" s="2"/>
     </row>
     <row r="228" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A228" s="1"/>
-      <c r="B228" s="2"/>
     </row>
     <row r="229" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A229" s="1"/>
+      <c r="B229" s="2"/>
     </row>
     <row r="230" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B230" s="2"/>
+      <c r="A230" s="1"/>
     </row>
     <row r="231" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A231" s="3" t="s">
+      <c r="B231" s="2"/>
+    </row>
+    <row r="232" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A232" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="232" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B232" s="2"/>
-    </row>
     <row r="233" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A233" s="3" t="s">
+      <c r="B233" s="2"/>
+    </row>
+    <row r="234" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A234" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="234" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B234" s="2"/>
-    </row>
     <row r="235" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A235" s="3" t="s">
+      <c r="B235" s="2"/>
+    </row>
+    <row r="236" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A236" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="237" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A237" s="3" t="s">
+    <row r="238" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A238" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="238" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B238" s="2"/>
-    </row>
     <row r="239" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A239" s="8" t="s">
+      <c r="B239" s="2"/>
+    </row>
+    <row r="240" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A240" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B239" s="2"/>
-    </row>
-    <row r="240" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B240" s="2"/>
     </row>
     <row r="241" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A241" s="3" t="s">
+      <c r="B241" s="2"/>
+    </row>
+    <row r="242" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A242" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A242" s="1"/>
-      <c r="B242" s="2"/>
-    </row>
     <row r="243" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A243" s="3" t="s">
+      <c r="A243" s="1"/>
+      <c r="B243" s="2"/>
+    </row>
+    <row r="244" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A244" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="245" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A245" s="3" t="s">
+    <row r="246" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A246" s="3" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
uses hours and vacation on update or create
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1007" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53908103-7A8F-49F5-8219-036B0187B914}"/>
+  <xr:revisionPtr revIDLastSave="1021" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{972890F8-03DD-4E88-BA40-CCEC3E019023}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -120,9 +120,6 @@
     <t>Entity Manager closed from every screen and from login button</t>
   </si>
   <si>
-    <t>Länge von Username und Passwort in der DB gleichziehen</t>
-  </si>
-  <si>
     <t>Wenn ich auf Logout button gehe context clearen</t>
   </si>
   <si>
@@ -279,6 +276,9 @@
   </si>
   <si>
     <t>Mit Deaktivierungen und Aktivierungen machen, dass Managers nur Employees zu Managern befördern können und dass Admins nur Managers zu Admins befördern können</t>
+  </si>
+  <si>
+    <t>Person entity lengths mit lengths in DB vergleichen</t>
   </si>
 </sst>
 </file>
@@ -508,13 +508,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1809525</xdr:colOff>
-      <xdr:row>94</xdr:row>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>193411</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -832,7 +832,7 @@
   <dimension ref="A1:G246"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -853,7 +853,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="2"/>
     </row>
@@ -862,7 +862,7 @@
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6" s="2"/>
     </row>
@@ -870,6 +870,9 @@
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -877,8 +880,8 @@
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>74</v>
+      <c r="A10" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="B10" s="2"/>
     </row>
@@ -888,7 +891,7 @@
     </row>
     <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B12" s="2"/>
     </row>
@@ -897,8 +900,8 @@
       <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>31</v>
+      <c r="A14" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="B14" s="2"/>
     </row>
@@ -906,9 +909,9 @@
       <c r="A15" s="3"/>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>75</v>
+    <row r="16" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A16" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="B16" s="2"/>
     </row>
@@ -918,7 +921,7 @@
     </row>
     <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B18" s="2"/>
     </row>
@@ -926,9 +929,9 @@
       <c r="A19" s="3"/>
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A20" s="4" t="s">
-        <v>78</v>
+    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B20" s="2"/>
     </row>
@@ -937,29 +940,24 @@
       <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="A24" s="3"/>
       <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
       <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
       <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -967,6 +965,7 @@
       <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="3"/>
       <c r="B29" s="2"/>
     </row>
     <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -990,70 +989,70 @@
       <c r="B34" s="2"/>
     </row>
     <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="3"/>
+      <c r="A35" s="1"/>
       <c r="B35" s="2"/>
     </row>
     <row r="36" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="3"/>
+      <c r="A36" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="B36" s="2"/>
     </row>
     <row r="37" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="3"/>
+      <c r="A37" s="1"/>
       <c r="B37" s="2"/>
     </row>
-    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="3"/>
+    <row r="38" spans="1:3" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
     </row>
     <row r="40" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>44</v>
+      <c r="A40" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B40" s="2"/>
     </row>
     <row r="41" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
-      <c r="B41" s="2"/>
-    </row>
-    <row r="42" spans="1:3" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B42" s="2"/>
-    </row>
-    <row r="43" spans="1:3" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="1"/>
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B44" s="2"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="2"/>
+    </row>
+    <row r="44" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="2"/>
     </row>
     <row r="45" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="11" t="s">
-        <v>43</v>
-      </c>
+    <row r="46" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B46" s="1"/>
+      <c r="C46" s="2"/>
     </row>
     <row r="47" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="2"/>
     </row>
-    <row r="48" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="13" t="s">
-        <v>55</v>
-      </c>
+    <row r="48" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
       <c r="C48" s="2"/>
     </row>
@@ -1062,35 +1061,33 @@
       <c r="C49" s="2"/>
     </row>
     <row r="50" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B50" s="1"/>
-      <c r="C50" s="2"/>
+      <c r="B50" s="2"/>
     </row>
     <row r="51" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B51" s="1"/>
-      <c r="C51" s="2"/>
+      <c r="B51" s="2"/>
     </row>
     <row r="52" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B52" s="1"/>
-      <c r="C52" s="2"/>
+      <c r="B52" s="2"/>
     </row>
     <row r="53" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B53" s="1"/>
-      <c r="C53" s="2"/>
+      <c r="A53" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B53" s="2"/>
     </row>
     <row r="54" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="1"/>
       <c r="B54" s="2"/>
     </row>
     <row r="55" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="1"/>
       <c r="B55" s="2"/>
     </row>
     <row r="56" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B56" s="2"/>
+      <c r="A56" s="1"/>
     </row>
     <row r="57" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B57" s="2"/>
+      <c r="A57" s="1"/>
     </row>
     <row r="58" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
@@ -1101,38 +1098,40 @@
       <c r="B59" s="2"/>
     </row>
     <row r="60" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="1"/>
+      <c r="A60" s="3"/>
+      <c r="B60" s="8"/>
     </row>
     <row r="61" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
+      <c r="B61" s="2"/>
     </row>
     <row r="62" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="1"/>
+      <c r="A62" s="3"/>
       <c r="B62" s="2"/>
     </row>
     <row r="63" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
-      <c r="B63" s="2"/>
-    </row>
-    <row r="64" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="3"/>
-      <c r="B64" s="8"/>
-    </row>
-    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="1"/>
-      <c r="B65" s="2"/>
     </row>
     <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="3"/>
+      <c r="A66" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="B66" s="2"/>
     </row>
     <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="1"/>
+      <c r="A67" s="9"/>
+      <c r="B67" s="2"/>
+    </row>
+    <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="9"/>
+      <c r="B68" s="2"/>
+    </row>
+    <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="9"/>
+      <c r="B69" s="2"/>
     </row>
     <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="A70" s="9"/>
       <c r="B70" s="2"/>
     </row>
     <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1144,59 +1143,59 @@
       <c r="B72" s="2"/>
     </row>
     <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="9"/>
+      <c r="A73" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="B73" s="2"/>
     </row>
     <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="9"/>
+      <c r="A74" s="3"/>
       <c r="B74" s="2"/>
     </row>
     <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="9"/>
+      <c r="A75" t="s">
+        <v>33</v>
+      </c>
       <c r="B75" s="2"/>
+      <c r="G75" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="9"/>
+      <c r="A76" s="1"/>
       <c r="B76" s="2"/>
     </row>
-    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B77" s="2"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="3"/>
+      <c r="A78" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="B78" s="2"/>
     </row>
     <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>34</v>
+      <c r="A79" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="B79" s="2"/>
-      <c r="G79" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
     </row>
-    <row r="81" spans="1:2" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A81" s="3" t="s">
-        <v>15</v>
-      </c>
+    <row r="81" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="1"/>
+      <c r="B81" s="2"/>
     </row>
     <row r="82" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="A82" s="1"/>
       <c r="B82" s="2"/>
     </row>
     <row r="83" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="7" t="s">
-        <v>16</v>
-      </c>
+      <c r="A83" s="1"/>
       <c r="B83" s="2"/>
     </row>
     <row r="84" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1244,38 +1243,34 @@
       <c r="B94" s="2"/>
     </row>
     <row r="95" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A95" s="1"/>
-      <c r="B95" s="2"/>
+      <c r="A95" s="3"/>
     </row>
     <row r="96" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A96" s="1"/>
-      <c r="B96" s="2"/>
-    </row>
-    <row r="97" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A97" s="1"/>
-      <c r="B97" s="2"/>
-    </row>
-    <row r="98" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A98" s="1"/>
-      <c r="B98" s="2"/>
-    </row>
-    <row r="99" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A99" s="3"/>
-    </row>
-    <row r="100" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A100" s="8"/>
+      <c r="A96" s="8"/>
+    </row>
+    <row r="99" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A99" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A100" s="12"/>
+    </row>
+    <row r="101" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A101" s="12"/>
+    </row>
+    <row r="102" spans="1:2" ht="50.4" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A102" s="12"/>
     </row>
     <row r="103" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A103" s="12" t="s">
-        <v>2</v>
-      </c>
+      <c r="A103" s="12"/>
     </row>
     <row r="104" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A104" s="12"/>
     </row>
     <row r="105" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.7">
@@ -1283,7 +1278,7 @@
     </row>
     <row r="107" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B107" s="2"/>
     </row>
@@ -1293,25 +1288,25 @@
     </row>
     <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B109" s="2"/>
     </row>
     <row r="110" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B110" s="2"/>
     </row>
     <row r="111" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B111" s="2"/>
     </row>
     <row r="112" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B112" s="2"/>
     </row>
@@ -1321,7 +1316,7 @@
     </row>
     <row r="114" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
@@ -1337,7 +1332,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
@@ -1345,7 +1340,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
@@ -1353,24 +1348,24 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A123" s="12"/>
     </row>
     <row r="124" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A125" s="12"/>
       <c r="B125" s="2"/>
     </row>
     <row r="126" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B126" s="2"/>
     </row>
@@ -1380,21 +1375,23 @@
     </row>
     <row r="128" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A129" s="12"/>
     </row>
-    <row r="130" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A130" s="12"/>
+    <row r="130" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="131" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A131" s="12"/>
     </row>
     <row r="132" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
@@ -1402,7 +1399,7 @@
     </row>
     <row r="134" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1410,7 +1407,7 @@
     </row>
     <row r="136" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
@@ -1418,7 +1415,7 @@
     </row>
     <row r="138" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
@@ -1426,7 +1423,7 @@
     </row>
     <row r="140" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
@@ -1434,12 +1431,12 @@
     </row>
     <row r="142" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1448,7 +1445,7 @@
     </row>
     <row r="145" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B145" s="2"/>
     </row>
@@ -1458,7 +1455,7 @@
     </row>
     <row r="147" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1466,7 +1463,7 @@
     </row>
     <row r="149" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="21" x14ac:dyDescent="0.4">
@@ -1474,7 +1471,7 @@
     </row>
     <row r="151" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1482,7 +1479,7 @@
     </row>
     <row r="153" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A153" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B153" s="2"/>
     </row>
@@ -1492,7 +1489,7 @@
     </row>
     <row r="155" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A155" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1500,7 +1497,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="21" x14ac:dyDescent="0.4">
@@ -1508,7 +1505,7 @@
     </row>
     <row r="159" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A159" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1516,7 +1513,7 @@
     </row>
     <row r="161" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A161" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="21" x14ac:dyDescent="0.4">
@@ -1524,7 +1521,7 @@
     </row>
     <row r="163" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A163" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="21" x14ac:dyDescent="0.4">
@@ -1541,7 +1538,7 @@
     </row>
     <row r="167" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A167" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1743,7 +1740,7 @@
     </row>
     <row r="240" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A240" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B240" s="2"/>
     </row>

</xml_diff>

<commit_message>
error handling to time stamp controller
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabia\OneDrive\Desktop\ProgrammierAnleitung\Java\2025 WIFI\EmployeeAdministration\documentation\ToDo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1028" documentId="11_AD4DB114E441178AC67DF488CE17C2E2683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{916F987F-3BC7-4108-A8ED-BB3D637DDDF4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986A775C-F911-4951-8B19-FA9110858A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>Scope, Nicht-Scope, funktionale Anforderungen( habe ich schon), nicht funktionale Anforderungen, Overview Ziel reinschreiben, Benutzerschnittstellen sind einzelne Windows,</t>
   </si>
@@ -296,6 +296,9 @@
   </si>
   <si>
     <t>- Bei Update auf Admin Status. Checken ob es eh keine Mitarbeiter gibt. Falls doch auch Bei Mitarbeitern forgesetzten auf null setzten.</t>
+  </si>
+  <si>
+    <t>Hibernate TODOS durchsuchen</t>
   </si>
 </sst>
 </file>
@@ -421,13 +424,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>210</xdr:row>
+      <xdr:row>216</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>224</xdr:row>
+      <xdr:row>230</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -482,13 +485,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
-      <xdr:row>178</xdr:row>
+      <xdr:row>184</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3295762</xdr:colOff>
-      <xdr:row>198</xdr:row>
+      <xdr:row>204</xdr:row>
       <xdr:rowOff>1595</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -526,13 +529,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1809525</xdr:colOff>
-      <xdr:row>88</xdr:row>
+      <xdr:row>94</xdr:row>
       <xdr:rowOff>193411</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -578,10 +581,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -847,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G244"/>
+  <dimension ref="A1:G250"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -882,48 +881,41 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>74</v>
-      </c>
+      <c r="A10" s="3"/>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
+      <c r="A11" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>75</v>
-      </c>
+      <c r="A12" s="3"/>
       <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A14" s="4" t="s">
-        <v>77</v>
+    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="B14" s="2"/>
     </row>
@@ -933,7 +925,7 @@
     </row>
     <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B16" s="2"/>
     </row>
@@ -943,7 +935,7 @@
     </row>
     <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B18" s="2"/>
     </row>
@@ -951,27 +943,30 @@
       <c r="A19" s="3"/>
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A20" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>82</v>
-      </c>
+      <c r="A21" s="3"/>
       <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
+      <c r="A22" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="14" t="s">
-        <v>83</v>
-      </c>
+      <c r="A23" s="3"/>
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
+      <c r="A24" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -979,11 +974,12 @@
       <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
+      <c r="A27" t="s">
+        <v>82</v>
+      </c>
       <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -991,7 +987,9 @@
       <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
+      <c r="A29" s="14" t="s">
+        <v>83</v>
+      </c>
       <c r="B29" s="2"/>
     </row>
     <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1007,221 +1005,221 @@
       <c r="B32" s="2"/>
     </row>
     <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
+      <c r="A33" s="3"/>
       <c r="B33" s="2"/>
     </row>
     <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="A34" s="3"/>
       <c r="B34" s="2"/>
     </row>
     <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
+      <c r="A35" s="3"/>
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="1:3" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>40</v>
-      </c>
+    <row r="36" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="3"/>
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="1:3" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
+    <row r="37" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="3"/>
       <c r="B37" s="2"/>
     </row>
     <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="A38" s="3"/>
       <c r="B38" s="2"/>
     </row>
     <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="2"/>
-    </row>
-    <row r="40" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="11" t="s">
-        <v>42</v>
-      </c>
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="2"/>
     </row>
     <row r="41" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="2"/>
-    </row>
-    <row r="42" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B42" s="1"/>
-      <c r="C42" s="2"/>
-    </row>
-    <row r="43" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B43" s="1"/>
-      <c r="C43" s="2"/>
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" spans="1:3" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="2"/>
+    </row>
+    <row r="43" spans="1:3" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="2"/>
     </row>
     <row r="44" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B44" s="1"/>
-      <c r="C44" s="2"/>
+      <c r="A44" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="2"/>
     </row>
     <row r="45" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B46" s="1"/>
-      <c r="C46" s="2"/>
+    <row r="46" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="11" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="47" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="2"/>
     </row>
-    <row r="48" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B48" s="2"/>
-    </row>
-    <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B50" s="2"/>
-    </row>
-    <row r="51" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="10" t="s">
+    <row r="48" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="2"/>
+    </row>
+    <row r="49" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B49" s="1"/>
+      <c r="C49" s="2"/>
+    </row>
+    <row r="50" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B50" s="1"/>
+      <c r="C50" s="2"/>
+    </row>
+    <row r="51" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B51" s="1"/>
+      <c r="C51" s="2"/>
+    </row>
+    <row r="52" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B52" s="1"/>
+      <c r="C52" s="2"/>
+    </row>
+    <row r="53" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B53" s="1"/>
+      <c r="C53" s="2"/>
+    </row>
+    <row r="54" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B54" s="2"/>
+    </row>
+    <row r="55" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B55" s="2"/>
+    </row>
+    <row r="56" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B56" s="2"/>
+    </row>
+    <row r="57" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B51" s="2"/>
-    </row>
-    <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="1"/>
-      <c r="B52" s="2"/>
-    </row>
-    <row r="53" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="1"/>
-      <c r="B53" s="2"/>
-    </row>
-    <row r="54" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="1"/>
-    </row>
-    <row r="55" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="1"/>
-    </row>
-    <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="1"/>
-      <c r="B56" s="2"/>
-    </row>
-    <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="1"/>
       <c r="B57" s="2"/>
     </row>
-    <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="3"/>
-      <c r="B58" s="8"/>
-    </row>
-    <row r="59" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="1"/>
+      <c r="B58" s="2"/>
+    </row>
+    <row r="59" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
     </row>
-    <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="3"/>
-      <c r="B60" s="2"/>
-    </row>
-    <row r="61" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="1"/>
+    </row>
+    <row r="61" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
     </row>
-    <row r="64" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="9" t="s">
+    <row r="62" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="1"/>
+      <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="1"/>
+      <c r="B63" s="2"/>
+    </row>
+    <row r="64" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="3"/>
+      <c r="B64" s="8"/>
+    </row>
+    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="1"/>
+      <c r="B65" s="2"/>
+    </row>
+    <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="3"/>
+      <c r="B66" s="2"/>
+    </row>
+    <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="1"/>
+    </row>
+    <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B64" s="2"/>
-    </row>
-    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="9"/>
-      <c r="B65" s="2"/>
-    </row>
-    <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="9"/>
-      <c r="B66" s="2"/>
-    </row>
-    <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="9"/>
-      <c r="B67" s="2"/>
-    </row>
-    <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A68" s="9"/>
-      <c r="B68" s="2"/>
-    </row>
-    <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="9"/>
-      <c r="B69" s="2"/>
-    </row>
-    <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="9"/>
       <c r="B70" s="2"/>
     </row>
     <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="9"/>
+      <c r="B71" s="2"/>
+    </row>
+    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="9"/>
+      <c r="B72" s="2"/>
+    </row>
+    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="9"/>
+      <c r="B73" s="2"/>
+    </row>
+    <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="9"/>
+      <c r="B74" s="2"/>
+    </row>
+    <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="9"/>
+      <c r="B75" s="2"/>
+    </row>
+    <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="9"/>
+      <c r="B76" s="2"/>
+    </row>
+    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B71" s="2"/>
-    </row>
-    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="3"/>
-      <c r="B72" s="2"/>
-    </row>
-    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+      <c r="B77" s="2"/>
+    </row>
+    <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="3"/>
+      <c r="B78" s="2"/>
+    </row>
+    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>33</v>
       </c>
-      <c r="B73" s="2"/>
-      <c r="G73" t="s">
+      <c r="B79" s="2"/>
+      <c r="G79" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="1"/>
-      <c r="B74" s="2"/>
-    </row>
-    <row r="75" spans="1:7" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B76" s="2"/>
-    </row>
-    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B77" s="2"/>
-    </row>
-    <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="1"/>
-      <c r="B78" s="2"/>
-    </row>
-    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A79" s="1"/>
-      <c r="B79" s="2"/>
     </row>
     <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
     </row>
-    <row r="81" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A81" s="1"/>
-      <c r="B81" s="2"/>
+    <row r="81" spans="1:2" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="82" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="1"/>
+      <c r="A82" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="B82" s="2"/>
     </row>
     <row r="83" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="1"/>
+      <c r="A83" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="B83" s="2"/>
     </row>
     <row r="84" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1261,285 +1259,285 @@
       <c r="B92" s="2"/>
     </row>
     <row r="93" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A93" s="3"/>
+      <c r="A93" s="1"/>
+      <c r="B93" s="2"/>
     </row>
     <row r="94" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A94" s="8"/>
-    </row>
-    <row r="97" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A97" s="12" t="s">
+      <c r="A94" s="1"/>
+      <c r="B94" s="2"/>
+    </row>
+    <row r="95" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A95" s="1"/>
+      <c r="B95" s="2"/>
+    </row>
+    <row r="96" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A96" s="1"/>
+      <c r="B96" s="2"/>
+    </row>
+    <row r="97" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A97" s="1"/>
+      <c r="B97" s="2"/>
+    </row>
+    <row r="98" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A98" s="1"/>
+      <c r="B98" s="2"/>
+    </row>
+    <row r="99" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A99" s="3"/>
+    </row>
+    <row r="100" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A100" s="8"/>
+    </row>
+    <row r="103" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A103" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A98" s="12"/>
-    </row>
-    <row r="99" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A99" s="12"/>
-    </row>
-    <row r="100" spans="1:2" ht="50.4" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A100" s="12"/>
-    </row>
-    <row r="101" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A101" s="12"/>
-    </row>
-    <row r="102" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A102" s="12"/>
-    </row>
-    <row r="103" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="3" t="s">
+    <row r="104" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A104" s="12"/>
+    </row>
+    <row r="105" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A105" s="12"/>
+    </row>
+    <row r="106" spans="1:2" ht="50.4" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A106" s="12"/>
+    </row>
+    <row r="107" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A107" s="12"/>
+    </row>
+    <row r="108" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A108" s="12"/>
+    </row>
+    <row r="109" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A104" s="12"/>
-    </row>
-    <row r="105" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A105" s="3" t="s">
+    <row r="110" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A110" s="12"/>
+    </row>
+    <row r="111" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A111" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B105" s="2"/>
-    </row>
-    <row r="106" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A106" s="3"/>
-      <c r="B106" s="2"/>
-    </row>
-    <row r="107" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A107" s="3" t="s">
+      <c r="B111" s="2"/>
+    </row>
+    <row r="112" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A112" s="3"/>
+      <c r="B112" s="2"/>
+    </row>
+    <row r="113" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A113" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B107" s="2"/>
-    </row>
-    <row r="108" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
+      <c r="B113" s="2"/>
+    </row>
+    <row r="114" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
         <v>57</v>
       </c>
-      <c r="B108" s="2"/>
-    </row>
-    <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A109" s="3" t="s">
+      <c r="B114" s="2"/>
+    </row>
+    <row r="115" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A115" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B109" s="2"/>
-    </row>
-    <row r="110" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A110" s="3" t="s">
+      <c r="B115" s="2"/>
+    </row>
+    <row r="116" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A116" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B110" s="2"/>
-    </row>
-    <row r="111" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A111" s="3"/>
-      <c r="B111" s="2"/>
-    </row>
-    <row r="112" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A112" s="3" t="s">
+      <c r="B116" s="2"/>
+    </row>
+    <row r="117" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A117" s="3"/>
+      <c r="B117" s="2"/>
+    </row>
+    <row r="118" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A118" s="3" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A113" s="12"/>
-    </row>
-    <row r="114" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A114" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A115" s="12"/>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A117" s="12"/>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A119" s="12"/>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
+    <row r="120" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A120" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A121" s="12"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A123" s="12"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A125" s="12"/>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A121" s="12"/>
-    </row>
-    <row r="122" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A122" s="3" t="s">
+    <row r="127" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A127" s="12"/>
+    </row>
+    <row r="128" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A128" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A123" s="12"/>
-      <c r="B123" s="2"/>
-    </row>
-    <row r="124" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A124" s="3" t="s">
+    <row r="129" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A129" s="12"/>
+      <c r="B129" s="2"/>
+    </row>
+    <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A130" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B124" s="2"/>
-    </row>
-    <row r="125" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A125" s="3"/>
-      <c r="B125" s="2"/>
-    </row>
-    <row r="126" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A126" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A127" s="12"/>
-    </row>
-    <row r="128" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A129" s="12"/>
-    </row>
-    <row r="130" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A131" s="12"/>
+      <c r="B130" s="2"/>
+    </row>
+    <row r="131" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A131" s="3"/>
+      <c r="B131" s="2"/>
     </row>
     <row r="132" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A133" s="3"/>
-    </row>
-    <row r="134" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A133" s="12"/>
+    </row>
+    <row r="134" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A135" s="12"/>
     </row>
-    <row r="136" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A137" s="12"/>
     </row>
-    <row r="138" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A139" s="12"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A139" s="3"/>
     </row>
     <row r="140" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A141" s="12"/>
+    </row>
+    <row r="142" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A143" s="12"/>
+    </row>
+    <row r="144" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A145" s="12"/>
+    </row>
+    <row r="146" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A146" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="3" t="s">
+    <row r="147" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A142" s="3"/>
-      <c r="B142" s="2"/>
-    </row>
-    <row r="143" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A143" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B143" s="2"/>
-    </row>
-    <row r="144" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A144" s="12"/>
-      <c r="B144" s="2"/>
-    </row>
-    <row r="145" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A145" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A146" s="3"/>
-    </row>
-    <row r="147" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A147" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A148" s="4"/>
+    <row r="148" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A148" s="3"/>
+      <c r="B148" s="2"/>
     </row>
     <row r="149" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="B149" s="2"/>
+    </row>
+    <row r="150" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A150" s="12"/>
       <c r="B150" s="2"/>
     </row>
     <row r="151" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B151" s="2"/>
-    </row>
-    <row r="152" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A152" s="4"/>
-      <c r="B152" s="2"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A152" s="3"/>
     </row>
     <row r="153" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A153" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A154" s="3"/>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A155" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A156" s="4"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A154" s="4"/>
+    </row>
+    <row r="155" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A155" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B156" s="2"/>
     </row>
     <row r="157" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A157" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A158" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="B157" s="2"/>
+    </row>
+    <row r="158" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A158" s="4"/>
+      <c r="B158" s="2"/>
     </row>
     <row r="159" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A159" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A160" s="4"/>
-    </row>
-    <row r="161" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A161" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A160" s="3"/>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="21" x14ac:dyDescent="0.4">
@@ -1547,36 +1545,32 @@
     </row>
     <row r="163" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A163" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A164" s="4"/>
-      <c r="B164" s="2"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A164" s="3"/>
     </row>
     <row r="165" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A165" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A166" s="3"/>
-      <c r="B166" s="2"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A166" s="4"/>
     </row>
     <row r="167" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A167" s="3" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A168" s="4"/>
-      <c r="B168" s="2"/>
     </row>
     <row r="169" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A169" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B169" s="2"/>
+        <v>22</v>
+      </c>
     </row>
     <row r="170" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A170" s="4"/>
@@ -1584,203 +1578,231 @@
     </row>
     <row r="171" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A171" s="3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A172" s="3"/>
       <c r="B172" s="2"/>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A173" t="s">
-        <v>21</v>
-      </c>
+    <row r="173" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A173" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A174" s="4"/>
+      <c r="B174" s="2"/>
     </row>
     <row r="175" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A175" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B175" s="2"/>
+    </row>
+    <row r="176" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A176" s="4"/>
+      <c r="B176" s="2"/>
+    </row>
+    <row r="177" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A177" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A178" s="3"/>
+      <c r="B178" s="2"/>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A181" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A177" t="s">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="198" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B198" s="2"/>
-    </row>
-    <row r="200" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B200" s="2"/>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A201" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B202" s="2"/>
-    </row>
-    <row r="203" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A203" t="s">
-        <v>1</v>
-      </c>
-      <c r="B203" s="2"/>
     </row>
     <row r="204" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B204" s="2"/>
     </row>
-    <row r="205" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A205" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B205" s="2"/>
-    </row>
     <row r="206" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A206" s="3"/>
       <c r="B206" s="2"/>
     </row>
-    <row r="207" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A207" s="3" t="s">
-        <v>20</v>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A208" s="3"/>
       <c r="B208" s="2"/>
     </row>
     <row r="209" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A209" s="3" t="s">
-        <v>12</v>
+      <c r="A209" t="s">
+        <v>1</v>
       </c>
       <c r="B209" s="2"/>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B210" s="5" t="s">
-        <v>6</v>
-      </c>
+    <row r="210" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B210" s="2"/>
     </row>
     <row r="211" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A211" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B211" s="2"/>
+    </row>
+    <row r="212" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A212" s="3"/>
+      <c r="B212" s="2"/>
+    </row>
+    <row r="213" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A213" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A214" s="3"/>
+      <c r="B214" s="2"/>
+    </row>
+    <row r="215" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A215" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B215" s="2"/>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B216" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A217" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="212" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A212" s="1"/>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A215" s="5"/>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A216" s="5"/>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A217" s="5"/>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A218" s="5" t="s">
+    <row r="218" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A218" s="1"/>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A221" s="5"/>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A222" s="5"/>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A223" s="5"/>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A224" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A219" s="5" t="s">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A225" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="220" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A220" s="5" t="s">
+    <row r="226" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A226" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B220" s="2"/>
-    </row>
-    <row r="221" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A221" s="5"/>
-      <c r="B221" s="2"/>
-    </row>
-    <row r="222" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A222" s="5" t="s">
+      <c r="B226" s="2"/>
+    </row>
+    <row r="227" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A227" s="5"/>
+      <c r="B227" s="2"/>
+    </row>
+    <row r="228" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A228" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B222" s="2"/>
-    </row>
-    <row r="223" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A223" s="1"/>
-      <c r="B223" s="2"/>
-    </row>
-    <row r="224" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A224" s="1"/>
-      <c r="B224" s="2"/>
-    </row>
-    <row r="225" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A225" s="1"/>
-      <c r="B225" s="2"/>
-    </row>
-    <row r="226" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A226" s="1"/>
-    </row>
-    <row r="227" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A227" s="1"/>
-      <c r="B227" s="2"/>
-    </row>
-    <row r="228" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A228" s="1"/>
+      <c r="B228" s="2"/>
     </row>
     <row r="229" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A229" s="1"/>
       <c r="B229" s="2"/>
     </row>
     <row r="230" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A230" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="A230" s="1"/>
+      <c r="B230" s="2"/>
     </row>
     <row r="231" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A231" s="1"/>
       <c r="B231" s="2"/>
     </row>
     <row r="232" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A232" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="A232" s="1"/>
     </row>
     <row r="233" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A233" s="1"/>
       <c r="B233" s="2"/>
     </row>
     <row r="234" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A234" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="A234" s="1"/>
+    </row>
+    <row r="235" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B235" s="2"/>
     </row>
     <row r="236" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A236" s="3" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B237" s="2"/>
     </row>
     <row r="238" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A238" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B238" s="2"/>
+      <c r="A238" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="239" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B239" s="2"/>
     </row>
     <row r="240" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A240" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A241" s="1"/>
-      <c r="B241" s="2"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="242" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A242" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B243" s="2"/>
+    </row>
+    <row r="244" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A244" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B244" s="2"/>
+    </row>
+    <row r="245" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B245" s="2"/>
+    </row>
+    <row r="246" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A246" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A247" s="1"/>
+      <c r="B247" s="2"/>
+    </row>
+    <row r="248" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A248" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="244" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A244" s="3" t="s">
+    <row r="250" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A250" s="3" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
error handling in vacations controller
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabia\OneDrive\Desktop\ProgrammierAnleitung\Java\2025 WIFI\EmployeeAdministration\documentation\ToDo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986A775C-F911-4951-8B19-FA9110858A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{986A775C-F911-4951-8B19-FA9110858A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61F03FCB-3C33-4C29-B1A4-848EE3C82489}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -274,9 +274,6 @@
     <t>Requirements durchgehen und ergänzen</t>
   </si>
   <si>
-    <t>ToDos Error handling</t>
-  </si>
-  <si>
     <t xml:space="preserve">Unmittelbar vor Abgabe: </t>
   </si>
   <si>
@@ -299,6 +296,9 @@
   </si>
   <si>
     <t>Hibernate TODOS durchsuchen</t>
+  </si>
+  <si>
+    <t>ToDos Error + rethrow exception in controllers to main stage</t>
   </si>
 </sst>
 </file>
@@ -849,7 +849,7 @@
   <dimension ref="A1:G250"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -891,7 +891,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="B9" s="2"/>
     </row>
@@ -901,7 +901,7 @@
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B11" s="2"/>
     </row>
@@ -915,7 +915,7 @@
     </row>
     <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B14" s="2"/>
     </row>
@@ -945,7 +945,7 @@
     </row>
     <row r="20" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A20" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B20" s="2"/>
     </row>
@@ -955,7 +955,7 @@
     </row>
     <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B22" s="2"/>
     </row>
@@ -965,7 +965,7 @@
     </row>
     <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24" s="2"/>
     </row>
@@ -978,7 +978,7 @@
     </row>
     <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B27" s="2"/>
     </row>
@@ -988,7 +988,7 @@
     </row>
     <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B29" s="2"/>
     </row>
@@ -1310,7 +1310,7 @@
     </row>
     <row r="109" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.7">

</xml_diff>

<commit_message>
adds error handling to vacation controller
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{986A775C-F911-4951-8B19-FA9110858A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61F03FCB-3C33-4C29-B1A4-848EE3C82489}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{986A775C-F911-4951-8B19-FA9110858A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAA0E43C-D359-4293-AA74-C34ED51561FD}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>Scope, Nicht-Scope, funktionale Anforderungen( habe ich schon), nicht funktionale Anforderungen, Overview Ziel reinschreiben, Benutzerschnittstellen sind einzelne Windows,</t>
   </si>
@@ -299,6 +299,9 @@
   </si>
   <si>
     <t>ToDos Error + rethrow exception in controllers to main stage</t>
+  </si>
+  <si>
+    <t>Error in Requests Controller</t>
   </si>
 </sst>
 </file>
@@ -583,6 +586,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -849,7 +856,7 @@
   <dimension ref="A1:G250"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -884,6 +891,9 @@
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>85</v>
+      </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updates docu, makes clock in and clock out a transaction
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{986A775C-F911-4951-8B19-FA9110858A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E654CD6E-945E-4D08-99DF-228CA9950F13}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{986A775C-F911-4951-8B19-FA9110858A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C436E98-4C11-4B6F-BBC8-513AA01C6CF8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>Scope, Nicht-Scope, funktionale Anforderungen( habe ich schon), nicht funktionale Anforderungen, Overview Ziel reinschreiben, Benutzerschnittstellen sind einzelne Windows,</t>
   </si>
@@ -205,12 +205,6 @@
     <t>Constants Employee overview</t>
   </si>
   <si>
-    <t>3.make sure that Admins can only make managers or other admins
-3. update logic for managers
-4.Manager is supposed to create other managers
-5.Admins can only create other adminss</t>
-  </si>
-  <si>
     <t xml:space="preserve">eigene AddressForm machen </t>
   </si>
   <si>
@@ -262,9 +256,6 @@
     <t>Master Data View - je nach Rolle des angesehenen Subordinates oder Superior anpassen</t>
   </si>
   <si>
-    <t>Schauen wo Exekutor Service noch fehlt oder nicht und einbauen</t>
-  </si>
-  <si>
     <t>Schauen dass beim Erstellen und Updaten sowohl Wochen als auch Urlaub beachtet und validiert werden nicht zu kurz kommen.</t>
   </si>
   <si>
@@ -283,9 +274,6 @@
     <t>ERD Diagramm aus PG Admin rausholen und bearbeiten</t>
   </si>
   <si>
-    <t>Mit Deaktivierungen und Aktivierungen machen, dass Managers nur Employees zu Managern befördern können und dass Admins nur Managers zu Admins befördern können</t>
-  </si>
-  <si>
     <t>Person entity lengths mit lengths in DB vergleichen</t>
   </si>
   <si>
@@ -302,6 +290,21 @@
   </si>
   <si>
     <t>Error in Handling in allen Controller und DAOS</t>
+  </si>
+  <si>
+    <t>3.make sure that Admins can only make managers or other admins</t>
+  </si>
+  <si>
+    <t>3. update logic for managers</t>
+  </si>
+  <si>
+    <t>4.Manager is supposed to create other managers</t>
+  </si>
+  <si>
+    <t>5.Admins can only create other adminss</t>
+  </si>
+  <si>
+    <t>Schauen wo Exekutor Service noch fehlt oder nicht und einbauen - bzw austauschen</t>
   </si>
 </sst>
 </file>
@@ -427,13 +430,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>216</xdr:row>
+      <xdr:row>219</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>230</xdr:row>
+      <xdr:row>233</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -488,13 +491,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
-      <xdr:row>184</xdr:row>
+      <xdr:row>187</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3295762</xdr:colOff>
-      <xdr:row>204</xdr:row>
+      <xdr:row>207</xdr:row>
       <xdr:rowOff>1595</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -532,13 +535,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1809525</xdr:colOff>
-      <xdr:row>94</xdr:row>
+      <xdr:row>96</xdr:row>
       <xdr:rowOff>193411</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -853,10 +856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G250"/>
+  <dimension ref="A1:G253"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -870,17 +873,18 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>39</v>
+      <c r="A2" t="s">
+        <v>82</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="B4" s="2"/>
     </row>
@@ -888,44 +892,48 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>85</v>
-      </c>
+      <c r="A7" s="3"/>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>77</v>
+      </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>84</v>
-      </c>
+      <c r="A9" s="3"/>
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>83</v>
-      </c>
+      <c r="A11" s="3"/>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
+      <c r="A12" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>80</v>
+    <row r="14" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A14" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="B14" s="2"/>
     </row>
@@ -935,7 +943,7 @@
     </row>
     <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B16" s="2"/>
     </row>
@@ -945,7 +953,7 @@
     </row>
     <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B18" s="2"/>
     </row>
@@ -953,30 +961,27 @@
       <c r="A19" s="3"/>
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A20" s="4" t="s">
-        <v>76</v>
-      </c>
+    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
+      <c r="A21" t="s">
+        <v>78</v>
+      </c>
       <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="A22" s="3"/>
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
+      <c r="A23" s="14" t="s">
+        <v>79</v>
+      </c>
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="A24" s="3"/>
       <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -984,12 +989,11 @@
       <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>81</v>
-      </c>
+      <c r="A27" s="3"/>
       <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -997,9 +1001,7 @@
       <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
-        <v>82</v>
-      </c>
+      <c r="A29" s="3"/>
       <c r="B29" s="2"/>
     </row>
     <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1015,27 +1017,29 @@
       <c r="B32" s="2"/>
     </row>
     <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
+      <c r="A33" s="1"/>
       <c r="B33" s="2"/>
     </row>
     <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="3"/>
+      <c r="A34" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="B34" s="2"/>
     </row>
     <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="3"/>
+      <c r="A35" s="1"/>
       <c r="B35" s="2"/>
     </row>
     <row r="36" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="3"/>
+      <c r="A36" s="1"/>
       <c r="B36" s="2"/>
     </row>
     <row r="37" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="3"/>
+      <c r="A37" s="1"/>
       <c r="B37" s="2"/>
     </row>
     <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="3"/>
+      <c r="A38" s="1"/>
       <c r="B38" s="2"/>
     </row>
     <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -1043,58 +1047,56 @@
       <c r="B39" s="2"/>
     </row>
     <row r="40" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="A40" s="1"/>
       <c r="B40" s="2"/>
     </row>
     <row r="41" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="1:3" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="2"/>
+    </row>
+    <row r="43" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="3"/>
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" spans="1:3" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="2"/>
-    </row>
-    <row r="43" spans="1:3" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="1"/>
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" spans="1:3" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="2"/>
+    </row>
+    <row r="46" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="2"/>
-    </row>
-    <row r="45" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="2"/>
-    </row>
-    <row r="46" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="11" t="s">
-        <v>42</v>
-      </c>
+      <c r="B46" s="2"/>
     </row>
     <row r="47" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="2"/>
     </row>
-    <row r="48" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B48" s="1"/>
-      <c r="C48" s="2"/>
+    <row r="48" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="11" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="49" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="2"/>
     </row>
     <row r="50" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="13"/>
       <c r="B50" s="1"/>
       <c r="C50" s="2"/>
     </row>
@@ -1111,176 +1113,178 @@
       <c r="C53" s="2"/>
     </row>
     <row r="54" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B54" s="2"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="2"/>
     </row>
     <row r="55" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B55" s="2"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="2"/>
     </row>
     <row r="56" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B56" s="2"/>
     </row>
     <row r="57" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="10" t="s">
+      <c r="B57" s="2"/>
+    </row>
+    <row r="58" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B58" s="2"/>
+    </row>
+    <row r="59" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B57" s="2"/>
-    </row>
-    <row r="58" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="1"/>
-      <c r="B58" s="2"/>
-    </row>
-    <row r="59" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="1"/>
       <c r="B59" s="2"/>
     </row>
     <row r="60" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
+      <c r="B60" s="2"/>
     </row>
     <row r="61" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
+      <c r="B61" s="2"/>
     </row>
     <row r="62" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
-      <c r="B62" s="2"/>
     </row>
     <row r="63" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
-      <c r="B63" s="2"/>
     </row>
     <row r="64" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="3"/>
-      <c r="B64" s="8"/>
-    </row>
-    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="1"/>
+      <c r="B64" s="2"/>
+    </row>
+    <row r="65" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
     </row>
-    <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
-      <c r="B66" s="2"/>
-    </row>
-    <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B66" s="8"/>
+    </row>
+    <row r="67" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
-    </row>
-    <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="9" t="s">
+      <c r="B67" s="2"/>
+    </row>
+    <row r="68" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="3"/>
+      <c r="B68" s="2"/>
+    </row>
+    <row r="69" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="1"/>
+    </row>
+    <row r="72" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B70" s="2"/>
-    </row>
-    <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A71" s="9"/>
-      <c r="B71" s="2"/>
-    </row>
-    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="9"/>
       <c r="B72" s="2"/>
     </row>
-    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="9"/>
       <c r="B73" s="2"/>
     </row>
-    <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="9"/>
       <c r="B74" s="2"/>
     </row>
-    <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="9"/>
       <c r="B75" s="2"/>
     </row>
-    <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="9"/>
       <c r="B76" s="2"/>
     </row>
-    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="B77" s="2"/>
     </row>
-    <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="3"/>
+    <row r="78" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="9"/>
       <c r="B78" s="2"/>
     </row>
-    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+    <row r="79" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B79" s="2"/>
+    </row>
+    <row r="80" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="3"/>
+      <c r="B80" s="2"/>
+    </row>
+    <row r="81" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>33</v>
       </c>
-      <c r="B79" s="2"/>
-      <c r="G79" t="s">
+      <c r="B81" s="2"/>
+      <c r="G81" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A80" s="1"/>
-      <c r="B80" s="2"/>
-    </row>
-    <row r="81" spans="1:2" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A81" s="3" t="s">
+    <row r="82" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="1"/>
+      <c r="B82" s="2"/>
+    </row>
+    <row r="83" spans="1:7" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="3" t="s">
+    <row r="84" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B82" s="2"/>
-    </row>
-    <row r="83" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="7" t="s">
+      <c r="B84" s="2"/>
+    </row>
+    <row r="85" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B83" s="2"/>
-    </row>
-    <row r="84" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A84" s="1"/>
-      <c r="B84" s="2"/>
-    </row>
-    <row r="85" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A85" s="1"/>
       <c r="B85" s="2"/>
     </row>
-    <row r="86" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
     </row>
-    <row r="87" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
     </row>
-    <row r="88" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
     </row>
-    <row r="89" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
     </row>
-    <row r="90" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
     </row>
-    <row r="91" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
     </row>
-    <row r="92" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
     </row>
-    <row r="93" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
     </row>
-    <row r="94" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
     </row>
-    <row r="95" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
     </row>
-    <row r="96" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
     </row>
@@ -1293,461 +1297,467 @@
       <c r="B98" s="2"/>
     </row>
     <row r="99" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A99" s="3"/>
+      <c r="A99" s="1"/>
+      <c r="B99" s="2"/>
     </row>
     <row r="100" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A100" s="8"/>
-    </row>
-    <row r="103" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A103" s="12" t="s">
+      <c r="A100" s="1"/>
+      <c r="B100" s="2"/>
+    </row>
+    <row r="101" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A101" s="3"/>
+    </row>
+    <row r="102" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A102" s="8"/>
+    </row>
+    <row r="105" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A105" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A104" s="12"/>
-    </row>
-    <row r="105" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A105" s="12"/>
-    </row>
-    <row r="106" spans="1:2" ht="50.4" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="106" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A106" s="12"/>
     </row>
-    <row r="107" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+    <row r="107" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A107" s="12"/>
     </row>
     <row r="108" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A108" s="12"/>
     </row>
-    <row r="109" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A110" s="12"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A110" s="3" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="111" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B111" s="2"/>
-    </row>
-    <row r="112" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A112" s="3"/>
-      <c r="B112" s="2"/>
-    </row>
-    <row r="113" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A113" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B113" s="2"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A113" s="12"/>
     </row>
     <row r="114" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
-        <v>57</v>
+      <c r="A114" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="B114" s="2"/>
     </row>
     <row r="115" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A115" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="A115" s="3"/>
       <c r="B115" s="2"/>
     </row>
     <row r="116" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B116" s="2"/>
     </row>
     <row r="117" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A117" s="3"/>
+      <c r="A117" t="s">
+        <v>56</v>
+      </c>
       <c r="B117" s="2"/>
     </row>
     <row r="118" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A119" s="12"/>
+      <c r="B118" s="2"/>
+    </row>
+    <row r="119" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A119" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B119" s="2"/>
     </row>
     <row r="120" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A120" s="3" t="s">
+      <c r="A120" s="3"/>
+      <c r="B120" s="2"/>
+    </row>
+    <row r="121" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A121" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A122" s="12"/>
+    </row>
+    <row r="123" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A123" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A121" s="12"/>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A123" s="12"/>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A125" s="12"/>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
+    <row r="124" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A124" s="12"/>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A126" s="12"/>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A127" s="12"/>
-    </row>
-    <row r="128" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A128" s="3" t="s">
+    <row r="128" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A128" s="12"/>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A129" s="12"/>
-      <c r="B129" s="2"/>
-    </row>
-    <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A130" s="3" t="s">
+    <row r="130" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A130" s="12"/>
+    </row>
+    <row r="131" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A131" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A132" s="12"/>
+      <c r="B132" s="2"/>
+    </row>
+    <row r="133" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A133" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B133" s="2"/>
+    </row>
+    <row r="134" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A134" s="3"/>
+      <c r="B134" s="2"/>
+    </row>
+    <row r="135" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A135" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B130" s="2"/>
-    </row>
-    <row r="131" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A131" s="3"/>
-      <c r="B131" s="2"/>
-    </row>
-    <row r="132" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A132" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A133" s="12"/>
-    </row>
-    <row r="134" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A135" s="12"/>
-    </row>
-    <row r="136" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A137" s="12"/>
-    </row>
-    <row r="138" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A138" s="3" t="s">
+    </row>
+    <row r="136" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A136" s="12"/>
+    </row>
+    <row r="137" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A138" s="12"/>
+    </row>
+    <row r="139" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A139" s="3"/>
-    </row>
-    <row r="140" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A140" s="3" t="s">
+    <row r="140" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A140" s="12"/>
+    </row>
+    <row r="141" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A141" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A141" s="12"/>
-    </row>
-    <row r="142" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="3" t="s">
+    <row r="142" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A142" s="3"/>
+    </row>
+    <row r="143" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A143" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A144" s="12"/>
+    </row>
+    <row r="145" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A143" s="12"/>
-    </row>
-    <row r="144" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="3" t="s">
+    <row r="146" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A146" s="12"/>
+    </row>
+    <row r="147" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A145" s="12"/>
-    </row>
-    <row r="146" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A146" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A148" s="3"/>
-      <c r="B148" s="2"/>
+    <row r="148" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A148" s="12"/>
     </row>
     <row r="149" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A151" s="3"/>
+      <c r="B151" s="2"/>
+    </row>
+    <row r="152" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A152" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B149" s="2"/>
-    </row>
-    <row r="150" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A150" s="12"/>
-      <c r="B150" s="2"/>
-    </row>
-    <row r="151" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A151" s="3" t="s">
+      <c r="B152" s="2"/>
+    </row>
+    <row r="153" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A153" s="12"/>
+      <c r="B153" s="2"/>
+    </row>
+    <row r="154" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A154" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A152" s="3"/>
-    </row>
-    <row r="153" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A153" s="3" t="s">
+    <row r="155" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A155" s="3"/>
+    </row>
+    <row r="156" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A156" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A154" s="4"/>
-    </row>
-    <row r="155" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A155" s="3" t="s">
+    <row r="157" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A157" s="4"/>
+    </row>
+    <row r="158" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A158" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B156" s="2"/>
-    </row>
-    <row r="157" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A157" s="3" t="s">
+    <row r="159" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B159" s="2"/>
+    </row>
+    <row r="160" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A160" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B157" s="2"/>
-    </row>
-    <row r="158" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A158" s="4"/>
-      <c r="B158" s="2"/>
-    </row>
-    <row r="159" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A159" s="3" t="s">
+      <c r="B160" s="2"/>
+    </row>
+    <row r="161" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A161" s="4"/>
+      <c r="B161" s="2"/>
+    </row>
+    <row r="162" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A162" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A160" s="3"/>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
+    <row r="163" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A163" s="3"/>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A162" s="4"/>
-    </row>
-    <row r="163" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A163" s="3" t="s">
+    <row r="165" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A165" s="4"/>
+    </row>
+    <row r="166" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A166" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A164" s="3"/>
-    </row>
-    <row r="165" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A165" s="3" t="s">
+    <row r="167" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A167" s="3"/>
+    </row>
+    <row r="168" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A168" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A166" s="4"/>
-    </row>
-    <row r="167" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A167" s="3" t="s">
+    <row r="169" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A169" s="4"/>
+    </row>
+    <row r="170" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A170" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A168" s="4"/>
-    </row>
-    <row r="169" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A169" s="3" t="s">
+    <row r="171" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A171" s="4"/>
+    </row>
+    <row r="172" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A172" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A170" s="4"/>
-      <c r="B170" s="2"/>
-    </row>
-    <row r="171" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A171" s="3" t="s">
+    <row r="173" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A173" s="4"/>
+      <c r="B173" s="2"/>
+    </row>
+    <row r="174" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A174" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A172" s="3"/>
-      <c r="B172" s="2"/>
-    </row>
-    <row r="173" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A173" s="3" t="s">
+    <row r="175" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A175" s="3"/>
+      <c r="B175" s="2"/>
+    </row>
+    <row r="176" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A176" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A174" s="4"/>
-      <c r="B174" s="2"/>
-    </row>
-    <row r="175" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A175" s="3" t="s">
+    <row r="177" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A177" s="4"/>
+      <c r="B177" s="2"/>
+    </row>
+    <row r="178" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A178" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B175" s="2"/>
-    </row>
-    <row r="176" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A176" s="4"/>
-      <c r="B176" s="2"/>
-    </row>
-    <row r="177" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A177" s="3" t="s">
+      <c r="B178" s="2"/>
+    </row>
+    <row r="179" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A179" s="4"/>
+      <c r="B179" s="2"/>
+    </row>
+    <row r="180" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A180" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A178" s="3"/>
-      <c r="B178" s="2"/>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A179" t="s">
+    <row r="181" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A181" s="3"/>
+      <c r="B181" s="2"/>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A181" s="3" t="s">
+    <row r="184" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A184" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A183" t="s">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="204" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B204" s="2"/>
-    </row>
-    <row r="206" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B206" s="2"/>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A207" t="s">
+    <row r="207" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B207" s="2"/>
+    </row>
+    <row r="209" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B209" s="2"/>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B208" s="2"/>
-    </row>
-    <row r="209" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A209" t="s">
+    <row r="211" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B211" s="2"/>
+    </row>
+    <row r="212" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
         <v>1</v>
       </c>
-      <c r="B209" s="2"/>
-    </row>
-    <row r="210" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B210" s="2"/>
-    </row>
-    <row r="211" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A211" s="3" t="s">
+      <c r="B212" s="2"/>
+    </row>
+    <row r="213" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B213" s="2"/>
+    </row>
+    <row r="214" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A214" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B211" s="2"/>
-    </row>
-    <row r="212" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A212" s="3"/>
-      <c r="B212" s="2"/>
-    </row>
-    <row r="213" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A213" s="3" t="s">
+      <c r="B214" s="2"/>
+    </row>
+    <row r="215" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A215" s="3"/>
+      <c r="B215" s="2"/>
+    </row>
+    <row r="216" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A216" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A214" s="3"/>
-      <c r="B214" s="2"/>
-    </row>
-    <row r="215" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A215" s="3" t="s">
+    <row r="217" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A217" s="3"/>
+      <c r="B217" s="2"/>
+    </row>
+    <row r="218" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A218" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B215" s="2"/>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B216" s="5" t="s">
+      <c r="B218" s="2"/>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B219" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="217" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A217" s="3" t="s">
+    <row r="220" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A220" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="218" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A218" s="1"/>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A221" s="5"/>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A222" s="5"/>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A223" s="5"/>
+    <row r="221" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A221" s="1"/>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A224" s="5" t="s">
+      <c r="A224" s="5"/>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A225" s="5"/>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A226" s="5"/>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A227" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A225" s="5" t="s">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A228" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="226" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A226" s="5" t="s">
+    <row r="229" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A229" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B226" s="2"/>
-    </row>
-    <row r="227" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A227" s="5"/>
-      <c r="B227" s="2"/>
-    </row>
-    <row r="228" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A228" s="5" t="s">
+      <c r="B229" s="2"/>
+    </row>
+    <row r="230" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A230" s="5"/>
+      <c r="B230" s="2"/>
+    </row>
+    <row r="231" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A231" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B228" s="2"/>
-    </row>
-    <row r="229" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A229" s="1"/>
-      <c r="B229" s="2"/>
-    </row>
-    <row r="230" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A230" s="1"/>
-      <c r="B230" s="2"/>
-    </row>
-    <row r="231" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A231" s="1"/>
       <c r="B231" s="2"/>
     </row>
     <row r="232" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A232" s="1"/>
+      <c r="B232" s="2"/>
     </row>
     <row r="233" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A233" s="1"/>
@@ -1755,64 +1765,75 @@
     </row>
     <row r="234" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A234" s="1"/>
+      <c r="B234" s="2"/>
     </row>
     <row r="235" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B235" s="2"/>
+      <c r="A235" s="1"/>
     </row>
     <row r="236" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A236" s="3" t="s">
+      <c r="A236" s="1"/>
+      <c r="B236" s="2"/>
+    </row>
+    <row r="237" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A237" s="1"/>
+    </row>
+    <row r="238" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B238" s="2"/>
+    </row>
+    <row r="239" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A239" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="237" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B237" s="2"/>
-    </row>
-    <row r="238" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A238" s="3" t="s">
+    <row r="240" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B240" s="2"/>
+    </row>
+    <row r="241" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A241" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="239" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B239" s="2"/>
-    </row>
-    <row r="240" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A240" s="3" t="s">
+    <row r="242" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B242" s="2"/>
+    </row>
+    <row r="243" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A243" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A242" s="3" t="s">
+    <row r="245" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A245" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B243" s="2"/>
-    </row>
-    <row r="244" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A244" s="8" t="s">
+    <row r="246" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B246" s="2"/>
+    </row>
+    <row r="247" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A247" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B244" s="2"/>
-    </row>
-    <row r="245" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B245" s="2"/>
-    </row>
-    <row r="246" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A246" s="3" t="s">
+      <c r="B247" s="2"/>
+    </row>
+    <row r="248" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B248" s="2"/>
+    </row>
+    <row r="249" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A249" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="247" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A247" s="1"/>
-      <c r="B247" s="2"/>
-    </row>
-    <row r="248" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A248" s="3" t="s">
+    <row r="250" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A250" s="1"/>
+      <c r="B250" s="2"/>
+    </row>
+    <row r="251" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A251" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="250" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A250" s="3" t="s">
+    <row r="253" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A253" s="3" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adds error handling to controllers and daos
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{986A775C-F911-4951-8B19-FA9110858A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C436E98-4C11-4B6F-BBC8-513AA01C6CF8}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{986A775C-F911-4951-8B19-FA9110858A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{941A3457-7CAD-404B-BA3D-5E294E2E8F27}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -430,13 +430,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>219</xdr:row>
+      <xdr:row>217</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>233</xdr:row>
+      <xdr:row>231</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -491,13 +491,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
-      <xdr:row>187</xdr:row>
+      <xdr:row>185</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3295762</xdr:colOff>
-      <xdr:row>207</xdr:row>
+      <xdr:row>205</xdr:row>
       <xdr:rowOff>1595</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -535,13 +535,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1809525</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>94</xdr:row>
       <xdr:rowOff>193411</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -856,10 +856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G253"/>
+  <dimension ref="A1:G251"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -873,27 +873,27 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>82</v>
+      <c r="A2" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>87</v>
+      <c r="A6" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="B6" s="2"/>
     </row>
@@ -902,8 +902,8 @@
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>77</v>
+      <c r="A8" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="B8" s="2"/>
     </row>
@@ -913,7 +913,7 @@
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B10" s="2"/>
     </row>
@@ -921,9 +921,9 @@
       <c r="A11" s="3"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>73</v>
+    <row r="12" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A12" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="B12" s="2"/>
     </row>
@@ -931,9 +931,9 @@
       <c r="A13" s="3"/>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A14" s="4" t="s">
-        <v>74</v>
+    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="B14" s="2"/>
     </row>
@@ -943,7 +943,7 @@
     </row>
     <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B16" s="2"/>
     </row>
@@ -952,21 +952,21 @@
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
+      <c r="A19" t="s">
+        <v>78</v>
+      </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
       <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>78</v>
+      <c r="A21" s="14" t="s">
+        <v>79</v>
       </c>
       <c r="B21" s="2"/>
     </row>
@@ -975,9 +975,7 @@
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="14" t="s">
-        <v>79</v>
-      </c>
+      <c r="A23" s="3"/>
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1009,11 +1007,13 @@
       <c r="B30" s="2"/>
     </row>
     <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="3"/>
+      <c r="A31" s="1"/>
       <c r="B31" s="2"/>
     </row>
     <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="3"/>
+      <c r="A32" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="B32" s="2"/>
     </row>
     <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -1021,9 +1021,7 @@
       <c r="B33" s="2"/>
     </row>
     <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="A34" s="1"/>
       <c r="B34" s="2"/>
     </row>
     <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -1047,56 +1045,56 @@
       <c r="B39" s="2"/>
     </row>
     <row r="40" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
+      <c r="A40" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="B40" s="2"/>
     </row>
     <row r="41" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="1"/>
+      <c r="A41" s="3"/>
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
-        <v>81</v>
+    <row r="42" spans="1:3" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="3"/>
+    <row r="43" spans="1:3" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:3" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>40</v>
+    <row r="44" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="1:3" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
-      <c r="B45" s="2"/>
-    </row>
-    <row r="46" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B46" s="2"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="11" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="47" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="2"/>
     </row>
-    <row r="48" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="11" t="s">
-        <v>42</v>
-      </c>
+    <row r="48" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="13"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="2"/>
     </row>
     <row r="49" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="2"/>
     </row>
     <row r="50" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="13"/>
       <c r="B50" s="1"/>
       <c r="C50" s="2"/>
     </row>
@@ -1113,178 +1111,178 @@
       <c r="C53" s="2"/>
     </row>
     <row r="54" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B54" s="1"/>
-      <c r="C54" s="2"/>
+      <c r="B54" s="2"/>
     </row>
     <row r="55" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B55" s="1"/>
-      <c r="C55" s="2"/>
+      <c r="B55" s="2"/>
     </row>
     <row r="56" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B56" s="2"/>
     </row>
     <row r="57" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="10" t="s">
+        <v>44</v>
+      </c>
       <c r="B57" s="2"/>
     </row>
     <row r="58" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="1"/>
       <c r="B58" s="2"/>
     </row>
     <row r="59" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="10" t="s">
-        <v>44</v>
-      </c>
+      <c r="A59" s="1"/>
       <c r="B59" s="2"/>
     </row>
     <row r="60" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
-      <c r="B60" s="2"/>
     </row>
     <row r="61" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
-      <c r="B61" s="2"/>
     </row>
     <row r="62" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
+      <c r="B62" s="2"/>
     </row>
     <row r="63" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
+      <c r="B63" s="2"/>
     </row>
     <row r="64" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="1"/>
-      <c r="B64" s="2"/>
-    </row>
-    <row r="65" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="3"/>
+      <c r="B64" s="8"/>
+    </row>
+    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="2"/>
     </row>
-    <row r="66" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
-      <c r="B66" s="8"/>
-    </row>
-    <row r="67" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B66" s="2"/>
+    </row>
+    <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
-      <c r="B67" s="2"/>
-    </row>
-    <row r="68" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A68" s="3"/>
-      <c r="B68" s="2"/>
-    </row>
-    <row r="69" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="1"/>
-    </row>
-    <row r="72" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="9" t="s">
+    </row>
+    <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="9" t="s">
         <v>38</v>
       </c>
+      <c r="B70" s="2"/>
+    </row>
+    <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A71" s="9"/>
+      <c r="B71" s="2"/>
+    </row>
+    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="9"/>
       <c r="B72" s="2"/>
     </row>
-    <row r="73" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="9"/>
       <c r="B73" s="2"/>
     </row>
-    <row r="74" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="9"/>
       <c r="B74" s="2"/>
     </row>
-    <row r="75" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="9"/>
+    <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="B75" s="2"/>
     </row>
-    <row r="76" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="9"/>
       <c r="B76" s="2"/>
     </row>
-    <row r="77" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="B77" s="2"/>
     </row>
-    <row r="78" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="9"/>
+    <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="3"/>
       <c r="B78" s="2"/>
     </row>
-    <row r="79" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A79" s="3" t="s">
-        <v>61</v>
+    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>33</v>
       </c>
       <c r="B79" s="2"/>
-    </row>
-    <row r="80" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A80" s="3"/>
+      <c r="G79" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="1"/>
       <c r="B80" s="2"/>
     </row>
-    <row r="81" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>33</v>
-      </c>
-      <c r="B81" s="2"/>
-      <c r="G81" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="1"/>
+    <row r="81" spans="1:2" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="B82" s="2"/>
     </row>
-    <row r="83" spans="1:7" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A84" s="3" t="s">
-        <v>18</v>
-      </c>
+    <row r="83" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B83" s="2"/>
+    </row>
+    <row r="84" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="1"/>
       <c r="B84" s="2"/>
     </row>
-    <row r="85" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A85" s="7" t="s">
-        <v>16</v>
-      </c>
+    <row r="85" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="1"/>
       <c r="B85" s="2"/>
     </row>
-    <row r="86" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
     </row>
-    <row r="87" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87" s="2"/>
     </row>
-    <row r="88" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="2"/>
     </row>
-    <row r="89" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="2"/>
     </row>
-    <row r="90" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90" s="2"/>
     </row>
-    <row r="91" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="B91" s="2"/>
     </row>
-    <row r="92" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="B92" s="2"/>
     </row>
-    <row r="93" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
       <c r="B93" s="2"/>
     </row>
-    <row r="94" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
       <c r="B94" s="2"/>
     </row>
-    <row r="95" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
     </row>
-    <row r="96" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
     </row>
@@ -1297,105 +1295,107 @@
       <c r="B98" s="2"/>
     </row>
     <row r="99" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A99" s="1"/>
-      <c r="B99" s="2"/>
+      <c r="A99" s="3"/>
     </row>
     <row r="100" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A100" s="1"/>
-      <c r="B100" s="2"/>
-    </row>
-    <row r="101" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A101" s="3"/>
-    </row>
-    <row r="102" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A102" s="8"/>
-    </row>
-    <row r="105" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A105" s="12" t="s">
+      <c r="A100" s="8"/>
+    </row>
+    <row r="103" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A103" s="12" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A104" s="12"/>
+    </row>
+    <row r="105" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A106" s="12"/>
     </row>
-    <row r="107" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A107" s="12"/>
-    </row>
-    <row r="108" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A108" s="12"/>
+    <row r="107" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A107" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A108" s="3" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A111" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A111" s="12"/>
+    </row>
+    <row r="112" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A113" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="B112" s="2"/>
+    </row>
+    <row r="113" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A113" s="3"/>
+      <c r="B113" s="2"/>
     </row>
     <row r="114" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B114" s="2"/>
     </row>
     <row r="115" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A115" s="3"/>
+      <c r="A115" t="s">
+        <v>56</v>
+      </c>
       <c r="B115" s="2"/>
     </row>
     <row r="116" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B116" s="2"/>
     </row>
     <row r="117" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
-        <v>56</v>
+      <c r="A117" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="B117" s="2"/>
     </row>
     <row r="118" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A118" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="A118" s="3"/>
       <c r="B118" s="2"/>
     </row>
     <row r="119" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B119" s="2"/>
-    </row>
-    <row r="120" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A120" s="3"/>
-      <c r="B120" s="2"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A120" s="12"/>
     </row>
     <row r="121" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A122" s="12"/>
     </row>
-    <row r="123" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A123" s="3" t="s">
-        <v>28</v>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
@@ -1403,7 +1403,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
@@ -1411,180 +1411,180 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A128" s="12"/>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="129" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A129" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A130" s="12"/>
+      <c r="B130" s="2"/>
     </row>
     <row r="131" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A132" s="12"/>
+        <v>65</v>
+      </c>
+      <c r="B131" s="2"/>
+    </row>
+    <row r="132" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A132" s="3"/>
       <c r="B132" s="2"/>
     </row>
     <row r="133" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B133" s="2"/>
-    </row>
-    <row r="134" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A134" s="3"/>
-      <c r="B134" s="2"/>
-    </row>
-    <row r="135" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A134" s="12"/>
+    </row>
+    <row r="135" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.7">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A136" s="12"/>
     </row>
-    <row r="137" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A138" s="12"/>
     </row>
-    <row r="139" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A140" s="12"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A140" s="3"/>
     </row>
     <row r="141" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A142" s="3"/>
-    </row>
-    <row r="143" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A142" s="12"/>
+    </row>
+    <row r="143" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A144" s="12"/>
     </row>
-    <row r="145" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A146" s="12"/>
     </row>
-    <row r="147" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A148" s="12"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="149" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A149" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="3"/>
+      <c r="B149" s="2"/>
+    </row>
+    <row r="150" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A151" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="B150" s="2"/>
+    </row>
+    <row r="151" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A151" s="12"/>
       <c r="B151" s="2"/>
     </row>
     <row r="152" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A152" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B152" s="2"/>
-    </row>
-    <row r="153" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A153" s="12"/>
-      <c r="B153" s="2"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A153" s="3"/>
     </row>
     <row r="154" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A154" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A155" s="3"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A155" s="4"/>
     </row>
     <row r="156" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A156" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A157" s="4"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B157" s="2"/>
     </row>
     <row r="158" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="B158" s="2"/>
+    </row>
+    <row r="159" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A159" s="4"/>
       <c r="B159" s="2"/>
     </row>
     <row r="160" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A160" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B160" s="2"/>
-    </row>
-    <row r="161" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A161" s="4"/>
-      <c r="B161" s="2"/>
-    </row>
-    <row r="162" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A162" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A163" s="3"/>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A164" t="s">
+    <row r="161" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A161" s="3"/>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A165" s="4"/>
+    <row r="163" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A163" s="4"/>
+    </row>
+    <row r="164" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A164" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A165" s="3"/>
     </row>
     <row r="166" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A166" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A167" s="3"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A167" s="4"/>
     </row>
     <row r="168" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A168" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="21" x14ac:dyDescent="0.4">
@@ -1592,34 +1592,36 @@
     </row>
     <row r="170" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A170" s="3" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A171" s="4"/>
+      <c r="B171" s="2"/>
     </row>
     <row r="172" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A172" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A173" s="4"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A173" s="3"/>
       <c r="B173" s="2"/>
     </row>
     <row r="174" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A174" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A175" s="3"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A175" s="4"/>
       <c r="B175" s="2"/>
     </row>
     <row r="176" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A176" s="3" t="s">
-        <v>14</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B176" s="2"/>
     </row>
     <row r="177" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A177" s="4"/>
@@ -1627,66 +1629,65 @@
     </row>
     <row r="178" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A178" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B178" s="2"/>
-    </row>
-    <row r="179" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A179" s="4"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A179" s="3"/>
       <c r="B179" s="2"/>
     </row>
-    <row r="180" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A180" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A181" s="3"/>
-      <c r="B181" s="2"/>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A182" t="s">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A184" s="3" t="s">
+    <row r="182" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A182" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A186" t="s">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="207" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B205" s="2"/>
+    </row>
+    <row r="207" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B207" s="2"/>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="209" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B209" s="2"/>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B210" s="2"/>
     </row>
     <row r="211" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B211" s="2"/>
     </row>
     <row r="212" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A212" t="s">
-        <v>1</v>
+      <c r="A212" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="B212" s="2"/>
     </row>
     <row r="213" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A213" s="3"/>
       <c r="B213" s="2"/>
     </row>
     <row r="214" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A214" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B214" s="2"/>
+        <v>20</v>
+      </c>
     </row>
     <row r="215" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A215" s="3"/>
@@ -1694,65 +1695,64 @@
     </row>
     <row r="216" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A216" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="217" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A217" s="3"/>
-      <c r="B217" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="B216" s="2"/>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B217" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="218" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A218" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B218" s="2"/>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B219" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A220" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="221" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A221" s="1"/>
+    <row r="219" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A219" s="1"/>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A222" s="5"/>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A223" s="5"/>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" s="5"/>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A225" s="5"/>
+      <c r="A225" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A226" s="5"/>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A226" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A227" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A228" s="5" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B227" s="2"/>
+    </row>
+    <row r="228" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A228" s="5"/>
+      <c r="B228" s="2"/>
     </row>
     <row r="229" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A229" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B229" s="2"/>
     </row>
     <row r="230" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A230" s="5"/>
+      <c r="A230" s="1"/>
       <c r="B230" s="2"/>
     </row>
     <row r="231" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A231" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="A231" s="1"/>
       <c r="B231" s="2"/>
     </row>
     <row r="232" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1761,7 +1761,6 @@
     </row>
     <row r="233" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A233" s="1"/>
-      <c r="B233" s="2"/>
     </row>
     <row r="234" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A234" s="1"/>
@@ -1771,18 +1770,19 @@
       <c r="A235" s="1"/>
     </row>
     <row r="236" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A236" s="1"/>
       <c r="B236" s="2"/>
     </row>
     <row r="237" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A237" s="1"/>
+      <c r="A237" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="238" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B238" s="2"/>
     </row>
     <row r="239" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A239" s="3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1790,50 +1790,42 @@
     </row>
     <row r="241" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A241" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="242" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B242" s="2"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="243" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A243" s="3" t="s">
-        <v>13</v>
-      </c>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B244" s="2"/>
     </row>
     <row r="245" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A245" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="A245" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B245" s="2"/>
     </row>
     <row r="246" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B246" s="2"/>
     </row>
     <row r="247" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A247" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B247" s="2"/>
+      <c r="A247" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="248" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A248" s="1"/>
       <c r="B248" s="2"/>
     </row>
     <row r="249" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A249" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A250" s="1"/>
-      <c r="B250" s="2"/>
+        <v>27</v>
+      </c>
     </row>
     <row r="251" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A251" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A253" s="3" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adds executor service to employee form controller
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{986A775C-F911-4951-8B19-FA9110858A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{941A3457-7CAD-404B-BA3D-5E294E2E8F27}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{986A775C-F911-4951-8B19-FA9110858A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93AB201D-1263-4D9B-A0F9-1B6CADC147DF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -430,13 +430,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>217</xdr:row>
+      <xdr:row>209</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>231</xdr:row>
+      <xdr:row>223</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -491,13 +491,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
-      <xdr:row>185</xdr:row>
+      <xdr:row>177</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3295762</xdr:colOff>
-      <xdr:row>205</xdr:row>
+      <xdr:row>197</xdr:row>
       <xdr:rowOff>1595</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -535,13 +535,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1809525</xdr:colOff>
-      <xdr:row>94</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>193411</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -856,10 +856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G251"/>
+  <dimension ref="A1:G243"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -892,9 +892,7 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>77</v>
-      </c>
+      <c r="A6" s="3"/>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -902,8 +900,8 @@
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>72</v>
+      <c r="A8" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="B8" s="2"/>
     </row>
@@ -913,7 +911,7 @@
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10" s="2"/>
     </row>
@@ -921,9 +919,9 @@
       <c r="A11" s="3"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A12" s="4" t="s">
-        <v>74</v>
+    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="B12" s="2"/>
     </row>
@@ -931,9 +929,9 @@
       <c r="A13" s="3"/>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>75</v>
+    <row r="14" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A14" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="B14" s="2"/>
     </row>
@@ -943,7 +941,7 @@
     </row>
     <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" s="2"/>
     </row>
@@ -952,21 +950,21 @@
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="3"/>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>78</v>
-      </c>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="14" t="s">
-        <v>79</v>
       </c>
       <c r="B21" s="2"/>
     </row>
@@ -975,7 +973,9 @@
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
+      <c r="A23" s="14" t="s">
+        <v>79</v>
+      </c>
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -987,23 +987,25 @@
       <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
+      <c r="A26" s="1"/>
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
+      <c r="A27" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
+      <c r="A28" s="1"/>
       <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
+      <c r="A29" s="1"/>
       <c r="B29" s="2"/>
     </row>
     <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="3"/>
+      <c r="A30" s="1"/>
       <c r="B30" s="2"/>
     </row>
     <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1011,227 +1013,225 @@
       <c r="B31" s="2"/>
     </row>
     <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>43</v>
+      <c r="A32" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="B32" s="2"/>
     </row>
     <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
+      <c r="A33" s="3"/>
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
+    <row r="34" spans="1:3" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B34" s="2"/>
     </row>
-    <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
     </row>
     <row r="36" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
+      <c r="A36" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="B36" s="2"/>
     </row>
     <row r="37" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
-      <c r="B38" s="2"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="11" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
-      <c r="B39" s="2"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="2"/>
     </row>
     <row r="40" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B40" s="2"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="2"/>
     </row>
     <row r="41" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="3"/>
-      <c r="B41" s="2"/>
-    </row>
-    <row r="42" spans="1:3" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B42" s="2"/>
-    </row>
-    <row r="43" spans="1:3" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="1"/>
-      <c r="B43" s="2"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B42" s="1"/>
+      <c r="C42" s="2"/>
+    </row>
+    <row r="43" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B43" s="1"/>
+      <c r="C43" s="2"/>
     </row>
     <row r="44" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B44" s="2"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="2"/>
     </row>
     <row r="45" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="11" t="s">
-        <v>42</v>
-      </c>
+    <row r="46" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B46" s="2"/>
     </row>
     <row r="47" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="2"/>
+      <c r="B47" s="2"/>
     </row>
     <row r="48" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="13"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="2"/>
-    </row>
-    <row r="49" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B49" s="1"/>
-      <c r="C49" s="2"/>
-    </row>
-    <row r="50" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B50" s="1"/>
-      <c r="C50" s="2"/>
-    </row>
-    <row r="51" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B51" s="1"/>
-      <c r="C51" s="2"/>
-    </row>
-    <row r="52" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B52" s="1"/>
-      <c r="C52" s="2"/>
-    </row>
-    <row r="53" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B53" s="1"/>
-      <c r="C53" s="2"/>
-    </row>
-    <row r="54" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B48" s="2"/>
+    </row>
+    <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B49" s="2"/>
+    </row>
+    <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+      <c r="B50" s="2"/>
+    </row>
+    <row r="51" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="1"/>
+      <c r="B51" s="2"/>
+    </row>
+    <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="1"/>
+    </row>
+    <row r="53" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
+    </row>
+    <row r="54" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="1"/>
       <c r="B54" s="2"/>
     </row>
-    <row r="55" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="1"/>
       <c r="B55" s="2"/>
     </row>
-    <row r="56" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B56" s="2"/>
-    </row>
-    <row r="57" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="10" t="s">
-        <v>44</v>
-      </c>
+    <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="3"/>
+      <c r="B56" s="8"/>
+    </row>
+    <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="1"/>
       <c r="B57" s="2"/>
     </row>
-    <row r="58" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="1"/>
+    <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="3"/>
       <c r="B58" s="2"/>
     </row>
-    <row r="59" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
-      <c r="B59" s="2"/>
-    </row>
-    <row r="60" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="1"/>
-    </row>
-    <row r="61" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="1"/>
-    </row>
-    <row r="62" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="1"/>
+    </row>
+    <row r="62" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="B62" s="2"/>
     </row>
-    <row r="63" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="1"/>
+    <row r="63" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="9"/>
       <c r="B63" s="2"/>
     </row>
-    <row r="64" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="3"/>
-      <c r="B64" s="8"/>
+    <row r="64" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="9"/>
+      <c r="B64" s="2"/>
     </row>
     <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="1"/>
+      <c r="A65" s="9"/>
       <c r="B65" s="2"/>
     </row>
     <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="3"/>
+      <c r="A66" s="9"/>
       <c r="B66" s="2"/>
     </row>
     <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="1"/>
+      <c r="A67" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B67" s="2"/>
+    </row>
+    <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="9"/>
+      <c r="B68" s="2"/>
+    </row>
+    <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B69" s="2"/>
     </row>
     <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="9" t="s">
-        <v>38</v>
-      </c>
+      <c r="A70" s="3"/>
       <c r="B70" s="2"/>
     </row>
     <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A71" s="9"/>
+      <c r="A71" t="s">
+        <v>33</v>
+      </c>
       <c r="B71" s="2"/>
+      <c r="G71" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="9"/>
+      <c r="A72" s="1"/>
       <c r="B72" s="2"/>
     </row>
-    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="9"/>
-      <c r="B73" s="2"/>
+    <row r="73" spans="1:7" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="9"/>
+      <c r="A74" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="B74" s="2"/>
     </row>
     <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="3" t="s">
-        <v>80</v>
+      <c r="A75" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="B75" s="2"/>
     </row>
     <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="9"/>
+      <c r="A76" s="1"/>
       <c r="B76" s="2"/>
     </row>
     <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="A77" s="1"/>
       <c r="B77" s="2"/>
     </row>
     <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="3"/>
+      <c r="A78" s="1"/>
       <c r="B78" s="2"/>
     </row>
     <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>33</v>
-      </c>
+      <c r="A79" s="1"/>
       <c r="B79" s="2"/>
-      <c r="G79" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
     </row>
-    <row r="81" spans="1:2" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A81" s="3" t="s">
-        <v>15</v>
-      </c>
+    <row r="81" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="1"/>
+      <c r="B81" s="2"/>
     </row>
     <row r="82" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="A82" s="1"/>
       <c r="B82" s="2"/>
     </row>
     <row r="83" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="7" t="s">
-        <v>16</v>
-      </c>
+      <c r="A83" s="1"/>
       <c r="B83" s="2"/>
     </row>
     <row r="84" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1263,198 +1263,198 @@
       <c r="B90" s="2"/>
     </row>
     <row r="91" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A91" s="1"/>
-      <c r="B91" s="2"/>
+      <c r="A91" s="3"/>
     </row>
     <row r="92" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A92" s="1"/>
-      <c r="B92" s="2"/>
-    </row>
-    <row r="93" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A93" s="1"/>
-      <c r="B93" s="2"/>
-    </row>
-    <row r="94" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A94" s="1"/>
-      <c r="B94" s="2"/>
-    </row>
-    <row r="95" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A95" s="1"/>
-      <c r="B95" s="2"/>
-    </row>
-    <row r="96" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A96" s="1"/>
-      <c r="B96" s="2"/>
-    </row>
-    <row r="97" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A97" s="1"/>
-      <c r="B97" s="2"/>
-    </row>
-    <row r="98" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A98" s="1"/>
-      <c r="B98" s="2"/>
+      <c r="A92" s="8"/>
+    </row>
+    <row r="95" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A95" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A96" s="12"/>
+    </row>
+    <row r="97" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A98" s="12"/>
     </row>
     <row r="99" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A99" s="3"/>
+      <c r="A99" s="3" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="100" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A100" s="8"/>
-    </row>
-    <row r="103" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A103" s="12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A104" s="12"/>
-    </row>
-    <row r="105" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A106" s="12"/>
+      <c r="A100" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A101" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A103" s="12"/>
+    </row>
+    <row r="104" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A104" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B104" s="2"/>
+    </row>
+    <row r="105" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A105" s="3"/>
+      <c r="B105" s="2"/>
+    </row>
+    <row r="106" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A106" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B106" s="2"/>
     </row>
     <row r="107" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A107" s="3" t="s">
-        <v>83</v>
-      </c>
+      <c r="A107" t="s">
+        <v>56</v>
+      </c>
+      <c r="B107" s="2"/>
     </row>
     <row r="108" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
-        <v>84</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B108" s="2"/>
     </row>
     <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A111" s="12"/>
-    </row>
-    <row r="112" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A112" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B112" s="2"/>
+        <v>57</v>
+      </c>
+      <c r="B109" s="2"/>
+    </row>
+    <row r="110" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A110" s="3"/>
+      <c r="B110" s="2"/>
+    </row>
+    <row r="111" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A111" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A112" s="12"/>
     </row>
     <row r="113" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A113" s="3"/>
-      <c r="B113" s="2"/>
-    </row>
-    <row r="114" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A114" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B114" s="2"/>
-    </row>
-    <row r="115" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A113" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A114" s="12"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>56</v>
-      </c>
-      <c r="B115" s="2"/>
-    </row>
-    <row r="116" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A116" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B116" s="2"/>
-    </row>
-    <row r="117" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A117" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B117" s="2"/>
-    </row>
-    <row r="118" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A118" s="3"/>
-      <c r="B118" s="2"/>
-    </row>
-    <row r="119" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A119" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A116" s="12"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A118" s="12"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A120" s="12"/>
     </row>
     <row r="121" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A122" s="12"/>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A124" s="12"/>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A125" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="B122" s="2"/>
+    </row>
+    <row r="123" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A123" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B123" s="2"/>
+    </row>
+    <row r="124" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A124" s="3"/>
+      <c r="B124" s="2"/>
+    </row>
+    <row r="125" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A125" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A126" s="12"/>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="127" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A128" s="12"/>
     </row>
-    <row r="129" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A130" s="12"/>
-      <c r="B130" s="2"/>
     </row>
     <row r="131" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B131" s="2"/>
+        <v>63</v>
+      </c>
     </row>
     <row r="132" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A132" s="3"/>
-      <c r="B132" s="2"/>
     </row>
     <row r="133" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.7">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A134" s="12"/>
     </row>
     <row r="135" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A136" s="12"/>
     </row>
-    <row r="137" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
@@ -1462,71 +1462,73 @@
     </row>
     <row r="139" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A140" s="3"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="141" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A141" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A142" s="12"/>
-    </row>
-    <row r="143" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A144" s="12"/>
-    </row>
-    <row r="145" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A146" s="12"/>
-    </row>
-    <row r="147" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A147" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="3"/>
+      <c r="B141" s="2"/>
+    </row>
+    <row r="142" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A142" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B142" s="2"/>
+    </row>
+    <row r="143" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A143" s="12"/>
+      <c r="B143" s="2"/>
+    </row>
+    <row r="144" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A144" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A145" s="3"/>
+    </row>
+    <row r="146" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A146" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A147" s="4"/>
+    </row>
+    <row r="148" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A149" s="3"/>
       <c r="B149" s="2"/>
     </row>
     <row r="150" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B150" s="2"/>
     </row>
-    <row r="151" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A151" s="12"/>
+    <row r="151" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A151" s="4"/>
       <c r="B151" s="2"/>
     </row>
     <row r="152" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A152" s="3" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A153" s="3"/>
     </row>
-    <row r="154" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A154" s="3" t="s">
-        <v>49</v>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="21" x14ac:dyDescent="0.4">
@@ -1534,298 +1536,264 @@
     </row>
     <row r="156" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A156" s="3" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B157" s="2"/>
+      <c r="A157" s="3"/>
     </row>
     <row r="158" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B158" s="2"/>
+        <v>47</v>
+      </c>
     </row>
     <row r="159" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A159" s="4"/>
-      <c r="B159" s="2"/>
     </row>
     <row r="160" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A160" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A161" s="3"/>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A162" t="s">
-        <v>32</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A161" s="4"/>
+    </row>
+    <row r="162" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A162" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A163" s="4"/>
+      <c r="B163" s="2"/>
     </row>
     <row r="164" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A164" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A165" s="3"/>
+      <c r="B165" s="2"/>
     </row>
     <row r="166" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A166" s="3" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A167" s="4"/>
+      <c r="B167" s="2"/>
     </row>
     <row r="168" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A168" s="3" t="s">
-        <v>37</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B168" s="2"/>
     </row>
     <row r="169" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A169" s="4"/>
+      <c r="B169" s="2"/>
     </row>
     <row r="170" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A170" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A171" s="4"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A171" s="3"/>
       <c r="B171" s="2"/>
     </row>
-    <row r="172" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A172" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A173" s="3"/>
-      <c r="B173" s="2"/>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="174" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A174" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A175" s="4"/>
-      <c r="B175" s="2"/>
-    </row>
-    <row r="176" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A176" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B176" s="2"/>
-    </row>
-    <row r="177" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A177" s="4"/>
-      <c r="B177" s="2"/>
-    </row>
-    <row r="178" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A178" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A179" s="3"/>
-      <c r="B179" s="2"/>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A180" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A182" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A184" t="s">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
         <v>24</v>
       </c>
     </row>
+    <row r="197" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B197" s="2"/>
+    </row>
+    <row r="199" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B199" s="2"/>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B201" s="2"/>
+    </row>
+    <row r="202" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>1</v>
+      </c>
+      <c r="B202" s="2"/>
+    </row>
+    <row r="203" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B203" s="2"/>
+    </row>
+    <row r="204" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A204" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B204" s="2"/>
+    </row>
     <row r="205" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A205" s="3"/>
       <c r="B205" s="2"/>
     </row>
+    <row r="206" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A206" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="207" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A207" s="3"/>
       <c r="B207" s="2"/>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A208" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B209" s="2"/>
+    <row r="208" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A208" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B208" s="2"/>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B209" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="210" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A210" t="s">
-        <v>1</v>
-      </c>
-      <c r="B210" s="2"/>
+      <c r="A210" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="211" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B211" s="2"/>
-    </row>
-    <row r="212" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A212" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B212" s="2"/>
-    </row>
-    <row r="213" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A213" s="3"/>
-      <c r="B213" s="2"/>
-    </row>
-    <row r="214" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A214" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A215" s="3"/>
-      <c r="B215" s="2"/>
-    </row>
-    <row r="216" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A216" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B216" s="2"/>
+      <c r="A211" s="1"/>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A214" s="5"/>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A215" s="5"/>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A216" s="5"/>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B217" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A218" s="3" t="s">
-        <v>5</v>
+      <c r="A217" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A218" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A219" s="1"/>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A222" s="5"/>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A223" s="5"/>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A224" s="5"/>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A225" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A226" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="A219" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B219" s="2"/>
+    </row>
+    <row r="220" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A220" s="5"/>
+      <c r="B220" s="2"/>
+    </row>
+    <row r="221" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A221" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B221" s="2"/>
+    </row>
+    <row r="222" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A222" s="1"/>
+      <c r="B222" s="2"/>
+    </row>
+    <row r="223" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A223" s="1"/>
+      <c r="B223" s="2"/>
+    </row>
+    <row r="224" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A224" s="1"/>
+      <c r="B224" s="2"/>
+    </row>
+    <row r="225" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A225" s="1"/>
+    </row>
+    <row r="226" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A226" s="1"/>
+      <c r="B226" s="2"/>
     </row>
     <row r="227" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A227" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B227" s="2"/>
+      <c r="A227" s="1"/>
     </row>
     <row r="228" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A228" s="5"/>
       <c r="B228" s="2"/>
     </row>
     <row r="229" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A229" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B229" s="2"/>
+      <c r="A229" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="230" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A230" s="1"/>
       <c r="B230" s="2"/>
     </row>
     <row r="231" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A231" s="1"/>
-      <c r="B231" s="2"/>
+      <c r="A231" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="232" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A232" s="1"/>
       <c r="B232" s="2"/>
     </row>
     <row r="233" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A233" s="1"/>
-    </row>
-    <row r="234" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A234" s="1"/>
-      <c r="B234" s="2"/>
+      <c r="A233" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="235" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A235" s="1"/>
+      <c r="A235" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="236" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B236" s="2"/>
     </row>
     <row r="237" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A237" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="A237" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B237" s="2"/>
     </row>
     <row r="238" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B238" s="2"/>
     </row>
     <row r="239" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A239" s="3" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A240" s="1"/>
       <c r="B240" s="2"/>
     </row>
-    <row r="241" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A241" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="243" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A243" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B244" s="2"/>
-    </row>
-    <row r="245" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A245" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B245" s="2"/>
-    </row>
-    <row r="246" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B246" s="2"/>
-    </row>
-    <row r="247" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A247" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A248" s="1"/>
-      <c r="B248" s="2"/>
-    </row>
-    <row r="249" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A249" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A251" s="3" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adds executor service to set employee to inactive
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{986A775C-F911-4951-8B19-FA9110858A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93AB201D-1263-4D9B-A0F9-1B6CADC147DF}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{986A775C-F911-4951-8B19-FA9110858A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{298F4977-5B26-4FD1-A6BA-35CCCE03C46E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>Scope, Nicht-Scope, funktionale Anforderungen( habe ich schon), nicht funktionale Anforderungen, Overview Ziel reinschreiben, Benutzerschnittstellen sind einzelne Windows,</t>
   </si>
@@ -153,9 +153,6 @@
   </si>
   <si>
     <t xml:space="preserve">Gegen Ende: </t>
-  </si>
-  <si>
-    <t>ExecutorService mit einem Singelton Provider Pattern der ganzen App zur Verfügung stellen und in der zentralen Stopp Methode beim Shutdown schließen</t>
   </si>
   <si>
     <t xml:space="preserve">Statt dem FetchType Eager Loading - folgendes machen: </t>
@@ -304,7 +301,7 @@
     <t>5.Admins can only create other adminss</t>
   </si>
   <si>
-    <t>Schauen wo Exekutor Service noch fehlt oder nicht und einbauen - bzw austauschen</t>
+    <t xml:space="preserve">Executor Service noch in CRUD Service verbinden und </t>
   </si>
 </sst>
 </file>
@@ -535,13 +532,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>79</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1809525</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>193411</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -858,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -874,7 +871,7 @@
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>86</v>
       </c>
       <c r="B2" s="2"/>
     </row>
@@ -882,9 +879,7 @@
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>87</v>
-      </c>
+      <c r="A4" s="3"/>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -901,7 +896,7 @@
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B8" s="2"/>
     </row>
@@ -911,7 +906,7 @@
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" s="2"/>
     </row>
@@ -921,7 +916,7 @@
     </row>
     <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" s="2"/>
     </row>
@@ -931,7 +926,7 @@
     </row>
     <row r="14" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14" s="2"/>
     </row>
@@ -941,7 +936,7 @@
     </row>
     <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16" s="2"/>
     </row>
@@ -951,7 +946,7 @@
     </row>
     <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B18" s="2"/>
     </row>
@@ -963,23 +958,18 @@
       <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>78</v>
-      </c>
       <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="14" t="s">
-        <v>79</v>
-      </c>
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
+      <c r="A24" t="s">
+        <v>77</v>
+      </c>
       <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -987,17 +977,17 @@
       <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
+      <c r="A26" s="14" t="s">
+        <v>78</v>
+      </c>
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="A27" s="3"/>
       <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
+      <c r="A28" s="3"/>
       <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1005,7 +995,9 @@
       <c r="B29" s="2"/>
     </row>
     <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="B30" s="2"/>
     </row>
     <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1013,60 +1005,60 @@
       <c r="B31" s="2"/>
     </row>
     <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>81</v>
-      </c>
+      <c r="A32" s="1"/>
       <c r="B32" s="2"/>
     </row>
     <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
+      <c r="A33" s="1"/>
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="1:3" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="3"/>
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38" spans="1:3" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="2"/>
+    </row>
+    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="1:3" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
-      <c r="B35" s="2"/>
-    </row>
-    <row r="36" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B36" s="2"/>
-    </row>
-    <row r="37" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="2"/>
-    </row>
-    <row r="38" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="2"/>
+      <c r="B39" s="2"/>
     </row>
     <row r="40" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="13"/>
+      <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="2"/>
     </row>
-    <row r="41" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B41" s="1"/>
-      <c r="C41" s="2"/>
+    <row r="41" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="11" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="42" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="2"/>
     </row>
     <row r="43" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="13"/>
       <c r="B43" s="1"/>
       <c r="C43" s="2"/>
     </row>
@@ -1079,33 +1071,35 @@
       <c r="C45" s="2"/>
     </row>
     <row r="46" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B46" s="2"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="2"/>
     </row>
     <row r="47" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B47" s="2"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="2"/>
     </row>
     <row r="48" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B48" s="2"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="2"/>
     </row>
     <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="B49" s="2"/>
     </row>
     <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="1"/>
       <c r="B50" s="2"/>
     </row>
     <row r="51" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="1"/>
       <c r="B51" s="2"/>
     </row>
     <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="1"/>
+      <c r="A52" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B52" s="2"/>
     </row>
     <row r="53" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
+      <c r="B53" s="2"/>
     </row>
     <row r="54" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
@@ -1113,39 +1107,37 @@
     </row>
     <row r="55" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
-      <c r="B55" s="2"/>
     </row>
     <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="3"/>
-      <c r="B56" s="8"/>
+      <c r="A56" s="1"/>
     </row>
     <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
     </row>
     <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="3"/>
+      <c r="A58" s="1"/>
       <c r="B58" s="2"/>
     </row>
     <row r="59" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="1"/>
+      <c r="A59" s="3"/>
+      <c r="B59" s="8"/>
+    </row>
+    <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="1"/>
+      <c r="B60" s="2"/>
+    </row>
+    <row r="61" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="3"/>
+      <c r="B61" s="2"/>
     </row>
     <row r="62" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="9" t="s">
+      <c r="A62" s="1"/>
+    </row>
+    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B62" s="2"/>
-    </row>
-    <row r="63" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="9"/>
-      <c r="B63" s="2"/>
-    </row>
-    <row r="64" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="9"/>
-      <c r="B64" s="2"/>
-    </row>
-    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="9"/>
       <c r="B65" s="2"/>
     </row>
     <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1153,9 +1145,7 @@
       <c r="B66" s="2"/>
     </row>
     <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="A67" s="9"/>
       <c r="B67" s="2"/>
     </row>
     <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1163,55 +1153,57 @@
       <c r="B68" s="2"/>
     </row>
     <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="A69" s="9"/>
       <c r="B69" s="2"/>
     </row>
     <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="3"/>
+      <c r="A70" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="B70" s="2"/>
     </row>
     <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+      <c r="A71" s="9"/>
+      <c r="B71" s="2"/>
+    </row>
+    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B72" s="2"/>
+    </row>
+    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="3"/>
+      <c r="B73" s="2"/>
+    </row>
+    <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>33</v>
       </c>
-      <c r="B71" s="2"/>
-      <c r="G71" t="s">
+      <c r="B74" s="2"/>
+      <c r="G74" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="1"/>
-      <c r="B72" s="2"/>
-    </row>
-    <row r="73" spans="1:7" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="3" t="s">
+    <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="1"/>
+      <c r="B75" s="2"/>
+    </row>
+    <row r="76" spans="1:7" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="3" t="s">
+    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B74" s="2"/>
-    </row>
-    <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="7" t="s">
+      <c r="B77" s="2"/>
+    </row>
+    <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B75" s="2"/>
-    </row>
-    <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="1"/>
-      <c r="B76" s="2"/>
-    </row>
-    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="1"/>
-      <c r="B77" s="2"/>
-    </row>
-    <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="1"/>
       <c r="B78" s="2"/>
     </row>
     <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1263,10 +1255,16 @@
       <c r="B90" s="2"/>
     </row>
     <row r="91" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A91" s="3"/>
+      <c r="A91" s="1"/>
+      <c r="B91" s="2"/>
     </row>
     <row r="92" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A92" s="8"/>
+      <c r="A92" s="1"/>
+      <c r="B92" s="2"/>
+    </row>
+    <row r="93" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A93" s="1"/>
+      <c r="B93" s="2"/>
     </row>
     <row r="95" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A95" s="12" t="s">
@@ -1276,9 +1274,9 @@
     <row r="96" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A96" s="12"/>
     </row>
-    <row r="97" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
@@ -1286,22 +1284,22 @@
     </row>
     <row r="99" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.7">
@@ -1309,7 +1307,7 @@
     </row>
     <row r="104" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B104" s="2"/>
     </row>
@@ -1319,25 +1317,25 @@
     </row>
     <row r="106" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B106" s="2"/>
     </row>
     <row r="107" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B107" s="2"/>
     </row>
     <row r="108" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B108" s="2"/>
     </row>
     <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B109" s="2"/>
     </row>
@@ -1347,7 +1345,7 @@
     </row>
     <row r="111" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
@@ -1363,7 +1361,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
@@ -1371,7 +1369,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
@@ -1379,7 +1377,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.7">
@@ -1387,7 +1385,7 @@
     </row>
     <row r="121" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.7">
@@ -1396,7 +1394,7 @@
     </row>
     <row r="123" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B123" s="2"/>
     </row>
@@ -1406,7 +1404,7 @@
     </row>
     <row r="125" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.7">
@@ -1414,7 +1412,7 @@
     </row>
     <row r="127" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.7">
@@ -1422,7 +1420,7 @@
     </row>
     <row r="129" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
@@ -1430,7 +1428,7 @@
     </row>
     <row r="131" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1438,7 +1436,7 @@
     </row>
     <row r="133" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
@@ -1446,7 +1444,7 @@
     </row>
     <row r="135" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
@@ -1454,7 +1452,7 @@
     </row>
     <row r="137" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
@@ -1462,12 +1460,12 @@
     </row>
     <row r="139" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1476,7 +1474,7 @@
     </row>
     <row r="142" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B142" s="2"/>
     </row>
@@ -1486,7 +1484,7 @@
     </row>
     <row r="144" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1494,7 +1492,7 @@
     </row>
     <row r="146" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="21" x14ac:dyDescent="0.4">
@@ -1502,7 +1500,7 @@
     </row>
     <row r="148" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1510,7 +1508,7 @@
     </row>
     <row r="150" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B150" s="2"/>
     </row>
@@ -1544,7 +1542,7 @@
     </row>
     <row r="158" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="21" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
adds executor service to employee crud service
</commit_message>
<xml_diff>
--- a/documentation/ToDo/ToDos.xlsx
+++ b/documentation/ToDo/ToDos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60117414f441014b/Desktop/ProgrammierAnleitung/Java/2025 WIFI/EmployeeAdministration/documentation/ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{986A775C-F911-4951-8B19-FA9110858A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{298F4977-5B26-4FD1-A6BA-35CCCE03C46E}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{986A775C-F911-4951-8B19-FA9110858A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD1F9234-79B1-486D-A812-CE30B985962E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>Scope, Nicht-Scope, funktionale Anforderungen( habe ich schon), nicht funktionale Anforderungen, Overview Ziel reinschreiben, Benutzerschnittstellen sind einzelne Windows,</t>
   </si>
@@ -272,12 +272,6 @@
   </si>
   <si>
     <t>Person entity lengths mit lengths in DB vergleichen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wenn noch Zeit: </t>
-  </si>
-  <si>
-    <t>- Bei Update auf Admin Status. Checken ob es eh keine Mitarbeiter gibt. Falls doch auch Bei Mitarbeitern forgesetzten auf null setzten.</t>
   </si>
   <si>
     <t>Hibernate TODOS durchsuchen</t>
@@ -427,13 +421,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>209</xdr:row>
+      <xdr:row>201</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>223</xdr:row>
+      <xdr:row>215</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -488,13 +482,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>71718</xdr:colOff>
-      <xdr:row>177</xdr:row>
+      <xdr:row>169</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>3295762</xdr:colOff>
-      <xdr:row>197</xdr:row>
+      <xdr:row>189</xdr:row>
       <xdr:rowOff>1595</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -532,13 +526,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>261918</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>96669</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1809525</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:row>79</xdr:row>
       <xdr:rowOff>193411</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -853,10 +847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G243"/>
+  <dimension ref="A1:G235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView tabSelected="1" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -870,16 +864,19 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>86</v>
+      <c r="A2" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -887,16 +884,18 @@
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>76</v>
+    <row r="8" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A8" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="B8" s="2"/>
     </row>
@@ -906,7 +905,7 @@
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B10" s="2"/>
     </row>
@@ -916,7 +915,7 @@
     </row>
     <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B12" s="2"/>
     </row>
@@ -924,10 +923,7 @@
       <c r="A13" s="3"/>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A14" s="4" t="s">
-        <v>73</v>
-      </c>
+    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -935,282 +931,278 @@
       <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>74</v>
-      </c>
+      <c r="A16" s="14"/>
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>75</v>
-      </c>
+    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
+    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:3" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:3" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="13"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B34" s="1"/>
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B35" s="1"/>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B36" s="1"/>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B37" s="1"/>
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B38" s="1"/>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="2"/>
+    </row>
+    <row r="43" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="1"/>
+    </row>
+    <row r="47" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
+      <c r="B48" s="2"/>
+    </row>
+    <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="3"/>
+      <c r="B49" s="8"/>
+    </row>
+    <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+      <c r="B50" s="2"/>
+    </row>
+    <row r="51" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="3"/>
+      <c r="B51" s="2"/>
+    </row>
+    <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="1"/>
+    </row>
+    <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B55" s="2"/>
+    </row>
+    <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="9"/>
+      <c r="B56" s="2"/>
+    </row>
+    <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="9"/>
+      <c r="B57" s="2"/>
+    </row>
+    <row r="58" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="9"/>
+      <c r="B58" s="2"/>
+    </row>
+    <row r="59" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="9"/>
+      <c r="B59" s="2"/>
+    </row>
+    <row r="60" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
-      <c r="B27" s="2"/>
-    </row>
-    <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="2"/>
-    </row>
-    <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B35" s="2"/>
-    </row>
-    <row r="36" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="3"/>
-      <c r="B36" s="2"/>
-    </row>
-    <row r="37" spans="1:3" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="1:3" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
-      <c r="B38" s="2"/>
-    </row>
-    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="2"/>
-    </row>
-    <row r="41" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="2"/>
-    </row>
-    <row r="43" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="13"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="2"/>
-    </row>
-    <row r="44" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B44" s="1"/>
-      <c r="C44" s="2"/>
-    </row>
-    <row r="45" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B45" s="1"/>
-      <c r="C45" s="2"/>
-    </row>
-    <row r="46" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B46" s="1"/>
-      <c r="C46" s="2"/>
-    </row>
-    <row r="47" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B47" s="1"/>
-      <c r="C47" s="2"/>
-    </row>
-    <row r="48" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B48" s="1"/>
-      <c r="C48" s="2"/>
-    </row>
-    <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B50" s="2"/>
-    </row>
-    <row r="51" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B51" s="2"/>
-    </row>
-    <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B52" s="2"/>
-    </row>
-    <row r="53" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="1"/>
-      <c r="B53" s="2"/>
-    </row>
-    <row r="54" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="1"/>
-      <c r="B54" s="2"/>
-    </row>
-    <row r="55" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="1"/>
-    </row>
-    <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="1"/>
-    </row>
-    <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="1"/>
-      <c r="B57" s="2"/>
-    </row>
-    <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="1"/>
-      <c r="B58" s="2"/>
-    </row>
-    <row r="59" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="3"/>
-      <c r="B59" s="8"/>
-    </row>
-    <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="1"/>
       <c r="B60" s="2"/>
     </row>
-    <row r="61" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="3"/>
+    <row r="61" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="9"/>
       <c r="B61" s="2"/>
     </row>
-    <row r="62" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="1"/>
-    </row>
-    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="9" t="s">
-        <v>38</v>
-      </c>
+    <row r="62" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="3"/>
+      <c r="B63" s="2"/>
+    </row>
+    <row r="64" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>33</v>
+      </c>
+      <c r="B64" s="2"/>
+      <c r="G64" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="1"/>
       <c r="B65" s="2"/>
     </row>
-    <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="9"/>
-      <c r="B66" s="2"/>
-    </row>
-    <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="9"/>
+    <row r="66" spans="1:2" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="B67" s="2"/>
     </row>
-    <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A68" s="9"/>
+    <row r="68" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="B68" s="2"/>
     </row>
-    <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="9"/>
+    <row r="69" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="1"/>
       <c r="B69" s="2"/>
     </row>
-    <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="3" t="s">
-        <v>79</v>
-      </c>
+    <row r="70" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="1"/>
       <c r="B70" s="2"/>
     </row>
-    <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A71" s="9"/>
+    <row r="71" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A71" s="1"/>
       <c r="B71" s="2"/>
     </row>
-    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="3" t="s">
-        <v>60</v>
-      </c>
+    <row r="72" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="1"/>
       <c r="B72" s="2"/>
     </row>
-    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="3"/>
+    <row r="73" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="1"/>
       <c r="B73" s="2"/>
     </row>
-    <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>33</v>
-      </c>
+    <row r="74" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="1"/>
       <c r="B74" s="2"/>
-      <c r="G74" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
     </row>
-    <row r="76" spans="1:7" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="3" t="s">
-        <v>18</v>
-      </c>
+    <row r="76" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="1"/>
+      <c r="B76" s="2"/>
+    </row>
+    <row r="77" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="1"/>
       <c r="B77" s="2"/>
     </row>
-    <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="7" t="s">
-        <v>16</v>
-      </c>
+    <row r="78" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="1"/>
       <c r="B78" s="2"/>
     </row>
-    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79" s="2"/>
     </row>
-    <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="2"/>
     </row>
@@ -1226,201 +1218,202 @@
       <c r="A83" s="1"/>
       <c r="B83" s="2"/>
     </row>
-    <row r="84" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A84" s="1"/>
-      <c r="B84" s="2"/>
-    </row>
-    <row r="85" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A85" s="1"/>
-      <c r="B85" s="2"/>
-    </row>
-    <row r="86" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="1"/>
-      <c r="B86" s="2"/>
+    <row r="85" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A85" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A86" s="12"/>
     </row>
     <row r="87" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A87" s="1"/>
+      <c r="A87" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="B87" s="2"/>
     </row>
-    <row r="88" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A88" s="1"/>
-      <c r="B88" s="2"/>
-    </row>
-    <row r="89" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A89" s="1"/>
-      <c r="B89" s="2"/>
-    </row>
-    <row r="90" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A90" s="1"/>
-      <c r="B90" s="2"/>
+    <row r="88" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A88" s="12"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A90" s="12"/>
     </row>
     <row r="91" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A91" s="1"/>
-      <c r="B91" s="2"/>
+      <c r="A91" s="3" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="92" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A92" s="1"/>
-      <c r="B92" s="2"/>
+      <c r="A92" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="93" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A93" s="1"/>
-      <c r="B93" s="2"/>
-    </row>
-    <row r="95" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A95" s="12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A96" s="12"/>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A98" s="12"/>
+      <c r="A93" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A95" s="12"/>
+    </row>
+    <row r="96" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A96" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B96" s="2"/>
+    </row>
+    <row r="97" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A97" s="3"/>
+      <c r="B97" s="2"/>
+    </row>
+    <row r="98" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A98" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B98" s="2"/>
     </row>
     <row r="99" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A99" s="3" t="s">
-        <v>82</v>
-      </c>
+      <c r="A99" t="s">
+        <v>55</v>
+      </c>
+      <c r="B99" s="2"/>
     </row>
     <row r="100" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
-        <v>83</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B100" s="2"/>
     </row>
     <row r="101" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A103" s="12"/>
-    </row>
-    <row r="104" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A104" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B104" s="2"/>
+        <v>56</v>
+      </c>
+      <c r="B101" s="2"/>
+    </row>
+    <row r="102" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A102" s="3"/>
+      <c r="B102" s="2"/>
+    </row>
+    <row r="103" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A103" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A104" s="12"/>
     </row>
     <row r="105" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A105" s="3"/>
-      <c r="B105" s="2"/>
-    </row>
-    <row r="106" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A106" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B106" s="2"/>
-    </row>
-    <row r="107" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A105" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A106" s="12"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>55</v>
-      </c>
-      <c r="B107" s="2"/>
-    </row>
-    <row r="108" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A108" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B108" s="2"/>
-    </row>
-    <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A109" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B109" s="2"/>
-    </row>
-    <row r="110" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A110" s="3"/>
-      <c r="B110" s="2"/>
-    </row>
-    <row r="111" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A111" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A108" s="12"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A110" s="12"/>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A112" s="12"/>
     </row>
     <row r="113" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A114" s="12"/>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A116" s="12"/>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="B114" s="2"/>
+    </row>
+    <row r="115" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A115" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B115" s="2"/>
+    </row>
+    <row r="116" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A116" s="3"/>
+      <c r="B116" s="2"/>
+    </row>
+    <row r="117" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A117" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A118" s="12"/>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" ht="22.2" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="119" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A120" s="12"/>
     </row>
-    <row r="121" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.7">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A122" s="12"/>
-      <c r="B122" s="2"/>
     </row>
     <row r="123" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B123" s="2"/>
+        <v>62</v>
+      </c>
     </row>
     <row r="124" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" s="3"/>
-      <c r="B124" s="2"/>
     </row>
     <row r="125" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" ht="12.6" customHeight="1" x14ac:dyDescent="0.7">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A126" s="12"/>
     </row>
     <row r="127" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.7">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A128" s="12"/>
     </row>
-    <row r="129" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
@@ -1428,71 +1421,73 @@
     </row>
     <row r="131" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A132" s="3"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="133" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A133" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A134" s="12"/>
-    </row>
-    <row r="135" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A136" s="12"/>
-    </row>
-    <row r="137" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A138" s="12"/>
-    </row>
-    <row r="139" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A139" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="3"/>
+      <c r="B133" s="2"/>
+    </row>
+    <row r="134" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A134" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B134" s="2"/>
+    </row>
+    <row r="135" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A135" s="12"/>
+      <c r="B135" s="2"/>
+    </row>
+    <row r="136" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A136" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A137" s="3"/>
+    </row>
+    <row r="138" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A138" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A139" s="4"/>
+    </row>
+    <row r="140" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A141" s="3"/>
       <c r="B141" s="2"/>
     </row>
     <row r="142" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B142" s="2"/>
     </row>
-    <row r="143" spans="1:2" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A143" s="12"/>
+    <row r="143" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A143" s="4"/>
       <c r="B143" s="2"/>
     </row>
     <row r="144" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A145" s="3"/>
     </row>
-    <row r="146" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A146" s="3" t="s">
-        <v>48</v>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="21" x14ac:dyDescent="0.4">
@@ -1500,298 +1495,264 @@
     </row>
     <row r="148" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B149" s="2"/>
+      <c r="A149" s="3"/>
     </row>
     <row r="150" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B150" s="2"/>
+        <v>46</v>
+      </c>
     </row>
     <row r="151" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A151" s="4"/>
-      <c r="B151" s="2"/>
     </row>
     <row r="152" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A152" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A153" s="3"/>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A154" t="s">
-        <v>32</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A153" s="4"/>
+    </row>
+    <row r="154" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A154" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A155" s="4"/>
+      <c r="B155" s="2"/>
     </row>
     <row r="156" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A156" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A157" s="3"/>
+      <c r="B157" s="2"/>
     </row>
     <row r="158" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A159" s="4"/>
+      <c r="B159" s="2"/>
     </row>
     <row r="160" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A160" s="3" t="s">
-        <v>37</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B160" s="2"/>
     </row>
     <row r="161" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A161" s="4"/>
+      <c r="B161" s="2"/>
     </row>
     <row r="162" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A162" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A163" s="4"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A163" s="3"/>
       <c r="B163" s="2"/>
     </row>
-    <row r="164" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A164" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A165" s="3"/>
-      <c r="B165" s="2"/>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="166" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A166" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A167" s="4"/>
-      <c r="B167" s="2"/>
-    </row>
-    <row r="168" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A168" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B168" s="2"/>
-    </row>
-    <row r="169" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A169" s="4"/>
-      <c r="B169" s="2"/>
-    </row>
-    <row r="170" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A170" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A171" s="3"/>
-      <c r="B171" s="2"/>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A172" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A174" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A176" t="s">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
         <v>24</v>
       </c>
     </row>
+    <row r="189" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B189" s="2"/>
+    </row>
+    <row r="191" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B191" s="2"/>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B193" s="2"/>
+    </row>
+    <row r="194" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>1</v>
+      </c>
+      <c r="B194" s="2"/>
+    </row>
+    <row r="195" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B195" s="2"/>
+    </row>
+    <row r="196" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A196" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B196" s="2"/>
+    </row>
     <row r="197" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A197" s="3"/>
       <c r="B197" s="2"/>
     </row>
+    <row r="198" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A198" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="199" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A199" s="3"/>
       <c r="B199" s="2"/>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A200" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B201" s="2"/>
+    <row r="200" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A200" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B200" s="2"/>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B201" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="202" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A202" t="s">
-        <v>1</v>
-      </c>
-      <c r="B202" s="2"/>
+      <c r="A202" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="203" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B203" s="2"/>
-    </row>
-    <row r="204" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A204" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B204" s="2"/>
-    </row>
-    <row r="205" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A205" s="3"/>
-      <c r="B205" s="2"/>
-    </row>
-    <row r="206" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A206" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A207" s="3"/>
-      <c r="B207" s="2"/>
-    </row>
-    <row r="208" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A208" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B208" s="2"/>
+      <c r="A203" s="1"/>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A206" s="5"/>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A207" s="5"/>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A208" s="5"/>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B209" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A210" s="3" t="s">
-        <v>5</v>
+      <c r="A209" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A210" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A211" s="1"/>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A214" s="5"/>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A215" s="5"/>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A216" s="5"/>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A217" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A218" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="A211" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B211" s="2"/>
+    </row>
+    <row r="212" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A212" s="5"/>
+      <c r="B212" s="2"/>
+    </row>
+    <row r="213" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A213" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B213" s="2"/>
+    </row>
+    <row r="214" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A214" s="1"/>
+      <c r="B214" s="2"/>
+    </row>
+    <row r="215" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A215" s="1"/>
+      <c r="B215" s="2"/>
+    </row>
+    <row r="216" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A216" s="1"/>
+      <c r="B216" s="2"/>
+    </row>
+    <row r="217" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A217" s="1"/>
+    </row>
+    <row r="218" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A218" s="1"/>
+      <c r="B218" s="2"/>
     </row>
     <row r="219" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A219" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B219" s="2"/>
+      <c r="A219" s="1"/>
     </row>
     <row r="220" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A220" s="5"/>
       <c r="B220" s="2"/>
     </row>
     <row r="221" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A221" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B221" s="2"/>
+      <c r="A221" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="222" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A222" s="1"/>
       <c r="B222" s="2"/>
     </row>
     <row r="223" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A223" s="1"/>
-      <c r="B223" s="2"/>
+      <c r="A223" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="224" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A224" s="1"/>
       <c r="B224" s="2"/>
     </row>
     <row r="225" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A225" s="1"/>
-    </row>
-    <row r="226" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A226" s="1"/>
-      <c r="B226" s="2"/>
+      <c r="A225" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="227" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A227" s="1"/>
+      <c r="A227" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="228" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B228" s="2"/>
     </row>
     <row r="229" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A229" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="A229" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B229" s="2"/>
     </row>
     <row r="230" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B230" s="2"/>
     </row>
     <row r="231" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A231" s="3" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A232" s="1"/>
       <c r="B232" s="2"/>
     </row>
     <row r="233" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A233" s="3" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A235" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B236" s="2"/>
-    </row>
-    <row r="237" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A237" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B237" s="2"/>
-    </row>
-    <row r="238" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B238" s="2"/>
-    </row>
-    <row r="239" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A239" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="240" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A240" s="1"/>
-      <c r="B240" s="2"/>
-    </row>
-    <row r="241" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A241" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="243" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A243" s="3" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>